<commit_message>
updated rules according to ticket #426
</commit_message>
<xml_diff>
--- a/Deliverables/RULES/USDM_CORE_Rules_Changes.xlsx
+++ b/Deliverables/RULES/USDM_CORE_Rules_Changes.xlsx
@@ -1,23 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Stack\CL027\Publish\CORE\3.4\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Stack\CL027\Publish\CORE\3.5\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD0024EF-FAA0-4867-BCC5-59141E154FF6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1F7C510-A7C2-46C6-846B-B820F9970ACA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7215" yWindow="-16755" windowWidth="24555" windowHeight="15225" xr2:uid="{418CF395-400B-43AB-9594-6DFC1F089218}"/>
+    <workbookView xWindow="-12165" yWindow="-18450" windowWidth="27495" windowHeight="15225" xr2:uid="{418CF395-400B-43AB-9594-6DFC1F089218}"/>
   </bookViews>
   <sheets>
-    <sheet name="Changes release 3.3-&gt;3.4" sheetId="5" r:id="rId1"/>
-    <sheet name="Changes release 3.1-&gt;3.3" sheetId="6" r:id="rId2"/>
+    <sheet name="Changes release 3.4-&gt;3.5" sheetId="7" r:id="rId1"/>
+    <sheet name="Changes release 3.3-&gt;3.4" sheetId="5" r:id="rId2"/>
+    <sheet name="Changes release 3.1-&gt;3.3" sheetId="6" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Changes release 3.3-&gt;3.4'!$A$1:$O$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Changes release 3.3-&gt;3.4'!$A$1:$O$1</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -40,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="601">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2393" uniqueCount="616">
   <si>
     <t>All</t>
   </si>
@@ -1794,9 +1795,6 @@
     <t>CHK0181</t>
   </si>
   <si>
-    <t>For a specified range at least a minimum or maximum value is expected.</t>
-  </si>
-  <si>
     <t>A study cell must only reference elements that are defined within the same study design as the study cell.</t>
   </si>
   <si>
@@ -1843,6 +1841,54 @@
   </si>
   <si>
     <t>CHK0187</t>
+  </si>
+  <si>
+    <t>Change?</t>
+  </si>
+  <si>
+    <t>All abbreviations defined for a study version must be unique.</t>
+  </si>
+  <si>
+    <t>Abbreviation</t>
+  </si>
+  <si>
+    <t>abbreviation</t>
+  </si>
+  <si>
+    <t>CHK0191</t>
+  </si>
+  <si>
+    <t>The long names for all abbreviations defined for a study version are expected to be unique.</t>
+  </si>
+  <si>
+    <t>longName</t>
+  </si>
+  <si>
+    <t>CHK0192</t>
+  </si>
+  <si>
+    <t>If the duration of an administration will vary, a quantity is not expected for the administration duration and vice versa.</t>
+  </si>
+  <si>
+    <t>Within a code system and corresponding version, a one-to-one relationship between code and decode is expected.</t>
+  </si>
+  <si>
+    <t>A study arm must only reference populations that are defined within the same study design as the study arm.</t>
+  </si>
+  <si>
+    <t>DDF00049</t>
+  </si>
+  <si>
+    <t>A study arm must only reference cohorts that are defined within the population that is defined within the same study design as the study arm.</t>
+  </si>
+  <si>
+    <t>DDF00050</t>
+  </si>
+  <si>
+    <t>CHK0190</t>
+  </si>
+  <si>
+    <t>Textual statement of rule (old, if changed)</t>
   </si>
 </sst>
 </file>
@@ -2279,11 +2325,362 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E53E83C4-68F7-4929-AA83-3F95502173FC}">
-  <dimension ref="A1:O17"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B456D714-2DB6-4B8B-BC8E-8AA7501F8C79}">
+  <dimension ref="A1:O7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection activeCell="J7" sqref="J7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="2" max="2" width="35.453125" customWidth="1"/>
+    <col min="4" max="4" width="18.81640625" customWidth="1"/>
+    <col min="5" max="5" width="25" customWidth="1"/>
+    <col min="10" max="10" width="47.7265625" customWidth="1"/>
+    <col min="11" max="11" width="19.6328125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:15" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>600</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>546</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>547</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>548</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>549</v>
+      </c>
+      <c r="F1" s="8" t="s">
+        <v>550</v>
+      </c>
+      <c r="G1" s="8" t="s">
+        <v>551</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>552</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>306</v>
+      </c>
+      <c r="J1" s="8" t="s">
+        <v>615</v>
+      </c>
+      <c r="K1" t="s">
+        <v>395</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>545</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>396</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>397</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" ht="29" x14ac:dyDescent="0.35">
+      <c r="A2" s="7" t="s">
+        <v>415</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>601</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>602</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>603</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="I2" t="s">
+        <v>604</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="K2" t="s">
+        <v>122</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="M2" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="N2" t="s">
+        <v>122</v>
+      </c>
+      <c r="O2" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A3" s="7" t="s">
+        <v>415</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>605</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>602</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>606</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="I3" t="s">
+        <v>607</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="K3" t="s">
+        <v>122</v>
+      </c>
+      <c r="L3" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="M3" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="N3" t="s">
+        <v>122</v>
+      </c>
+      <c r="O3" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A4" s="7" t="s">
+        <v>416</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>608</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>244</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>435</v>
+      </c>
+      <c r="I4" t="s">
+        <v>242</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>243</v>
+      </c>
+      <c r="K4" t="s">
+        <v>438</v>
+      </c>
+      <c r="L4" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="M4" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="N4" t="s">
+        <v>122</v>
+      </c>
+      <c r="O4" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A5" s="7" t="s">
+        <v>416</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>609</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>227</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>451</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="H5" s="3" t="s">
+        <v>452</v>
+      </c>
+      <c r="I5" t="s">
+        <v>453</v>
+      </c>
+      <c r="J5" s="1" t="s">
+        <v>450</v>
+      </c>
+      <c r="K5" t="s">
+        <v>122</v>
+      </c>
+      <c r="L5" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="M5" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="N5" t="s">
+        <v>122</v>
+      </c>
+      <c r="O5" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A6" s="7" t="s">
+        <v>416</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>610</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="H6" s="3" t="s">
+        <v>611</v>
+      </c>
+      <c r="I6" t="s">
+        <v>135</v>
+      </c>
+      <c r="J6" s="1" t="s">
+        <v>501</v>
+      </c>
+      <c r="K6" t="s">
+        <v>122</v>
+      </c>
+      <c r="L6" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="M6" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="N6" t="s">
+        <v>122</v>
+      </c>
+      <c r="O6" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" ht="58" x14ac:dyDescent="0.35">
+      <c r="A7" s="7" t="s">
+        <v>415</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>612</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="G7" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="H7" s="3" t="s">
+        <v>613</v>
+      </c>
+      <c r="I7" t="s">
+        <v>614</v>
+      </c>
+      <c r="J7" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="K7" t="s">
+        <v>122</v>
+      </c>
+      <c r="L7" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="M7" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="N7" t="s">
+        <v>122</v>
+      </c>
+      <c r="O7" t="s">
+        <v>122</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E53E83C4-68F7-4929-AA83-3F95502173FC}">
+  <dimension ref="A1:O195"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2323,7 +2720,7 @@
       <c r="G1" s="8" t="s">
         <v>551</v>
       </c>
-      <c r="H1" s="9" t="s">
+      <c r="H1" s="2" t="s">
         <v>552</v>
       </c>
       <c r="I1" s="2" t="s">
@@ -2373,25 +2770,25 @@
       <c r="H2" s="3" t="s">
         <v>446</v>
       </c>
-      <c r="I2" t="s">
+      <c r="I2" s="4" t="s">
         <v>105</v>
       </c>
-      <c r="J2" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="K2" t="s">
-        <v>122</v>
-      </c>
-      <c r="L2" s="1" t="s">
+      <c r="J2" s="6" t="s">
+        <v>122</v>
+      </c>
+      <c r="K2" s="4" t="s">
+        <v>122</v>
+      </c>
+      <c r="L2" s="6" t="s">
         <v>568</v>
       </c>
-      <c r="M2" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="N2" t="s">
-        <v>122</v>
-      </c>
-      <c r="O2" t="s">
+      <c r="M2" s="6" t="s">
+        <v>122</v>
+      </c>
+      <c r="N2" s="4" t="s">
+        <v>122</v>
+      </c>
+      <c r="O2" s="4" t="s">
         <v>122</v>
       </c>
     </row>
@@ -2420,25 +2817,25 @@
       <c r="H3" s="3" t="s">
         <v>122</v>
       </c>
-      <c r="I3" t="s">
+      <c r="I3" s="4" t="s">
         <v>571</v>
       </c>
-      <c r="J3" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="K3" t="s">
-        <v>122</v>
-      </c>
-      <c r="L3" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="M3" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="N3" t="s">
-        <v>122</v>
-      </c>
-      <c r="O3" t="s">
+      <c r="J3" s="6" t="s">
+        <v>122</v>
+      </c>
+      <c r="K3" s="4" t="s">
+        <v>122</v>
+      </c>
+      <c r="L3" s="6" t="s">
+        <v>122</v>
+      </c>
+      <c r="M3" s="6" t="s">
+        <v>122</v>
+      </c>
+      <c r="N3" s="4" t="s">
+        <v>122</v>
+      </c>
+      <c r="O3" s="4" t="s">
         <v>122</v>
       </c>
     </row>
@@ -2467,25 +2864,25 @@
       <c r="H4" s="3" t="s">
         <v>122</v>
       </c>
-      <c r="I4" t="s">
+      <c r="I4" s="4" t="s">
         <v>574</v>
       </c>
-      <c r="J4" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="K4" t="s">
-        <v>122</v>
-      </c>
-      <c r="L4" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="M4" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="N4" t="s">
-        <v>122</v>
-      </c>
-      <c r="O4" t="s">
+      <c r="J4" s="6" t="s">
+        <v>122</v>
+      </c>
+      <c r="K4" s="4" t="s">
+        <v>122</v>
+      </c>
+      <c r="L4" s="6" t="s">
+        <v>122</v>
+      </c>
+      <c r="M4" s="6" t="s">
+        <v>122</v>
+      </c>
+      <c r="N4" s="4" t="s">
+        <v>122</v>
+      </c>
+      <c r="O4" s="4" t="s">
         <v>122</v>
       </c>
     </row>
@@ -2514,25 +2911,25 @@
       <c r="H5" s="3" t="s">
         <v>122</v>
       </c>
-      <c r="I5" t="s">
+      <c r="I5" s="4" t="s">
         <v>146</v>
       </c>
-      <c r="J5" s="1" t="s">
+      <c r="J5" s="6" t="s">
         <v>147</v>
       </c>
-      <c r="K5" t="s">
-        <v>122</v>
-      </c>
-      <c r="L5" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="M5" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="N5" t="s">
-        <v>122</v>
-      </c>
-      <c r="O5" t="s">
+      <c r="K5" s="4" t="s">
+        <v>122</v>
+      </c>
+      <c r="L5" s="6" t="s">
+        <v>122</v>
+      </c>
+      <c r="M5" s="6" t="s">
+        <v>122</v>
+      </c>
+      <c r="N5" s="4" t="s">
+        <v>122</v>
+      </c>
+      <c r="O5" s="4" t="s">
         <v>122</v>
       </c>
     </row>
@@ -2561,25 +2958,25 @@
       <c r="H6" s="3" t="s">
         <v>122</v>
       </c>
-      <c r="I6" t="s">
+      <c r="I6" s="4" t="s">
         <v>578</v>
       </c>
-      <c r="J6" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="K6" t="s">
-        <v>122</v>
-      </c>
-      <c r="L6" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="M6" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="N6" t="s">
-        <v>122</v>
-      </c>
-      <c r="O6" t="s">
+      <c r="J6" s="6" t="s">
+        <v>122</v>
+      </c>
+      <c r="K6" s="4" t="s">
+        <v>122</v>
+      </c>
+      <c r="L6" s="6" t="s">
+        <v>122</v>
+      </c>
+      <c r="M6" s="6" t="s">
+        <v>122</v>
+      </c>
+      <c r="N6" s="4" t="s">
+        <v>122</v>
+      </c>
+      <c r="O6" s="4" t="s">
         <v>122</v>
       </c>
     </row>
@@ -2608,25 +3005,25 @@
       <c r="H7" s="3" t="s">
         <v>122</v>
       </c>
-      <c r="I7" t="s">
+      <c r="I7" s="4" t="s">
         <v>581</v>
       </c>
-      <c r="J7" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="K7" t="s">
-        <v>122</v>
-      </c>
-      <c r="L7" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="M7" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="N7" t="s">
-        <v>122</v>
-      </c>
-      <c r="O7" t="s">
+      <c r="J7" s="6" t="s">
+        <v>122</v>
+      </c>
+      <c r="K7" s="4" t="s">
+        <v>122</v>
+      </c>
+      <c r="L7" s="6" t="s">
+        <v>122</v>
+      </c>
+      <c r="M7" s="6" t="s">
+        <v>122</v>
+      </c>
+      <c r="N7" s="4" t="s">
+        <v>122</v>
+      </c>
+      <c r="O7" s="4" t="s">
         <v>122</v>
       </c>
     </row>
@@ -2655,25 +3052,25 @@
       <c r="H8" s="3" t="s">
         <v>122</v>
       </c>
-      <c r="I8" t="s">
+      <c r="I8" s="4" t="s">
         <v>102</v>
       </c>
-      <c r="J8" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="K8" t="s">
-        <v>122</v>
-      </c>
-      <c r="L8" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="M8" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="N8" t="s">
-        <v>122</v>
-      </c>
-      <c r="O8" t="s">
+      <c r="J8" s="6" t="s">
+        <v>122</v>
+      </c>
+      <c r="K8" s="4" t="s">
+        <v>122</v>
+      </c>
+      <c r="L8" s="6" t="s">
+        <v>122</v>
+      </c>
+      <c r="M8" s="6" t="s">
+        <v>122</v>
+      </c>
+      <c r="N8" s="4" t="s">
+        <v>122</v>
+      </c>
+      <c r="O8" s="4" t="s">
         <v>407</v>
       </c>
     </row>
@@ -2702,29 +3099,29 @@
       <c r="H9" s="3" t="s">
         <v>122</v>
       </c>
-      <c r="I9" t="s">
+      <c r="I9" s="4" t="s">
         <v>583</v>
       </c>
-      <c r="J9" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="K9" t="s">
-        <v>122</v>
-      </c>
-      <c r="L9" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="M9" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="N9" t="s">
-        <v>122</v>
-      </c>
-      <c r="O9" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="J9" s="6" t="s">
+        <v>122</v>
+      </c>
+      <c r="K9" s="4" t="s">
+        <v>122</v>
+      </c>
+      <c r="L9" s="6" t="s">
+        <v>122</v>
+      </c>
+      <c r="M9" s="6" t="s">
+        <v>122</v>
+      </c>
+      <c r="N9" s="4" t="s">
+        <v>122</v>
+      </c>
+      <c r="O9" s="4" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" ht="29" x14ac:dyDescent="0.35">
       <c r="A10" s="7" t="s">
         <v>416</v>
       </c>
@@ -2732,48 +3129,48 @@
         <v>584</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>95</v>
+        <v>1</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>469</v>
+        <v>83</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>474</v>
+        <v>84</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="G10" s="3" t="s">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="H10" s="3" t="s">
         <v>122</v>
       </c>
-      <c r="I10" t="s">
-        <v>475</v>
-      </c>
-      <c r="J10" s="1" t="s">
-        <v>473</v>
-      </c>
-      <c r="K10" t="s">
-        <v>122</v>
-      </c>
-      <c r="L10" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="M10" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="N10" t="s">
-        <v>122</v>
-      </c>
-      <c r="O10" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="11" spans="1:15" ht="29" x14ac:dyDescent="0.35">
+      <c r="I10" s="4" t="s">
+        <v>240</v>
+      </c>
+      <c r="J10" s="6" t="s">
+        <v>241</v>
+      </c>
+      <c r="K10" s="4" t="s">
+        <v>122</v>
+      </c>
+      <c r="L10" s="6" t="s">
+        <v>122</v>
+      </c>
+      <c r="M10" s="6" t="s">
+        <v>122</v>
+      </c>
+      <c r="N10" s="4" t="s">
+        <v>122</v>
+      </c>
+      <c r="O10" s="4" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A11" s="7" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="B11" s="3" t="s">
         <v>585</v>
@@ -2788,33 +3185,33 @@
         <v>84</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="G11" s="3" t="s">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="H11" s="3" t="s">
         <v>122</v>
       </c>
-      <c r="I11" t="s">
-        <v>240</v>
-      </c>
-      <c r="J11" s="1" t="s">
-        <v>241</v>
-      </c>
-      <c r="K11" t="s">
-        <v>122</v>
-      </c>
-      <c r="L11" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="M11" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="N11" t="s">
-        <v>122</v>
-      </c>
-      <c r="O11" t="s">
+      <c r="I11" s="4" t="s">
+        <v>586</v>
+      </c>
+      <c r="J11" s="6" t="s">
+        <v>122</v>
+      </c>
+      <c r="K11" s="4" t="s">
+        <v>122</v>
+      </c>
+      <c r="L11" s="6" t="s">
+        <v>122</v>
+      </c>
+      <c r="M11" s="6" t="s">
+        <v>122</v>
+      </c>
+      <c r="N11" s="4" t="s">
+        <v>122</v>
+      </c>
+      <c r="O11" s="4" t="s">
         <v>122</v>
       </c>
     </row>
@@ -2823,45 +3220,45 @@
         <v>415</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>586</v>
+        <v>587</v>
       </c>
       <c r="C12" s="3" t="s">
         <v>1</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>83</v>
+        <v>588</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>84</v>
+        <v>589</v>
       </c>
       <c r="F12" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G12" s="3" t="s">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="H12" s="3" t="s">
         <v>122</v>
       </c>
-      <c r="I12" t="s">
-        <v>587</v>
-      </c>
-      <c r="J12" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="K12" t="s">
-        <v>122</v>
-      </c>
-      <c r="L12" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="M12" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="N12" t="s">
-        <v>122</v>
-      </c>
-      <c r="O12" t="s">
+      <c r="I12" s="4" t="s">
+        <v>590</v>
+      </c>
+      <c r="J12" s="6" t="s">
+        <v>122</v>
+      </c>
+      <c r="K12" s="4" t="s">
+        <v>122</v>
+      </c>
+      <c r="L12" s="6" t="s">
+        <v>122</v>
+      </c>
+      <c r="M12" s="6" t="s">
+        <v>122</v>
+      </c>
+      <c r="N12" s="4" t="s">
+        <v>122</v>
+      </c>
+      <c r="O12" s="4" t="s">
         <v>122</v>
       </c>
     </row>
@@ -2870,16 +3267,16 @@
         <v>415</v>
       </c>
       <c r="B13" s="3" t="s">
+        <v>591</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D13" s="3" t="s">
         <v>588</v>
       </c>
-      <c r="C13" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="D13" s="3" t="s">
-        <v>589</v>
-      </c>
       <c r="E13" s="3" t="s">
-        <v>590</v>
+        <v>66</v>
       </c>
       <c r="F13" s="3" t="s">
         <v>8</v>
@@ -2890,43 +3287,43 @@
       <c r="H13" s="3" t="s">
         <v>122</v>
       </c>
-      <c r="I13" t="s">
-        <v>591</v>
-      </c>
-      <c r="J13" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="K13" t="s">
-        <v>122</v>
-      </c>
-      <c r="L13" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="M13" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="N13" t="s">
-        <v>122</v>
-      </c>
-      <c r="O13" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="I13" s="4" t="s">
+        <v>592</v>
+      </c>
+      <c r="J13" s="6" t="s">
+        <v>122</v>
+      </c>
+      <c r="K13" s="4" t="s">
+        <v>122</v>
+      </c>
+      <c r="L13" s="6" t="s">
+        <v>122</v>
+      </c>
+      <c r="M13" s="6" t="s">
+        <v>122</v>
+      </c>
+      <c r="N13" s="4" t="s">
+        <v>122</v>
+      </c>
+      <c r="O13" s="4" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" ht="29" x14ac:dyDescent="0.35">
       <c r="A14" s="7" t="s">
         <v>415</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>592</v>
+        <v>593</v>
       </c>
       <c r="C14" s="3" t="s">
         <v>1</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>589</v>
+        <v>594</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>66</v>
+        <v>595</v>
       </c>
       <c r="F14" s="3" t="s">
         <v>8</v>
@@ -2937,168 +3334,1195 @@
       <c r="H14" s="3" t="s">
         <v>122</v>
       </c>
-      <c r="I14" t="s">
-        <v>593</v>
-      </c>
-      <c r="J14" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="K14" t="s">
-        <v>122</v>
-      </c>
-      <c r="L14" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="M14" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="N14" t="s">
-        <v>122</v>
-      </c>
-      <c r="O14" t="s">
+      <c r="I14" s="4" t="s">
+        <v>596</v>
+      </c>
+      <c r="J14" s="6" t="s">
+        <v>122</v>
+      </c>
+      <c r="K14" s="4" t="s">
+        <v>122</v>
+      </c>
+      <c r="L14" s="6" t="s">
+        <v>122</v>
+      </c>
+      <c r="M14" s="6" t="s">
+        <v>122</v>
+      </c>
+      <c r="N14" s="4" t="s">
+        <v>122</v>
+      </c>
+      <c r="O14" s="4" t="s">
         <v>122</v>
       </c>
     </row>
     <row r="15" spans="1:15" ht="29" x14ac:dyDescent="0.35">
       <c r="A15" s="7" t="s">
-        <v>415</v>
+        <v>416</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>594</v>
+        <v>186</v>
       </c>
       <c r="C15" s="3" t="s">
         <v>1</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>595</v>
+        <v>187</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>596</v>
+        <v>188</v>
       </c>
       <c r="F15" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="G15" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="G15" s="3" t="s">
-        <v>2</v>
-      </c>
       <c r="H15" s="3" t="s">
         <v>122</v>
       </c>
-      <c r="I15" t="s">
-        <v>597</v>
-      </c>
-      <c r="J15" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="K15" t="s">
-        <v>122</v>
-      </c>
-      <c r="L15" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="M15" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="N15" t="s">
-        <v>122</v>
-      </c>
-      <c r="O15" t="s">
-        <v>122</v>
+      <c r="I15" s="4" t="s">
+        <v>185</v>
+      </c>
+      <c r="J15" s="6" t="s">
+        <v>122</v>
+      </c>
+      <c r="K15" s="4" t="s">
+        <v>122</v>
+      </c>
+      <c r="L15" s="6" t="s">
+        <v>122</v>
+      </c>
+      <c r="M15" s="6" t="s">
+        <v>122</v>
+      </c>
+      <c r="N15" s="4" t="s">
+        <v>122</v>
+      </c>
+      <c r="O15" s="4" t="s">
+        <v>407</v>
       </c>
     </row>
     <row r="16" spans="1:15" ht="29" x14ac:dyDescent="0.35">
       <c r="A16" s="7" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>186</v>
+        <v>597</v>
       </c>
       <c r="C16" s="3" t="s">
         <v>1</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>187</v>
+        <v>22</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>188</v>
+        <v>598</v>
       </c>
       <c r="F16" s="3" t="s">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="G16" s="3" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="H16" s="3" t="s">
         <v>122</v>
       </c>
-      <c r="I16" t="s">
-        <v>185</v>
-      </c>
-      <c r="J16" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="K16" t="s">
-        <v>122</v>
-      </c>
-      <c r="L16" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="M16" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="N16" t="s">
-        <v>122</v>
-      </c>
-      <c r="O16" t="s">
-        <v>407</v>
-      </c>
-    </row>
-    <row r="17" spans="1:15" ht="29" x14ac:dyDescent="0.35">
-      <c r="A17" s="7" t="s">
-        <v>415</v>
-      </c>
-      <c r="B17" s="3" t="s">
-        <v>598</v>
-      </c>
-      <c r="C17" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="D17" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="E17" s="3" t="s">
+      <c r="I16" s="4" t="s">
         <v>599</v>
       </c>
-      <c r="F17" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="G17" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="H17" s="3" t="s">
-        <v>122</v>
-      </c>
-      <c r="I17" t="s">
-        <v>600</v>
-      </c>
-      <c r="J17" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="K17" t="s">
-        <v>122</v>
-      </c>
-      <c r="L17" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="M17" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="N17" t="s">
-        <v>122</v>
-      </c>
-      <c r="O17" t="s">
-        <v>122</v>
-      </c>
+      <c r="J16" s="6" t="s">
+        <v>122</v>
+      </c>
+      <c r="K16" s="4" t="s">
+        <v>122</v>
+      </c>
+      <c r="L16" s="6" t="s">
+        <v>122</v>
+      </c>
+      <c r="M16" s="6" t="s">
+        <v>122</v>
+      </c>
+      <c r="N16" s="4" t="s">
+        <v>122</v>
+      </c>
+      <c r="O16" s="4" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="17" spans="2:13" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="B17" s="1"/>
+      <c r="J17" s="1"/>
+      <c r="L17" s="1"/>
+      <c r="M17" s="1"/>
+    </row>
+    <row r="18" spans="2:13" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="B18" s="1"/>
+      <c r="J18" s="1"/>
+      <c r="L18" s="1"/>
+      <c r="M18" s="1"/>
+    </row>
+    <row r="19" spans="2:13" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="B19" s="1"/>
+      <c r="J19" s="1"/>
+      <c r="L19" s="1"/>
+      <c r="M19" s="1"/>
+    </row>
+    <row r="20" spans="2:13" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="B20" s="1"/>
+      <c r="J20" s="1"/>
+      <c r="L20" s="1"/>
+      <c r="M20" s="1"/>
+    </row>
+    <row r="21" spans="2:13" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="B21" s="1"/>
+      <c r="J21" s="1"/>
+      <c r="L21" s="1"/>
+      <c r="M21" s="1"/>
+    </row>
+    <row r="22" spans="2:13" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="B22" s="1"/>
+      <c r="J22" s="1"/>
+      <c r="L22" s="1"/>
+      <c r="M22" s="1"/>
+    </row>
+    <row r="23" spans="2:13" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="B23" s="1"/>
+      <c r="J23" s="1"/>
+      <c r="L23" s="1"/>
+      <c r="M23" s="1"/>
+    </row>
+    <row r="24" spans="2:13" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="B24" s="1"/>
+      <c r="J24" s="1"/>
+      <c r="L24" s="1"/>
+      <c r="M24" s="1"/>
+    </row>
+    <row r="25" spans="2:13" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="B25" s="1"/>
+      <c r="J25" s="1"/>
+      <c r="L25" s="1"/>
+      <c r="M25" s="1"/>
+    </row>
+    <row r="26" spans="2:13" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="B26" s="1"/>
+      <c r="J26" s="1"/>
+      <c r="L26" s="1"/>
+      <c r="M26" s="1"/>
+    </row>
+    <row r="27" spans="2:13" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="B27" s="1"/>
+      <c r="J27" s="1"/>
+      <c r="L27" s="1"/>
+      <c r="M27" s="1"/>
+    </row>
+    <row r="28" spans="2:13" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="B28" s="1"/>
+      <c r="J28" s="1"/>
+      <c r="L28" s="1"/>
+      <c r="M28" s="1"/>
+    </row>
+    <row r="29" spans="2:13" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="B29" s="1"/>
+      <c r="J29" s="1"/>
+      <c r="L29" s="1"/>
+      <c r="M29" s="1"/>
+    </row>
+    <row r="30" spans="2:13" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="B30" s="1"/>
+      <c r="J30" s="1"/>
+      <c r="L30" s="1"/>
+      <c r="M30" s="1"/>
+    </row>
+    <row r="31" spans="2:13" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="B31" s="1"/>
+      <c r="J31" s="1"/>
+      <c r="L31" s="1"/>
+      <c r="M31" s="1"/>
+    </row>
+    <row r="32" spans="2:13" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="B32" s="1"/>
+      <c r="J32" s="1"/>
+      <c r="L32" s="1"/>
+      <c r="M32" s="1"/>
+    </row>
+    <row r="33" spans="2:13" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="B33" s="1"/>
+      <c r="J33" s="1"/>
+      <c r="L33" s="1"/>
+      <c r="M33" s="1"/>
+    </row>
+    <row r="34" spans="2:13" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="B34" s="1"/>
+      <c r="J34" s="1"/>
+      <c r="L34" s="1"/>
+      <c r="M34" s="1"/>
+    </row>
+    <row r="35" spans="2:13" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="B35" s="1"/>
+      <c r="J35" s="1"/>
+      <c r="L35" s="1"/>
+      <c r="M35" s="1"/>
+    </row>
+    <row r="36" spans="2:13" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="B36" s="1"/>
+      <c r="J36" s="1"/>
+      <c r="L36" s="1"/>
+      <c r="M36" s="1"/>
+    </row>
+    <row r="37" spans="2:13" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="B37" s="1"/>
+      <c r="J37" s="1"/>
+      <c r="L37" s="1"/>
+      <c r="M37" s="1"/>
+    </row>
+    <row r="38" spans="2:13" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="B38" s="1"/>
+      <c r="J38" s="1"/>
+      <c r="L38" s="1"/>
+      <c r="M38" s="1"/>
+    </row>
+    <row r="39" spans="2:13" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="B39" s="1"/>
+      <c r="J39" s="1"/>
+      <c r="L39" s="1"/>
+      <c r="M39" s="1"/>
+    </row>
+    <row r="40" spans="2:13" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="B40" s="1"/>
+      <c r="J40" s="1"/>
+      <c r="L40" s="1"/>
+      <c r="M40" s="1"/>
+    </row>
+    <row r="41" spans="2:13" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="B41" s="1"/>
+      <c r="J41" s="1"/>
+      <c r="L41" s="1"/>
+      <c r="M41" s="1"/>
+    </row>
+    <row r="42" spans="2:13" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="B42" s="1"/>
+      <c r="J42" s="1"/>
+      <c r="L42" s="1"/>
+      <c r="M42" s="1"/>
+    </row>
+    <row r="43" spans="2:13" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="B43" s="1"/>
+      <c r="J43" s="1"/>
+      <c r="L43" s="1"/>
+      <c r="M43" s="1"/>
+    </row>
+    <row r="44" spans="2:13" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="B44" s="1"/>
+      <c r="J44" s="1"/>
+      <c r="L44" s="1"/>
+      <c r="M44" s="1"/>
+    </row>
+    <row r="45" spans="2:13" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="B45" s="1"/>
+      <c r="J45" s="1"/>
+      <c r="L45" s="1"/>
+      <c r="M45" s="1"/>
+    </row>
+    <row r="46" spans="2:13" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="B46" s="1"/>
+      <c r="J46" s="1"/>
+      <c r="L46" s="1"/>
+      <c r="M46" s="1"/>
+    </row>
+    <row r="47" spans="2:13" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="B47" s="1"/>
+      <c r="J47" s="1"/>
+      <c r="L47" s="1"/>
+      <c r="M47" s="1"/>
+    </row>
+    <row r="48" spans="2:13" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="B48" s="1"/>
+      <c r="J48" s="1"/>
+      <c r="L48" s="1"/>
+      <c r="M48" s="1"/>
+    </row>
+    <row r="49" spans="2:13" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="B49" s="1"/>
+      <c r="J49" s="1"/>
+      <c r="L49" s="1"/>
+      <c r="M49" s="1"/>
+    </row>
+    <row r="50" spans="2:13" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="B50" s="1"/>
+      <c r="J50" s="1"/>
+      <c r="L50" s="1"/>
+      <c r="M50" s="1"/>
+    </row>
+    <row r="51" spans="2:13" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="B51" s="1"/>
+      <c r="J51" s="1"/>
+      <c r="L51" s="1"/>
+      <c r="M51" s="1"/>
+    </row>
+    <row r="52" spans="2:13" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="B52" s="1"/>
+      <c r="J52" s="1"/>
+      <c r="L52" s="1"/>
+      <c r="M52" s="1"/>
+    </row>
+    <row r="53" spans="2:13" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="B53" s="1"/>
+      <c r="J53" s="1"/>
+      <c r="L53" s="1"/>
+      <c r="M53" s="1"/>
+    </row>
+    <row r="54" spans="2:13" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="B54" s="1"/>
+      <c r="J54" s="1"/>
+      <c r="L54" s="1"/>
+      <c r="M54" s="1"/>
+    </row>
+    <row r="55" spans="2:13" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="B55" s="1"/>
+      <c r="J55" s="1"/>
+      <c r="L55" s="1"/>
+      <c r="M55" s="1"/>
+    </row>
+    <row r="56" spans="2:13" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="B56" s="1"/>
+      <c r="J56" s="1"/>
+      <c r="L56" s="1"/>
+      <c r="M56" s="1"/>
+    </row>
+    <row r="57" spans="2:13" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="B57" s="1"/>
+      <c r="J57" s="1"/>
+      <c r="L57" s="1"/>
+      <c r="M57" s="1"/>
+    </row>
+    <row r="58" spans="2:13" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="B58" s="1"/>
+      <c r="J58" s="1"/>
+      <c r="L58" s="1"/>
+      <c r="M58" s="1"/>
+    </row>
+    <row r="59" spans="2:13" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="B59" s="1"/>
+      <c r="J59" s="1"/>
+      <c r="L59" s="1"/>
+      <c r="M59" s="1"/>
+    </row>
+    <row r="60" spans="2:13" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="B60" s="1"/>
+      <c r="J60" s="1"/>
+      <c r="L60" s="1"/>
+      <c r="M60" s="1"/>
+    </row>
+    <row r="61" spans="2:13" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="B61" s="1"/>
+      <c r="J61" s="1"/>
+      <c r="L61" s="1"/>
+      <c r="M61" s="1"/>
+    </row>
+    <row r="62" spans="2:13" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="B62" s="1"/>
+      <c r="J62" s="1"/>
+      <c r="L62" s="1"/>
+      <c r="M62" s="1"/>
+    </row>
+    <row r="63" spans="2:13" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="B63" s="1"/>
+      <c r="J63" s="1"/>
+      <c r="L63" s="1"/>
+      <c r="M63" s="1"/>
+    </row>
+    <row r="64" spans="2:13" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="B64" s="1"/>
+      <c r="J64" s="1"/>
+      <c r="L64" s="1"/>
+      <c r="M64" s="1"/>
+    </row>
+    <row r="65" spans="2:13" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="B65" s="1"/>
+      <c r="J65" s="1"/>
+      <c r="L65" s="1"/>
+      <c r="M65" s="1"/>
+    </row>
+    <row r="66" spans="2:13" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="B66" s="1"/>
+      <c r="J66" s="1"/>
+      <c r="L66" s="1"/>
+      <c r="M66" s="1"/>
+    </row>
+    <row r="67" spans="2:13" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="B67" s="1"/>
+      <c r="J67" s="1"/>
+      <c r="L67" s="1"/>
+      <c r="M67" s="1"/>
+    </row>
+    <row r="68" spans="2:13" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="B68" s="1"/>
+      <c r="J68" s="1"/>
+      <c r="L68" s="1"/>
+      <c r="M68" s="1"/>
+    </row>
+    <row r="69" spans="2:13" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="B69" s="1"/>
+      <c r="J69" s="1"/>
+      <c r="L69" s="1"/>
+      <c r="M69" s="1"/>
+    </row>
+    <row r="70" spans="2:13" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="B70" s="1"/>
+      <c r="J70" s="1"/>
+      <c r="L70" s="1"/>
+      <c r="M70" s="1"/>
+    </row>
+    <row r="71" spans="2:13" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="B71" s="1"/>
+      <c r="J71" s="1"/>
+      <c r="L71" s="1"/>
+      <c r="M71" s="1"/>
+    </row>
+    <row r="72" spans="2:13" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="B72" s="1"/>
+      <c r="J72" s="1"/>
+      <c r="L72" s="1"/>
+      <c r="M72" s="1"/>
+    </row>
+    <row r="73" spans="2:13" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="B73" s="1"/>
+      <c r="J73" s="1"/>
+      <c r="L73" s="1"/>
+      <c r="M73" s="1"/>
+    </row>
+    <row r="74" spans="2:13" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="B74" s="1"/>
+      <c r="J74" s="1"/>
+      <c r="L74" s="1"/>
+      <c r="M74" s="1"/>
+    </row>
+    <row r="75" spans="2:13" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="B75" s="1"/>
+      <c r="J75" s="1"/>
+      <c r="L75" s="1"/>
+      <c r="M75" s="1"/>
+    </row>
+    <row r="76" spans="2:13" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="B76" s="1"/>
+      <c r="J76" s="1"/>
+      <c r="L76" s="1"/>
+      <c r="M76" s="1"/>
+    </row>
+    <row r="77" spans="2:13" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="B77" s="1"/>
+      <c r="J77" s="1"/>
+      <c r="L77" s="1"/>
+      <c r="M77" s="1"/>
+    </row>
+    <row r="78" spans="2:13" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="B78" s="1"/>
+      <c r="J78" s="1"/>
+      <c r="L78" s="1"/>
+      <c r="M78" s="1"/>
+    </row>
+    <row r="79" spans="2:13" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="B79" s="1"/>
+      <c r="J79" s="1"/>
+      <c r="L79" s="1"/>
+      <c r="M79" s="1"/>
+    </row>
+    <row r="80" spans="2:13" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="B80" s="1"/>
+      <c r="J80" s="1"/>
+      <c r="L80" s="1"/>
+      <c r="M80" s="1"/>
+    </row>
+    <row r="81" spans="2:13" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="B81" s="1"/>
+      <c r="J81" s="1"/>
+      <c r="L81" s="1"/>
+      <c r="M81" s="1"/>
+    </row>
+    <row r="82" spans="2:13" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="B82" s="1"/>
+      <c r="J82" s="1"/>
+      <c r="L82" s="1"/>
+      <c r="M82" s="1"/>
+    </row>
+    <row r="83" spans="2:13" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="B83" s="1"/>
+      <c r="J83" s="1"/>
+      <c r="L83" s="1"/>
+      <c r="M83" s="1"/>
+    </row>
+    <row r="84" spans="2:13" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="B84" s="1"/>
+      <c r="J84" s="1"/>
+      <c r="L84" s="1"/>
+      <c r="M84" s="1"/>
+    </row>
+    <row r="85" spans="2:13" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="B85" s="1"/>
+      <c r="J85" s="1"/>
+      <c r="L85" s="1"/>
+      <c r="M85" s="1"/>
+    </row>
+    <row r="86" spans="2:13" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="B86" s="1"/>
+      <c r="J86" s="1"/>
+      <c r="L86" s="1"/>
+      <c r="M86" s="1"/>
+    </row>
+    <row r="87" spans="2:13" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="B87" s="1"/>
+      <c r="J87" s="1"/>
+      <c r="L87" s="1"/>
+      <c r="M87" s="1"/>
+    </row>
+    <row r="88" spans="2:13" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="B88" s="1"/>
+      <c r="J88" s="1"/>
+      <c r="L88" s="1"/>
+      <c r="M88" s="1"/>
+    </row>
+    <row r="89" spans="2:13" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="B89" s="1"/>
+      <c r="J89" s="1"/>
+      <c r="L89" s="1"/>
+      <c r="M89" s="1"/>
+    </row>
+    <row r="90" spans="2:13" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="B90" s="1"/>
+      <c r="J90" s="1"/>
+      <c r="L90" s="1"/>
+      <c r="M90" s="1"/>
+    </row>
+    <row r="91" spans="2:13" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="B91" s="1"/>
+      <c r="J91" s="1"/>
+      <c r="L91" s="1"/>
+      <c r="M91" s="1"/>
+    </row>
+    <row r="92" spans="2:13" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="B92" s="1"/>
+      <c r="J92" s="1"/>
+      <c r="L92" s="1"/>
+      <c r="M92" s="1"/>
+    </row>
+    <row r="93" spans="2:13" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="B93" s="1"/>
+      <c r="J93" s="1"/>
+      <c r="L93" s="1"/>
+      <c r="M93" s="1"/>
+    </row>
+    <row r="94" spans="2:13" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="B94" s="1"/>
+      <c r="J94" s="1"/>
+      <c r="L94" s="1"/>
+      <c r="M94" s="1"/>
+    </row>
+    <row r="95" spans="2:13" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="B95" s="1"/>
+      <c r="J95" s="1"/>
+      <c r="L95" s="1"/>
+      <c r="M95" s="1"/>
+    </row>
+    <row r="96" spans="2:13" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="B96" s="1"/>
+      <c r="J96" s="1"/>
+      <c r="L96" s="1"/>
+      <c r="M96" s="1"/>
+    </row>
+    <row r="97" spans="2:13" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="B97" s="1"/>
+      <c r="J97" s="1"/>
+      <c r="L97" s="1"/>
+      <c r="M97" s="1"/>
+    </row>
+    <row r="98" spans="2:13" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="B98" s="1"/>
+      <c r="J98" s="1"/>
+      <c r="L98" s="1"/>
+      <c r="M98" s="1"/>
+    </row>
+    <row r="99" spans="2:13" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="B99" s="1"/>
+      <c r="J99" s="1"/>
+      <c r="L99" s="1"/>
+      <c r="M99" s="1"/>
+    </row>
+    <row r="100" spans="2:13" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="B100" s="1"/>
+      <c r="J100" s="1"/>
+      <c r="L100" s="1"/>
+      <c r="M100" s="1"/>
+    </row>
+    <row r="101" spans="2:13" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="B101" s="1"/>
+      <c r="J101" s="1"/>
+      <c r="L101" s="1"/>
+      <c r="M101" s="1"/>
+    </row>
+    <row r="102" spans="2:13" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="B102" s="1"/>
+      <c r="J102" s="1"/>
+      <c r="L102" s="1"/>
+      <c r="M102" s="1"/>
+    </row>
+    <row r="103" spans="2:13" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="B103" s="1"/>
+      <c r="J103" s="1"/>
+      <c r="L103" s="1"/>
+      <c r="M103" s="1"/>
+    </row>
+    <row r="104" spans="2:13" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="B104" s="1"/>
+      <c r="J104" s="1"/>
+      <c r="L104" s="1"/>
+      <c r="M104" s="1"/>
+    </row>
+    <row r="105" spans="2:13" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="B105" s="1"/>
+      <c r="J105" s="1"/>
+      <c r="L105" s="1"/>
+      <c r="M105" s="1"/>
+    </row>
+    <row r="106" spans="2:13" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="B106" s="1"/>
+      <c r="J106" s="1"/>
+      <c r="L106" s="1"/>
+      <c r="M106" s="1"/>
+    </row>
+    <row r="107" spans="2:13" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="B107" s="1"/>
+      <c r="J107" s="1"/>
+      <c r="L107" s="1"/>
+      <c r="M107" s="1"/>
+    </row>
+    <row r="108" spans="2:13" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="B108" s="1"/>
+      <c r="J108" s="1"/>
+      <c r="L108" s="1"/>
+      <c r="M108" s="1"/>
+    </row>
+    <row r="109" spans="2:13" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="B109" s="1"/>
+      <c r="J109" s="1"/>
+      <c r="L109" s="1"/>
+      <c r="M109" s="1"/>
+    </row>
+    <row r="110" spans="2:13" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="B110" s="1"/>
+      <c r="J110" s="1"/>
+      <c r="L110" s="1"/>
+      <c r="M110" s="1"/>
+    </row>
+    <row r="111" spans="2:13" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="B111" s="1"/>
+      <c r="J111" s="1"/>
+      <c r="L111" s="1"/>
+      <c r="M111" s="1"/>
+    </row>
+    <row r="112" spans="2:13" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="B112" s="1"/>
+      <c r="J112" s="1"/>
+      <c r="L112" s="1"/>
+      <c r="M112" s="1"/>
+    </row>
+    <row r="113" spans="2:13" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="B113" s="1"/>
+      <c r="J113" s="1"/>
+      <c r="L113" s="1"/>
+      <c r="M113" s="1"/>
+    </row>
+    <row r="114" spans="2:13" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="B114" s="1"/>
+      <c r="J114" s="1"/>
+      <c r="L114" s="1"/>
+      <c r="M114" s="1"/>
+    </row>
+    <row r="115" spans="2:13" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="B115" s="1"/>
+      <c r="J115" s="1"/>
+      <c r="L115" s="1"/>
+      <c r="M115" s="1"/>
+    </row>
+    <row r="116" spans="2:13" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="B116" s="1"/>
+      <c r="J116" s="1"/>
+      <c r="L116" s="1"/>
+      <c r="M116" s="1"/>
+    </row>
+    <row r="117" spans="2:13" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="B117" s="1"/>
+      <c r="J117" s="1"/>
+      <c r="L117" s="1"/>
+      <c r="M117" s="1"/>
+    </row>
+    <row r="118" spans="2:13" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="B118" s="1"/>
+      <c r="J118" s="1"/>
+      <c r="L118" s="1"/>
+      <c r="M118" s="1"/>
+    </row>
+    <row r="119" spans="2:13" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="B119" s="1"/>
+      <c r="J119" s="1"/>
+      <c r="L119" s="1"/>
+      <c r="M119" s="1"/>
+    </row>
+    <row r="120" spans="2:13" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="B120" s="1"/>
+      <c r="J120" s="1"/>
+      <c r="L120" s="1"/>
+      <c r="M120" s="1"/>
+    </row>
+    <row r="121" spans="2:13" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="B121" s="1"/>
+      <c r="J121" s="1"/>
+      <c r="L121" s="1"/>
+      <c r="M121" s="1"/>
+    </row>
+    <row r="122" spans="2:13" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="B122" s="1"/>
+      <c r="J122" s="1"/>
+      <c r="L122" s="1"/>
+      <c r="M122" s="1"/>
+    </row>
+    <row r="123" spans="2:13" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="B123" s="1"/>
+      <c r="J123" s="1"/>
+      <c r="L123" s="1"/>
+      <c r="M123" s="1"/>
+    </row>
+    <row r="124" spans="2:13" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="B124" s="1"/>
+      <c r="J124" s="1"/>
+      <c r="L124" s="1"/>
+      <c r="M124" s="1"/>
+    </row>
+    <row r="125" spans="2:13" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="B125" s="1"/>
+      <c r="J125" s="1"/>
+      <c r="L125" s="1"/>
+      <c r="M125" s="1"/>
+    </row>
+    <row r="126" spans="2:13" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="B126" s="1"/>
+      <c r="J126" s="1"/>
+      <c r="L126" s="1"/>
+      <c r="M126" s="1"/>
+    </row>
+    <row r="127" spans="2:13" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="B127" s="1"/>
+      <c r="J127" s="1"/>
+      <c r="L127" s="1"/>
+      <c r="M127" s="1"/>
+    </row>
+    <row r="128" spans="2:13" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="B128" s="1"/>
+      <c r="J128" s="1"/>
+      <c r="L128" s="1"/>
+      <c r="M128" s="1"/>
+    </row>
+    <row r="129" spans="2:13" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="B129" s="1"/>
+      <c r="J129" s="1"/>
+      <c r="L129" s="1"/>
+      <c r="M129" s="1"/>
+    </row>
+    <row r="130" spans="2:13" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="B130" s="1"/>
+      <c r="J130" s="1"/>
+      <c r="L130" s="1"/>
+      <c r="M130" s="1"/>
+    </row>
+    <row r="131" spans="2:13" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="B131" s="1"/>
+      <c r="J131" s="1"/>
+      <c r="L131" s="1"/>
+      <c r="M131" s="1"/>
+    </row>
+    <row r="132" spans="2:13" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="B132" s="1"/>
+      <c r="J132" s="1"/>
+      <c r="L132" s="1"/>
+      <c r="M132" s="1"/>
+    </row>
+    <row r="133" spans="2:13" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="B133" s="1"/>
+      <c r="J133" s="1"/>
+      <c r="L133" s="1"/>
+      <c r="M133" s="1"/>
+    </row>
+    <row r="134" spans="2:13" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="B134" s="1"/>
+      <c r="J134" s="1"/>
+      <c r="L134" s="1"/>
+      <c r="M134" s="1"/>
+    </row>
+    <row r="135" spans="2:13" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="B135" s="1"/>
+      <c r="J135" s="1"/>
+      <c r="L135" s="1"/>
+      <c r="M135" s="1"/>
+    </row>
+    <row r="136" spans="2:13" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="B136" s="1"/>
+      <c r="J136" s="1"/>
+      <c r="L136" s="1"/>
+      <c r="M136" s="1"/>
+    </row>
+    <row r="137" spans="2:13" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="B137" s="1"/>
+      <c r="J137" s="1"/>
+      <c r="L137" s="1"/>
+      <c r="M137" s="1"/>
+    </row>
+    <row r="138" spans="2:13" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="B138" s="1"/>
+      <c r="J138" s="1"/>
+      <c r="L138" s="1"/>
+      <c r="M138" s="1"/>
+    </row>
+    <row r="139" spans="2:13" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="B139" s="1"/>
+      <c r="J139" s="1"/>
+      <c r="L139" s="1"/>
+      <c r="M139" s="1"/>
+    </row>
+    <row r="140" spans="2:13" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="B140" s="1"/>
+      <c r="J140" s="1"/>
+      <c r="L140" s="1"/>
+      <c r="M140" s="1"/>
+    </row>
+    <row r="141" spans="2:13" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="B141" s="1"/>
+      <c r="J141" s="1"/>
+      <c r="L141" s="1"/>
+      <c r="M141" s="1"/>
+    </row>
+    <row r="142" spans="2:13" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="B142" s="1"/>
+      <c r="J142" s="1"/>
+      <c r="L142" s="1"/>
+      <c r="M142" s="1"/>
+    </row>
+    <row r="143" spans="2:13" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="B143" s="1"/>
+      <c r="J143" s="1"/>
+      <c r="L143" s="1"/>
+      <c r="M143" s="1"/>
+    </row>
+    <row r="144" spans="2:13" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="B144" s="1"/>
+      <c r="J144" s="1"/>
+      <c r="L144" s="1"/>
+      <c r="M144" s="1"/>
+    </row>
+    <row r="145" spans="2:13" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="B145" s="1"/>
+      <c r="J145" s="1"/>
+      <c r="L145" s="1"/>
+      <c r="M145" s="1"/>
+    </row>
+    <row r="146" spans="2:13" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="B146" s="1"/>
+      <c r="J146" s="1"/>
+      <c r="L146" s="1"/>
+      <c r="M146" s="1"/>
+    </row>
+    <row r="147" spans="2:13" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="B147" s="1"/>
+      <c r="J147" s="1"/>
+      <c r="L147" s="1"/>
+      <c r="M147" s="1"/>
+    </row>
+    <row r="148" spans="2:13" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="B148" s="1"/>
+      <c r="J148" s="1"/>
+      <c r="L148" s="1"/>
+      <c r="M148" s="1"/>
+    </row>
+    <row r="149" spans="2:13" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="B149" s="1"/>
+      <c r="J149" s="1"/>
+      <c r="L149" s="1"/>
+      <c r="M149" s="1"/>
+    </row>
+    <row r="150" spans="2:13" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="B150" s="1"/>
+      <c r="J150" s="1"/>
+      <c r="L150" s="1"/>
+      <c r="M150" s="1"/>
+    </row>
+    <row r="151" spans="2:13" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="B151" s="1"/>
+      <c r="J151" s="1"/>
+      <c r="L151" s="1"/>
+      <c r="M151" s="1"/>
+    </row>
+    <row r="152" spans="2:13" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="B152" s="1"/>
+      <c r="J152" s="1"/>
+      <c r="L152" s="1"/>
+      <c r="M152" s="1"/>
+    </row>
+    <row r="153" spans="2:13" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="B153" s="1"/>
+      <c r="J153" s="1"/>
+      <c r="L153" s="1"/>
+      <c r="M153" s="1"/>
+    </row>
+    <row r="154" spans="2:13" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="B154" s="1"/>
+      <c r="J154" s="1"/>
+      <c r="L154" s="1"/>
+      <c r="M154" s="1"/>
+    </row>
+    <row r="155" spans="2:13" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="B155" s="1"/>
+      <c r="J155" s="1"/>
+      <c r="L155" s="1"/>
+      <c r="M155" s="1"/>
+    </row>
+    <row r="156" spans="2:13" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="B156" s="1"/>
+      <c r="J156" s="1"/>
+      <c r="L156" s="1"/>
+      <c r="M156" s="1"/>
+    </row>
+    <row r="157" spans="2:13" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="B157" s="1"/>
+      <c r="J157" s="1"/>
+      <c r="L157" s="1"/>
+      <c r="M157" s="1"/>
+    </row>
+    <row r="158" spans="2:13" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="B158" s="1"/>
+      <c r="J158" s="1"/>
+      <c r="L158" s="1"/>
+      <c r="M158" s="1"/>
+    </row>
+    <row r="159" spans="2:13" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="B159" s="1"/>
+      <c r="J159" s="1"/>
+      <c r="L159" s="1"/>
+      <c r="M159" s="1"/>
+    </row>
+    <row r="160" spans="2:13" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="B160" s="1"/>
+      <c r="J160" s="1"/>
+      <c r="L160" s="1"/>
+      <c r="M160" s="1"/>
+    </row>
+    <row r="161" spans="2:13" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="B161" s="1"/>
+      <c r="J161" s="1"/>
+      <c r="L161" s="1"/>
+      <c r="M161" s="1"/>
+    </row>
+    <row r="162" spans="2:13" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="B162" s="1"/>
+      <c r="J162" s="1"/>
+      <c r="L162" s="1"/>
+      <c r="M162" s="1"/>
+    </row>
+    <row r="163" spans="2:13" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="B163" s="1"/>
+      <c r="J163" s="1"/>
+      <c r="L163" s="1"/>
+      <c r="M163" s="1"/>
+    </row>
+    <row r="164" spans="2:13" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="B164" s="1"/>
+      <c r="J164" s="1"/>
+      <c r="L164" s="1"/>
+      <c r="M164" s="1"/>
+    </row>
+    <row r="165" spans="2:13" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="B165" s="1"/>
+      <c r="J165" s="1"/>
+      <c r="L165" s="1"/>
+      <c r="M165" s="1"/>
+    </row>
+    <row r="166" spans="2:13" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="B166" s="1"/>
+      <c r="J166" s="1"/>
+      <c r="L166" s="1"/>
+      <c r="M166" s="1"/>
+    </row>
+    <row r="167" spans="2:13" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="B167" s="1"/>
+      <c r="J167" s="1"/>
+      <c r="L167" s="1"/>
+      <c r="M167" s="1"/>
+    </row>
+    <row r="168" spans="2:13" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="B168" s="1"/>
+      <c r="J168" s="1"/>
+      <c r="L168" s="1"/>
+      <c r="M168" s="1"/>
+    </row>
+    <row r="169" spans="2:13" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="B169" s="1"/>
+      <c r="J169" s="1"/>
+      <c r="L169" s="1"/>
+      <c r="M169" s="1"/>
+    </row>
+    <row r="170" spans="2:13" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="B170" s="1"/>
+      <c r="J170" s="1"/>
+      <c r="L170" s="1"/>
+      <c r="M170" s="1"/>
+    </row>
+    <row r="171" spans="2:13" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="B171" s="1"/>
+      <c r="J171" s="1"/>
+      <c r="L171" s="1"/>
+      <c r="M171" s="1"/>
+    </row>
+    <row r="172" spans="2:13" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="B172" s="1"/>
+      <c r="J172" s="1"/>
+      <c r="L172" s="1"/>
+      <c r="M172" s="1"/>
+    </row>
+    <row r="173" spans="2:13" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="B173" s="1"/>
+      <c r="J173" s="1"/>
+      <c r="L173" s="1"/>
+      <c r="M173" s="1"/>
+    </row>
+    <row r="174" spans="2:13" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="B174" s="1"/>
+      <c r="J174" s="1"/>
+      <c r="L174" s="1"/>
+      <c r="M174" s="1"/>
+    </row>
+    <row r="175" spans="2:13" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="B175" s="1"/>
+      <c r="J175" s="1"/>
+      <c r="L175" s="1"/>
+      <c r="M175" s="1"/>
+    </row>
+    <row r="176" spans="2:13" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="B176" s="1"/>
+      <c r="J176" s="1"/>
+      <c r="L176" s="1"/>
+      <c r="M176" s="1"/>
+    </row>
+    <row r="177" spans="2:13" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="B177" s="1"/>
+      <c r="J177" s="1"/>
+      <c r="L177" s="1"/>
+      <c r="M177" s="1"/>
+    </row>
+    <row r="178" spans="2:13" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="B178" s="1"/>
+      <c r="J178" s="1"/>
+      <c r="L178" s="1"/>
+      <c r="M178" s="1"/>
+    </row>
+    <row r="179" spans="2:13" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="B179" s="1"/>
+      <c r="J179" s="1"/>
+      <c r="L179" s="1"/>
+      <c r="M179" s="1"/>
+    </row>
+    <row r="180" spans="2:13" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="B180" s="1"/>
+      <c r="J180" s="1"/>
+      <c r="L180" s="1"/>
+      <c r="M180" s="1"/>
+    </row>
+    <row r="181" spans="2:13" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="B181" s="1"/>
+      <c r="J181" s="1"/>
+      <c r="L181" s="1"/>
+      <c r="M181" s="1"/>
+    </row>
+    <row r="182" spans="2:13" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="B182" s="1"/>
+      <c r="J182" s="1"/>
+      <c r="L182" s="1"/>
+      <c r="M182" s="1"/>
+    </row>
+    <row r="183" spans="2:13" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="B183" s="1"/>
+      <c r="J183" s="1"/>
+      <c r="L183" s="1"/>
+      <c r="M183" s="1"/>
+    </row>
+    <row r="184" spans="2:13" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="B184" s="1"/>
+      <c r="J184" s="1"/>
+      <c r="L184" s="1"/>
+      <c r="M184" s="1"/>
+    </row>
+    <row r="185" spans="2:13" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="B185" s="1"/>
+      <c r="J185" s="1"/>
+      <c r="L185" s="1"/>
+      <c r="M185" s="1"/>
+    </row>
+    <row r="186" spans="2:13" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="B186" s="1"/>
+      <c r="J186" s="1"/>
+      <c r="L186" s="1"/>
+      <c r="M186" s="1"/>
+    </row>
+    <row r="187" spans="2:13" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="B187" s="1"/>
+      <c r="J187" s="1"/>
+      <c r="L187" s="1"/>
+      <c r="M187" s="1"/>
+    </row>
+    <row r="188" spans="2:13" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="B188" s="1"/>
+      <c r="J188" s="1"/>
+      <c r="L188" s="1"/>
+      <c r="M188" s="1"/>
+    </row>
+    <row r="189" spans="2:13" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="B189" s="1"/>
+      <c r="J189" s="1"/>
+      <c r="L189" s="1"/>
+      <c r="M189" s="1"/>
+    </row>
+    <row r="190" spans="2:13" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="B190" s="1"/>
+      <c r="J190" s="1"/>
+      <c r="L190" s="1"/>
+      <c r="M190" s="1"/>
+    </row>
+    <row r="191" spans="2:13" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="B191" s="1"/>
+      <c r="J191" s="1"/>
+      <c r="L191" s="1"/>
+      <c r="M191" s="1"/>
+    </row>
+    <row r="192" spans="2:13" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="B192" s="1"/>
+      <c r="J192" s="1"/>
+      <c r="L192" s="1"/>
+      <c r="M192" s="1"/>
+    </row>
+    <row r="193" spans="2:13" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="B193" s="1"/>
+      <c r="J193" s="1"/>
+      <c r="L193" s="1"/>
+      <c r="M193" s="1"/>
+    </row>
+    <row r="194" spans="2:13" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="B194" s="1"/>
+      <c r="J194" s="1"/>
+      <c r="L194" s="1"/>
+      <c r="M194" s="1"/>
+    </row>
+    <row r="195" spans="2:13" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="B195" s="1"/>
+      <c r="J195" s="1"/>
+      <c r="L195" s="1"/>
+      <c r="M195" s="1"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:O1" xr:uid="{E53E83C4-68F7-4929-AA83-3F95502173FC}"/>
@@ -3106,7 +4530,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2720FBDC-F538-4F79-9784-827E5ACB3995}">
   <dimension ref="A1:P130"/>
   <sheetViews>

</xml_diff>

<commit_message>
changes acc to tickets #446, #438 and #452
</commit_message>
<xml_diff>
--- a/Deliverables/RULES/USDM_CORE_Rules_Changes.xlsx
+++ b/Deliverables/RULES/USDM_CORE_Rules_Changes.xlsx
@@ -1,24 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Stack\CL027\Publish\CORE\3.5\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Stack\CL027\Publish\CORE\3.6\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1F7C510-A7C2-46C6-846B-B820F9970ACA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7E2AF5C-8C65-4C65-99FC-F0CB8BCE0B73}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-12165" yWindow="-18450" windowWidth="27495" windowHeight="15225" xr2:uid="{418CF395-400B-43AB-9594-6DFC1F089218}"/>
+    <workbookView xWindow="-10515" yWindow="-18885" windowWidth="25020" windowHeight="15225" xr2:uid="{418CF395-400B-43AB-9594-6DFC1F089218}"/>
   </bookViews>
   <sheets>
-    <sheet name="Changes release 3.4-&gt;3.5" sheetId="7" r:id="rId1"/>
-    <sheet name="Changes release 3.3-&gt;3.4" sheetId="5" r:id="rId2"/>
-    <sheet name="Changes release 3.1-&gt;3.3" sheetId="6" r:id="rId3"/>
+    <sheet name="Changes release 3.5-&gt;3.6" sheetId="8" r:id="rId1"/>
+    <sheet name="Changes release 3.4-&gt;3.5" sheetId="7" r:id="rId2"/>
+    <sheet name="Changes release 3.3-&gt;3.4" sheetId="5" r:id="rId3"/>
+    <sheet name="Changes release 3.1-&gt;3.3" sheetId="6" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Changes release 3.3-&gt;3.4'!$A$1:$O$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'Changes release 3.3-&gt;3.4'!$A$1:$O$1</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -41,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2393" uniqueCount="616">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1104" uniqueCount="732">
   <si>
     <t>All</t>
   </si>
@@ -1889,6 +1890,354 @@
   </si>
   <si>
     <t>Textual statement of rule (old, if changed)</t>
+  </si>
+  <si>
+    <t>An administrable dose form must be specfied according to the extensible Pharmaceutical Dosage Form (C66726) SDTM codelist (e.g. an entry with a code or decode used from the codelist should be consistent with the full entry in the codelist).</t>
+  </si>
+  <si>
+    <t>AdministrableProduct</t>
+  </si>
+  <si>
+    <t>administrableDoseForm</t>
+  </si>
+  <si>
+    <t>CHK0203</t>
+  </si>
+  <si>
+    <t>An administrable product property type must be specified according to the extensible administrable property type (Cxxxx) DDF codelist (e.g. an entry with a code or decode used from the codelist should be consistent with the full entry in the codelist).</t>
+  </si>
+  <si>
+    <t>AdministrableProductProperty</t>
+  </si>
+  <si>
+    <t>CHK0204</t>
+  </si>
+  <si>
+    <t>If a dose is specified then a corresponding frequency must also be specified.</t>
+  </si>
+  <si>
+    <t>Administration</t>
+  </si>
+  <si>
+    <t>dose</t>
+  </si>
+  <si>
+    <t>CHK0202</t>
+  </si>
+  <si>
+    <t>If a dose is specified then a corresponding administrable product must also be specified and vice versa.</t>
+  </si>
+  <si>
+    <t>dose, administrableProduct</t>
+  </si>
+  <si>
+    <t>CHK0220</t>
+  </si>
+  <si>
+    <t>If an administration's dose is specified then a corresponding route is expected and vice versa.</t>
+  </si>
+  <si>
+    <t>dose, route</t>
+  </si>
+  <si>
+    <t>CHK0201</t>
+  </si>
+  <si>
+    <t>An administration's frequency must be specfied according to the extensible Frequency (C71113) SDTM codelist (e.g. an entry with a code or decode used from the codelist should be consistent with the full entry in the codelist).</t>
+  </si>
+  <si>
+    <t>CHK0199</t>
+  </si>
+  <si>
+    <t>An administration's route must be specfied according to the extensible Route of Administration Response (C66729) SDTM codelist (e.g. an entry with a code or decode used from the codelist should be consistent with the full entry in the codelist).</t>
+  </si>
+  <si>
+    <t>CHK0200</t>
+  </si>
+  <si>
+    <t>An agent administration's frequency must be specfied according to the extensible Frequency (C71113) SDTM codelist (e.g. an entry with a code or decode used from the codelist should be consistent with the full entry in the codelist).</t>
+  </si>
+  <si>
+    <t>An agent administration's route must be specfied according to the extensible Route of Administration Response (C66729) SDTM codelist (e.g. an entry with a code or decode used from the codelist should be consistent with the full entry in the codelist).</t>
+  </si>
+  <si>
+    <t>All standard code aliases referenced by an instance of the alias code class must be unique.</t>
+  </si>
+  <si>
+    <t>DDF00052</t>
+  </si>
+  <si>
+    <t>An encounter's contact modes must be specfied according to the Mode of Subject Contact (C171445) SDTM codelist (e.g. an entry with a code or decode used from the codelist should be consistent with the full entry in the codelist).</t>
+  </si>
+  <si>
+    <t>An encounter's environmental setting must be specified according to the extensible Environmental Setting (C127262) SDTM codelist (e.g. an entry with a code or decode used from the codelist should be consistent with the full entry in the codelist).</t>
+  </si>
+  <si>
+    <t>An encounter type must be specified according to the extensible encounter type (C188728) DDF codelist (e.g. an entry with a code or decode used from the codelist should be consistent with the full entry in the codelist).</t>
+  </si>
+  <si>
+    <t>CHK0218</t>
+  </si>
+  <si>
+    <t>An endpoint level must be specified using the endpoint level (C188726) DDF codelist.</t>
+  </si>
+  <si>
+    <t>CHK0216</t>
+  </si>
+  <si>
+    <t>A study geographic scope type must be specified using the geographic scope type (C207412) DDF codelist.</t>
+  </si>
+  <si>
+    <t>GeographicScope</t>
+  </si>
+  <si>
+    <t>CHK0211</t>
+  </si>
+  <si>
+    <t>A governance date type must be specified according to the extensible governance date type (C207413) DDF codelist (e.g. an entry with a code or decode used from the codelist should be consistent with the full entry in the codelist).</t>
+  </si>
+  <si>
+    <t>CHK0209</t>
+  </si>
+  <si>
+    <t>A masking role must be specifed according to the extensible masking role (C207414) DDF codelist (e.g. an entry with a code or decode used from the codelist should be consistent with the full entry in the codelist).</t>
+  </si>
+  <si>
+    <t>Section numbers are expected to be continuous. No gaps are expected in numbering.</t>
+  </si>
+  <si>
+    <t>sectionNumber, previous, next</t>
+  </si>
+  <si>
+    <t>Section numbers are expected to follow the ordering as specified in the previous next attributes.</t>
+  </si>
+  <si>
+    <t>An objective level must be specified using the objective level (C188725) DDF codelist.</t>
+  </si>
+  <si>
+    <t>CHK0215</t>
+  </si>
+  <si>
+    <t>An organization type must be specified according to the extensible organization type (C188724) DDF codelist (e.g. an entry with a code or decode used from the codelist should be consistent with the full entry in the codelist).</t>
+  </si>
+  <si>
+    <t>Organization, ResearchOrganization</t>
+  </si>
+  <si>
+    <t>organizationType</t>
+  </si>
+  <si>
+    <t>CHK0205</t>
+  </si>
+  <si>
+    <t>The minimum value of a range must be less than the maximum value of the range.</t>
+  </si>
+  <si>
+    <t>CHK0198</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A unit must be coded according to the extensible unit (C71620) SDTM codelist (e.g. an entry with a code or decode used from the codelist should be consistent with the full entry in the codelist). </t>
+  </si>
+  <si>
+    <t>Range, Quantity</t>
+  </si>
+  <si>
+    <t>CHK0212</t>
+  </si>
+  <si>
+    <t>A reference identifier type must be specified according to the extensible reference identifier type (Cxxx) DDF codelist  (e.g. an entry with a code or decode used from the codelist should be consistent with the full entry in the codelist).</t>
+  </si>
+  <si>
+    <t>ReferenceIdentifier</t>
+  </si>
+  <si>
+    <t>CHK0214</t>
+  </si>
+  <si>
+    <t>A unit must be specified for every strength denominator and numerator</t>
+  </si>
+  <si>
+    <t>Strength</t>
+  </si>
+  <si>
+    <t>numerator, denominator</t>
+  </si>
+  <si>
+    <t>CHK0221</t>
+  </si>
+  <si>
+    <t>A study amendment reason must be coded using the study amendment reason (C207415) DDF codelist.</t>
+  </si>
+  <si>
+    <t>code</t>
+  </si>
+  <si>
+    <t>CHK0210</t>
+  </si>
+  <si>
+    <t>A study arm data origin type must be specified according to the extensible data origin type (C188727) DDF codelist  (e.g. an entry with a code or decode used from the codelist should be consistent with the full entry in the codelist).</t>
+  </si>
+  <si>
+    <t>dataOriginType</t>
+  </si>
+  <si>
+    <t>CHK0217</t>
+  </si>
+  <si>
+    <t>A study arm must only reference cohorts that are defined within the same study design as the study arm.</t>
+  </si>
+  <si>
+    <t>A study definition document type must be specifed according to the extensible XXX (Cnnn) DDF codelist (e.g. an entry with a code or decode used from the codelist should be consistent with the full entry in the codelist).</t>
+  </si>
+  <si>
+    <t>dateValues</t>
+  </si>
+  <si>
+    <t>CHK0207</t>
+  </si>
+  <si>
+    <t>Within a study protocol document version, if a date of a specific type exists with a global geographic scope then no other dates are expected with the same type.</t>
+  </si>
+  <si>
+    <t>CHK0208</t>
+  </si>
+  <si>
+    <t>A study definition document version's status must be specifed using the status Value Set Terminology (C188723) DDF codelist.</t>
+  </si>
+  <si>
+    <t>A study design's blinding schema must be specified according to the extensible Trial Blinding Schema Response (C66735) SDTM codelist (e.g. an entry with a code or decode used from the codelist should be consistent with the full entry in the codelist).</t>
+  </si>
+  <si>
+    <t>A study design's characteristics must be specifed according to the Study design characteristics (C207416) DDF codelist (e.g. an entry with a code or decode used from the codelist should be consistent with the full entry in the codelist).</t>
+  </si>
+  <si>
+    <t>A study design's intervention model must be specified according to the extensible Intervention Model Response (C99076) SDTM codelist (e.g. an entry with a code or decode used from the codelist should be consistent with the full entry in the codelist).</t>
+  </si>
+  <si>
+    <t>A study design's trial intent types must be specified according to the extensible Trial Intent Type Response (C66736) SDTM codelist (e.g. an entry with a code or decode used from the codelist should be consistent with the full entry in the codelist).</t>
+  </si>
+  <si>
+    <t>A study design's trial types must be specified according to the extensible Trial Type Response (C66739) SDTM codelist (e.g. an entry with a code or decode used from the codelist should be consistent with the full entry in the codelist).</t>
+  </si>
+  <si>
+    <t>Range =&gt; StudyDesignPopulation, StudyCohort</t>
+  </si>
+  <si>
+    <t>unit =&gt; plannedAge</t>
+  </si>
+  <si>
+    <t>plannedEnrollmentNumber, plannedCompletionNumber</t>
+  </si>
+  <si>
+    <t>DDF00043</t>
+  </si>
+  <si>
+    <t>unit =&gt; plannedEnrollmentNumber, plannedCompletionNumber</t>
+  </si>
+  <si>
+    <t>A planned sex must be specfied using to the Sex of participants (C66732) SDTM codelist.</t>
+  </si>
+  <si>
+    <t>CHK0206</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Every study version must have exactly one study identifier with an identifier scope that references a clinical study sponsor organization. </t>
+  </si>
+  <si>
+    <t>scope</t>
+  </si>
+  <si>
+    <t>CHK0193</t>
+  </si>
+  <si>
+    <t>An identified organization is not expected to have more than 1 identifier for the study.</t>
+  </si>
+  <si>
+    <t>CHK0197</t>
+  </si>
+  <si>
+    <t>Every identifier must be unique within the scope of an identified organization.</t>
+  </si>
+  <si>
+    <t>studyIdentifier</t>
+  </si>
+  <si>
+    <t>CHK0194</t>
+  </si>
+  <si>
+    <t>CHK0196</t>
+  </si>
+  <si>
+    <t>StudyIdentifier, ReferenceIdentifier, AdministrableProductIdentifier</t>
+  </si>
+  <si>
+    <t>CHK0195</t>
+  </si>
+  <si>
+    <t>A study intervention's product designation must be specifed using the product Designation (C207418) DDF codelist.</t>
+  </si>
+  <si>
+    <t>A study intervention's role must be specifed using the study intervention role (C207417) DDF codelist.</t>
+  </si>
+  <si>
+    <t>GovernanceDate =&gt; StudyProtocolDocumentVersion</t>
+  </si>
+  <si>
+    <t>type, geographicScopes =&gt; dateValues</t>
+  </si>
+  <si>
+    <t>A study title type must be specified using the study title type (C207419) DDF codelist.</t>
+  </si>
+  <si>
+    <t>CHK0213</t>
+  </si>
+  <si>
+    <t>GovernanceDate =&gt; StudyVersion</t>
+  </si>
+  <si>
+    <t>Within a study version, if a date of a specific type exists with a global geographic scope then no other dates are expected with the same type.</t>
+  </si>
+  <si>
+    <t>A study version's study phase must be specifed according to the extensible Trial Phase Response (C66737) SDTM codelist (e.g. an entry with a code or decode used from the codelist should be consistent with the full entry in the codelist).</t>
+  </si>
+  <si>
+    <t>titles</t>
+  </si>
+  <si>
+    <t>StudyTitle =&gt; StudyVersion</t>
+  </si>
+  <si>
+    <t>type =&gt; titles</t>
+  </si>
+  <si>
+    <t>Every study version must have a title of type "Official Study Title".</t>
+  </si>
+  <si>
+    <t>SubjectEnrollment</t>
+  </si>
+  <si>
+    <t>Quantity =&gt; SubjectEnrollment</t>
+  </si>
+  <si>
+    <t>unit =&gt; quantity</t>
+  </si>
+  <si>
+    <t>A referenced substance must not have any references itself.</t>
+  </si>
+  <si>
+    <t>Substance</t>
+  </si>
+  <si>
+    <t>referenceSubstance</t>
+  </si>
+  <si>
+    <t>CHK0219</t>
+  </si>
+  <si>
+    <t>A timing must only be specified as being relative to/from a scheduled activity/decision instance that is defined within the same timeline as the timing.</t>
+  </si>
+  <si>
+    <t>DDF00046</t>
   </si>
 </sst>
 </file>
@@ -2325,11 +2674,2997 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A424D0F2-3B88-4770-93C0-98D49DE8D516}">
+  <dimension ref="A1:O63"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="2" max="2" width="59.6328125" customWidth="1"/>
+    <col min="4" max="4" width="24.453125" customWidth="1"/>
+    <col min="5" max="5" width="27.1796875" customWidth="1"/>
+    <col min="8" max="8" width="17.90625" customWidth="1"/>
+    <col min="10" max="10" width="63.6328125" customWidth="1"/>
+    <col min="11" max="11" width="18.7265625" customWidth="1"/>
+    <col min="12" max="12" width="20.36328125" customWidth="1"/>
+    <col min="13" max="13" width="24" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:15" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>600</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>546</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>547</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>548</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>549</v>
+      </c>
+      <c r="F1" s="8" t="s">
+        <v>550</v>
+      </c>
+      <c r="G1" s="8" t="s">
+        <v>551</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>552</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>306</v>
+      </c>
+      <c r="J1" s="8" t="s">
+        <v>615</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>395</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>545</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>396</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>397</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" ht="58" x14ac:dyDescent="0.35">
+      <c r="A2" s="7" t="s">
+        <v>415</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>616</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>617</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>618</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="I2" t="s">
+        <v>619</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="K2" t="s">
+        <v>122</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="M2" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="N2" t="s">
+        <v>122</v>
+      </c>
+      <c r="O2" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" ht="58" x14ac:dyDescent="0.35">
+      <c r="A3" s="7" t="s">
+        <v>415</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>620</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>621</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="I3" t="s">
+        <v>622</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="K3" t="s">
+        <v>122</v>
+      </c>
+      <c r="L3" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="M3" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="N3" t="s">
+        <v>122</v>
+      </c>
+      <c r="O3" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" ht="29" x14ac:dyDescent="0.35">
+      <c r="A4" s="7" t="s">
+        <v>415</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>623</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>624</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>625</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="I4" t="s">
+        <v>626</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="K4" t="s">
+        <v>122</v>
+      </c>
+      <c r="L4" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="M4" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="N4" t="s">
+        <v>122</v>
+      </c>
+      <c r="O4" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" ht="29" x14ac:dyDescent="0.35">
+      <c r="A5" s="7" t="s">
+        <v>415</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>627</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>624</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>628</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="H5" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="I5" t="s">
+        <v>629</v>
+      </c>
+      <c r="J5" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="K5" t="s">
+        <v>122</v>
+      </c>
+      <c r="L5" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="M5" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="N5" t="s">
+        <v>122</v>
+      </c>
+      <c r="O5" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" ht="29" x14ac:dyDescent="0.35">
+      <c r="A6" s="7" t="s">
+        <v>415</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>630</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>624</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>631</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="H6" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="I6" t="s">
+        <v>632</v>
+      </c>
+      <c r="J6" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="K6" t="s">
+        <v>122</v>
+      </c>
+      <c r="L6" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="M6" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="N6" t="s">
+        <v>122</v>
+      </c>
+      <c r="O6" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" ht="58" x14ac:dyDescent="0.35">
+      <c r="A7" s="7" t="s">
+        <v>415</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>633</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>624</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>177</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="G7" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="H7" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="I7" t="s">
+        <v>634</v>
+      </c>
+      <c r="J7" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="K7" t="s">
+        <v>122</v>
+      </c>
+      <c r="L7" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="M7" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="N7" t="s">
+        <v>122</v>
+      </c>
+      <c r="O7" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" ht="58" x14ac:dyDescent="0.35">
+      <c r="A8" s="7" t="s">
+        <v>415</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>635</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>624</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>252</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="G8" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="H8" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="I8" t="s">
+        <v>636</v>
+      </c>
+      <c r="J8" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="K8" t="s">
+        <v>122</v>
+      </c>
+      <c r="L8" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="M8" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="N8" t="s">
+        <v>122</v>
+      </c>
+      <c r="O8" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" ht="58" x14ac:dyDescent="0.35">
+      <c r="A9" s="7" t="s">
+        <v>416</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>637</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>176</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>177</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="G9" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="H9" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="I9" t="s">
+        <v>174</v>
+      </c>
+      <c r="J9" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="K9" t="s">
+        <v>122</v>
+      </c>
+      <c r="L9" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="M9" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="N9" t="s">
+        <v>122</v>
+      </c>
+      <c r="O9" t="s">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" ht="58" x14ac:dyDescent="0.35">
+      <c r="A10" s="7" t="s">
+        <v>416</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>638</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>176</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>252</v>
+      </c>
+      <c r="F10" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="G10" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="H10" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="I10" t="s">
+        <v>250</v>
+      </c>
+      <c r="J10" s="1" t="s">
+        <v>251</v>
+      </c>
+      <c r="K10" t="s">
+        <v>122</v>
+      </c>
+      <c r="L10" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="M10" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="N10" t="s">
+        <v>122</v>
+      </c>
+      <c r="O10" t="s">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" ht="29" x14ac:dyDescent="0.35">
+      <c r="A11" s="7" t="s">
+        <v>416</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>639</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="F11" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="G11" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="H11" s="3" t="s">
+        <v>640</v>
+      </c>
+      <c r="I11" t="s">
+        <v>116</v>
+      </c>
+      <c r="J11" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="K11" t="s">
+        <v>122</v>
+      </c>
+      <c r="L11" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="M11" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="N11" t="s">
+        <v>122</v>
+      </c>
+      <c r="O11" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" ht="58" x14ac:dyDescent="0.35">
+      <c r="A12" s="7" t="s">
+        <v>416</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>641</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>258</v>
+      </c>
+      <c r="F12" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="G12" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="H12" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="I12" t="s">
+        <v>284</v>
+      </c>
+      <c r="J12" s="1" t="s">
+        <v>285</v>
+      </c>
+      <c r="K12" t="s">
+        <v>122</v>
+      </c>
+      <c r="L12" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="M12" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="N12" t="s">
+        <v>122</v>
+      </c>
+      <c r="O12" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" ht="58" x14ac:dyDescent="0.35">
+      <c r="A13" s="7" t="s">
+        <v>416</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>642</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>166</v>
+      </c>
+      <c r="F13" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="G13" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="H13" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="I13" t="s">
+        <v>282</v>
+      </c>
+      <c r="J13" s="1" t="s">
+        <v>283</v>
+      </c>
+      <c r="K13" t="s">
+        <v>122</v>
+      </c>
+      <c r="L13" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="M13" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="N13" t="s">
+        <v>122</v>
+      </c>
+      <c r="O13" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" ht="58" x14ac:dyDescent="0.35">
+      <c r="A14" s="7" t="s">
+        <v>416</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>642</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="E14" s="3" t="s">
+        <v>295</v>
+      </c>
+      <c r="F14" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="G14" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="H14" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="I14" t="s">
+        <v>296</v>
+      </c>
+      <c r="J14" s="1" t="s">
+        <v>297</v>
+      </c>
+      <c r="K14" t="s">
+        <v>122</v>
+      </c>
+      <c r="L14" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="M14" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="N14" t="s">
+        <v>122</v>
+      </c>
+      <c r="O14" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" ht="58" x14ac:dyDescent="0.35">
+      <c r="A15" s="7" t="s">
+        <v>415</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>643</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="E15" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="F15" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="G15" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="H15" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="I15" t="s">
+        <v>644</v>
+      </c>
+      <c r="J15" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="K15" t="s">
+        <v>122</v>
+      </c>
+      <c r="L15" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="M15" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="N15" t="s">
+        <v>122</v>
+      </c>
+      <c r="O15" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" ht="29" x14ac:dyDescent="0.35">
+      <c r="A16" s="7" t="s">
+        <v>415</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>645</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="E16" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="F16" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="G16" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="H16" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="I16" t="s">
+        <v>646</v>
+      </c>
+      <c r="J16" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="K16" t="s">
+        <v>122</v>
+      </c>
+      <c r="L16" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="M16" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="N16" t="s">
+        <v>122</v>
+      </c>
+      <c r="O16" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15" ht="29" x14ac:dyDescent="0.35">
+      <c r="A17" s="7" t="s">
+        <v>415</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>647</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>648</v>
+      </c>
+      <c r="E17" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="F17" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="G17" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="H17" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="I17" t="s">
+        <v>649</v>
+      </c>
+      <c r="J17" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="K17" t="s">
+        <v>122</v>
+      </c>
+      <c r="L17" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="M17" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="N17" t="s">
+        <v>122</v>
+      </c>
+      <c r="O17" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15" ht="58" x14ac:dyDescent="0.35">
+      <c r="A18" s="7" t="s">
+        <v>415</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>650</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D18" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="E18" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="F18" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="G18" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="H18" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="I18" t="s">
+        <v>651</v>
+      </c>
+      <c r="J18" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="K18" t="s">
+        <v>122</v>
+      </c>
+      <c r="L18" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="M18" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="N18" t="s">
+        <v>122</v>
+      </c>
+      <c r="O18" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A19" s="7" t="s">
+        <v>416</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>652</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D19" s="3" t="s">
+        <v>207</v>
+      </c>
+      <c r="E19" s="3" t="s">
+        <v>173</v>
+      </c>
+      <c r="F19" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="G19" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="H19" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="I19" t="s">
+        <v>205</v>
+      </c>
+      <c r="J19" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="K19" t="s">
+        <v>122</v>
+      </c>
+      <c r="L19" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="M19" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="N19" t="s">
+        <v>122</v>
+      </c>
+      <c r="O19" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15" ht="29" x14ac:dyDescent="0.35">
+      <c r="A20" s="7" t="s">
+        <v>417</v>
+      </c>
+      <c r="B20" s="3">
+        <v>0</v>
+      </c>
+      <c r="C20" s="3">
+        <v>0</v>
+      </c>
+      <c r="D20" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="E20" s="3" t="s">
+        <v>148</v>
+      </c>
+      <c r="F20" s="3">
+        <v>0</v>
+      </c>
+      <c r="G20" s="3">
+        <v>0</v>
+      </c>
+      <c r="H20" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="I20">
+        <v>0</v>
+      </c>
+      <c r="J20" s="1" t="s">
+        <v>653</v>
+      </c>
+      <c r="K20" t="s">
+        <v>122</v>
+      </c>
+      <c r="L20" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="M20" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="N20" t="s">
+        <v>122</v>
+      </c>
+      <c r="O20" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15" ht="29" x14ac:dyDescent="0.35">
+      <c r="A21" s="7" t="s">
+        <v>417</v>
+      </c>
+      <c r="B21" s="3">
+        <v>0</v>
+      </c>
+      <c r="C21" s="3">
+        <v>0</v>
+      </c>
+      <c r="D21" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="E21" s="3" t="s">
+        <v>654</v>
+      </c>
+      <c r="F21" s="3">
+        <v>0</v>
+      </c>
+      <c r="G21" s="3">
+        <v>0</v>
+      </c>
+      <c r="H21" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="I21">
+        <v>0</v>
+      </c>
+      <c r="J21" s="1" t="s">
+        <v>655</v>
+      </c>
+      <c r="K21" t="s">
+        <v>122</v>
+      </c>
+      <c r="L21" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="M21" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="N21" t="s">
+        <v>122</v>
+      </c>
+      <c r="O21" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="22" spans="1:15" ht="29" x14ac:dyDescent="0.35">
+      <c r="A22" s="7" t="s">
+        <v>415</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>656</v>
+      </c>
+      <c r="C22" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D22" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="E22" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="F22" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="G22" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="H22" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="I22" t="s">
+        <v>657</v>
+      </c>
+      <c r="J22" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="K22" t="s">
+        <v>122</v>
+      </c>
+      <c r="L22" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="M22" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="N22" t="s">
+        <v>122</v>
+      </c>
+      <c r="O22" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="23" spans="1:15" ht="58" x14ac:dyDescent="0.35">
+      <c r="A23" s="7" t="s">
+        <v>415</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>658</v>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D23" s="3" t="s">
+        <v>659</v>
+      </c>
+      <c r="E23" s="3" t="s">
+        <v>660</v>
+      </c>
+      <c r="F23" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="G23" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="H23" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="I23" t="s">
+        <v>661</v>
+      </c>
+      <c r="J23" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="K23" t="s">
+        <v>122</v>
+      </c>
+      <c r="L23" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="M23" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="N23" t="s">
+        <v>122</v>
+      </c>
+      <c r="O23" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="24" spans="1:15" ht="29" x14ac:dyDescent="0.35">
+      <c r="A24" s="7" t="s">
+        <v>415</v>
+      </c>
+      <c r="B24" s="3" t="s">
+        <v>662</v>
+      </c>
+      <c r="C24" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D24" s="3" t="s">
+        <v>469</v>
+      </c>
+      <c r="E24" s="3" t="s">
+        <v>474</v>
+      </c>
+      <c r="F24" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="G24" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="H24" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="I24" t="s">
+        <v>663</v>
+      </c>
+      <c r="J24" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="K24" t="s">
+        <v>122</v>
+      </c>
+      <c r="L24" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="M24" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="N24" t="s">
+        <v>122</v>
+      </c>
+      <c r="O24" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="25" spans="1:15" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A25" s="7" t="s">
+        <v>415</v>
+      </c>
+      <c r="B25" s="3" t="s">
+        <v>664</v>
+      </c>
+      <c r="C25" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D25" s="3" t="s">
+        <v>665</v>
+      </c>
+      <c r="E25" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="F25" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="G25" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="H25" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="I25" t="s">
+        <v>666</v>
+      </c>
+      <c r="J25" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="K25" t="s">
+        <v>122</v>
+      </c>
+      <c r="L25" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="M25" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="N25" t="s">
+        <v>122</v>
+      </c>
+      <c r="O25" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="26" spans="1:15" ht="58" x14ac:dyDescent="0.35">
+      <c r="A26" s="7" t="s">
+        <v>415</v>
+      </c>
+      <c r="B26" s="3" t="s">
+        <v>667</v>
+      </c>
+      <c r="C26" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D26" s="3" t="s">
+        <v>668</v>
+      </c>
+      <c r="E26" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="F26" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="G26" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="H26" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="I26" t="s">
+        <v>669</v>
+      </c>
+      <c r="J26" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="K26" t="s">
+        <v>122</v>
+      </c>
+      <c r="L26" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="M26" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="N26" t="s">
+        <v>122</v>
+      </c>
+      <c r="O26" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="27" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A27" s="7" t="s">
+        <v>415</v>
+      </c>
+      <c r="B27" s="3" t="s">
+        <v>670</v>
+      </c>
+      <c r="C27" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D27" s="3" t="s">
+        <v>671</v>
+      </c>
+      <c r="E27" s="3" t="s">
+        <v>672</v>
+      </c>
+      <c r="F27" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="G27" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="H27" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="I27" t="s">
+        <v>673</v>
+      </c>
+      <c r="J27" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="K27" t="s">
+        <v>122</v>
+      </c>
+      <c r="L27" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="M27" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="N27" t="s">
+        <v>122</v>
+      </c>
+      <c r="O27" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="28" spans="1:15" ht="29" x14ac:dyDescent="0.35">
+      <c r="A28" s="7" t="s">
+        <v>415</v>
+      </c>
+      <c r="B28" s="3" t="s">
+        <v>674</v>
+      </c>
+      <c r="C28" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D28" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="E28" s="3" t="s">
+        <v>675</v>
+      </c>
+      <c r="F28" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="G28" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="H28" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="I28" t="s">
+        <v>676</v>
+      </c>
+      <c r="J28" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="K28" t="s">
+        <v>122</v>
+      </c>
+      <c r="L28" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="M28" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="N28" t="s">
+        <v>122</v>
+      </c>
+      <c r="O28" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="29" spans="1:15" ht="58" x14ac:dyDescent="0.35">
+      <c r="A29" s="7" t="s">
+        <v>415</v>
+      </c>
+      <c r="B29" s="3" t="s">
+        <v>677</v>
+      </c>
+      <c r="C29" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D29" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="E29" s="3" t="s">
+        <v>678</v>
+      </c>
+      <c r="F29" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="G29" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="H29" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="I29" t="s">
+        <v>679</v>
+      </c>
+      <c r="J29" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="K29" t="s">
+        <v>122</v>
+      </c>
+      <c r="L29" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="M29" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="N29" t="s">
+        <v>122</v>
+      </c>
+      <c r="O29" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="30" spans="1:15" ht="29" x14ac:dyDescent="0.35">
+      <c r="A30" s="7" t="s">
+        <v>416</v>
+      </c>
+      <c r="B30" s="3" t="s">
+        <v>680</v>
+      </c>
+      <c r="C30" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D30" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="E30" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="F30" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="G30" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="H30" s="3" t="s">
+        <v>613</v>
+      </c>
+      <c r="I30" t="s">
+        <v>614</v>
+      </c>
+      <c r="J30" s="1" t="s">
+        <v>612</v>
+      </c>
+      <c r="K30" t="s">
+        <v>122</v>
+      </c>
+      <c r="L30" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="M30" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="N30" t="s">
+        <v>122</v>
+      </c>
+      <c r="O30" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="31" spans="1:15" ht="29" x14ac:dyDescent="0.35">
+      <c r="A31" s="7" t="s">
+        <v>417</v>
+      </c>
+      <c r="B31" s="3">
+        <v>0</v>
+      </c>
+      <c r="C31" s="3">
+        <v>0</v>
+      </c>
+      <c r="D31" s="3" t="s">
+        <v>588</v>
+      </c>
+      <c r="E31" s="3" t="s">
+        <v>589</v>
+      </c>
+      <c r="F31" s="3">
+        <v>0</v>
+      </c>
+      <c r="G31" s="3">
+        <v>0</v>
+      </c>
+      <c r="H31" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="I31">
+        <v>0</v>
+      </c>
+      <c r="J31" s="1" t="s">
+        <v>587</v>
+      </c>
+      <c r="K31" t="s">
+        <v>122</v>
+      </c>
+      <c r="L31" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="M31" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="N31" t="s">
+        <v>122</v>
+      </c>
+      <c r="O31" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="32" spans="1:15" ht="58" x14ac:dyDescent="0.35">
+      <c r="A32" s="7" t="s">
+        <v>416</v>
+      </c>
+      <c r="B32" s="3" t="s">
+        <v>681</v>
+      </c>
+      <c r="C32" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D32" s="3" t="s">
+        <v>588</v>
+      </c>
+      <c r="E32" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="F32" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="G32" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="H32" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="I32" t="s">
+        <v>592</v>
+      </c>
+      <c r="J32" s="1" t="s">
+        <v>591</v>
+      </c>
+      <c r="K32" t="s">
+        <v>122</v>
+      </c>
+      <c r="L32" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="M32" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="N32" t="s">
+        <v>122</v>
+      </c>
+      <c r="O32" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="33" spans="1:15" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A33" s="7" t="s">
+        <v>415</v>
+      </c>
+      <c r="B33" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="C33" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D33" s="3" t="s">
+        <v>594</v>
+      </c>
+      <c r="E33" s="3" t="s">
+        <v>682</v>
+      </c>
+      <c r="F33" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="G33" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="H33" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="I33" t="s">
+        <v>683</v>
+      </c>
+      <c r="J33" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="K33" t="s">
+        <v>122</v>
+      </c>
+      <c r="L33" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="M33" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="N33" t="s">
+        <v>122</v>
+      </c>
+      <c r="O33" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="34" spans="1:15" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A34" s="7" t="s">
+        <v>415</v>
+      </c>
+      <c r="B34" s="3" t="s">
+        <v>684</v>
+      </c>
+      <c r="C34" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="D34" s="3" t="s">
+        <v>594</v>
+      </c>
+      <c r="E34" s="3" t="s">
+        <v>682</v>
+      </c>
+      <c r="F34" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="G34" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="H34" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="I34" t="s">
+        <v>685</v>
+      </c>
+      <c r="J34" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="K34" t="s">
+        <v>122</v>
+      </c>
+      <c r="L34" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="M34" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="N34" t="s">
+        <v>122</v>
+      </c>
+      <c r="O34" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="35" spans="1:15" ht="29" x14ac:dyDescent="0.35">
+      <c r="A35" s="7" t="s">
+        <v>416</v>
+      </c>
+      <c r="B35" s="3" t="s">
+        <v>686</v>
+      </c>
+      <c r="C35" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D35" s="3" t="s">
+        <v>594</v>
+      </c>
+      <c r="E35" s="3" t="s">
+        <v>595</v>
+      </c>
+      <c r="F35" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="G35" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="H35" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="I35" t="s">
+        <v>596</v>
+      </c>
+      <c r="J35" s="1" t="s">
+        <v>593</v>
+      </c>
+      <c r="K35" t="s">
+        <v>122</v>
+      </c>
+      <c r="L35" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="M35" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="N35" t="s">
+        <v>122</v>
+      </c>
+      <c r="O35" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="36" spans="1:15" ht="58" x14ac:dyDescent="0.35">
+      <c r="A36" s="7" t="s">
+        <v>416</v>
+      </c>
+      <c r="B36" s="3" t="s">
+        <v>687</v>
+      </c>
+      <c r="C36" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D36" s="3" t="s">
+        <v>191</v>
+      </c>
+      <c r="E36" s="3" t="s">
+        <v>201</v>
+      </c>
+      <c r="F36" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="G36" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="H36" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="I36" t="s">
+        <v>199</v>
+      </c>
+      <c r="J36" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="K36" t="s">
+        <v>122</v>
+      </c>
+      <c r="L36" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="M36" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="N36" t="s">
+        <v>122</v>
+      </c>
+      <c r="O36" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="37" spans="1:15" ht="58" x14ac:dyDescent="0.35">
+      <c r="A37" s="7" t="s">
+        <v>416</v>
+      </c>
+      <c r="B37" s="3" t="s">
+        <v>688</v>
+      </c>
+      <c r="C37" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D37" s="3" t="s">
+        <v>191</v>
+      </c>
+      <c r="E37" s="3" t="s">
+        <v>204</v>
+      </c>
+      <c r="F37" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="G37" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="H37" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="I37" t="s">
+        <v>202</v>
+      </c>
+      <c r="J37" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="K37" t="s">
+        <v>122</v>
+      </c>
+      <c r="L37" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="M37" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="N37" t="s">
+        <v>122</v>
+      </c>
+      <c r="O37" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="38" spans="1:15" ht="58" x14ac:dyDescent="0.35">
+      <c r="A38" s="7" t="s">
+        <v>416</v>
+      </c>
+      <c r="B38" s="3" t="s">
+        <v>689</v>
+      </c>
+      <c r="C38" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D38" s="3" t="s">
+        <v>191</v>
+      </c>
+      <c r="E38" s="3" t="s">
+        <v>198</v>
+      </c>
+      <c r="F38" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="G38" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="H38" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="I38" t="s">
+        <v>196</v>
+      </c>
+      <c r="J38" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="K38" t="s">
+        <v>122</v>
+      </c>
+      <c r="L38" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="M38" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="N38" t="s">
+        <v>122</v>
+      </c>
+      <c r="O38" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="39" spans="1:15" ht="58" x14ac:dyDescent="0.35">
+      <c r="A39" s="7" t="s">
+        <v>416</v>
+      </c>
+      <c r="B39" s="3" t="s">
+        <v>690</v>
+      </c>
+      <c r="C39" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D39" s="3" t="s">
+        <v>191</v>
+      </c>
+      <c r="E39" s="3" t="s">
+        <v>192</v>
+      </c>
+      <c r="F39" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="G39" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="H39" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="I39" t="s">
+        <v>189</v>
+      </c>
+      <c r="J39" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="K39" t="s">
+        <v>122</v>
+      </c>
+      <c r="L39" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="M39" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="N39" t="s">
+        <v>122</v>
+      </c>
+      <c r="O39" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="40" spans="1:15" ht="58" x14ac:dyDescent="0.35">
+      <c r="A40" s="7" t="s">
+        <v>416</v>
+      </c>
+      <c r="B40" s="3" t="s">
+        <v>691</v>
+      </c>
+      <c r="C40" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D40" s="3" t="s">
+        <v>191</v>
+      </c>
+      <c r="E40" s="3" t="s">
+        <v>195</v>
+      </c>
+      <c r="F40" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="G40" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="H40" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="I40" t="s">
+        <v>193</v>
+      </c>
+      <c r="J40" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="K40" t="s">
+        <v>122</v>
+      </c>
+      <c r="L40" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="M40" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="N40" t="s">
+        <v>122</v>
+      </c>
+      <c r="O40" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="41" spans="1:15" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A41" s="7" t="s">
+        <v>416</v>
+      </c>
+      <c r="B41" s="3" t="s">
+        <v>479</v>
+      </c>
+      <c r="C41" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D41" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E41" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="F41" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="G41" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="H41" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="I41" t="s">
+        <v>480</v>
+      </c>
+      <c r="J41" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="K41" t="s">
+        <v>122</v>
+      </c>
+      <c r="L41" s="1" t="s">
+        <v>692</v>
+      </c>
+      <c r="M41" s="1" t="s">
+        <v>693</v>
+      </c>
+      <c r="N41" t="s">
+        <v>122</v>
+      </c>
+      <c r="O41" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="42" spans="1:15" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A42" s="7" t="s">
+        <v>416</v>
+      </c>
+      <c r="B42" s="3" t="s">
+        <v>477</v>
+      </c>
+      <c r="C42" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D42" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E42" s="3" t="s">
+        <v>694</v>
+      </c>
+      <c r="F42" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="G42" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="H42" s="3" t="s">
+        <v>695</v>
+      </c>
+      <c r="I42" t="s">
+        <v>478</v>
+      </c>
+      <c r="J42" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="K42" t="s">
+        <v>122</v>
+      </c>
+      <c r="L42" s="1" t="s">
+        <v>692</v>
+      </c>
+      <c r="M42" s="1" t="s">
+        <v>696</v>
+      </c>
+      <c r="N42" t="s">
+        <v>122</v>
+      </c>
+      <c r="O42" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="43" spans="1:15" ht="29" x14ac:dyDescent="0.35">
+      <c r="A43" s="7" t="s">
+        <v>415</v>
+      </c>
+      <c r="B43" s="3" t="s">
+        <v>697</v>
+      </c>
+      <c r="C43" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D43" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E43" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="F43" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="G43" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="H43" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="I43" t="s">
+        <v>698</v>
+      </c>
+      <c r="J43" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="K43" t="s">
+        <v>122</v>
+      </c>
+      <c r="L43" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="M43" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="N43" t="s">
+        <v>122</v>
+      </c>
+      <c r="O43" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="44" spans="1:15" ht="29" x14ac:dyDescent="0.35">
+      <c r="A44" s="7" t="s">
+        <v>415</v>
+      </c>
+      <c r="B44" s="3" t="s">
+        <v>699</v>
+      </c>
+      <c r="C44" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D44" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E44" s="3" t="s">
+        <v>700</v>
+      </c>
+      <c r="F44" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="G44" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="H44" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="I44" t="s">
+        <v>701</v>
+      </c>
+      <c r="J44" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="K44" t="s">
+        <v>122</v>
+      </c>
+      <c r="L44" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="M44" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="N44" t="s">
+        <v>122</v>
+      </c>
+      <c r="O44" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="45" spans="1:15" ht="29" x14ac:dyDescent="0.35">
+      <c r="A45" s="7" t="s">
+        <v>415</v>
+      </c>
+      <c r="B45" s="3" t="s">
+        <v>702</v>
+      </c>
+      <c r="C45" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="D45" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E45" s="3" t="s">
+        <v>700</v>
+      </c>
+      <c r="F45" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="G45" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="H45" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="I45" t="s">
+        <v>703</v>
+      </c>
+      <c r="J45" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="K45" t="s">
+        <v>122</v>
+      </c>
+      <c r="L45" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="M45" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="N45" t="s">
+        <v>122</v>
+      </c>
+      <c r="O45" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="46" spans="1:15" ht="29" x14ac:dyDescent="0.35">
+      <c r="A46" s="7" t="s">
+        <v>415</v>
+      </c>
+      <c r="B46" s="3" t="s">
+        <v>704</v>
+      </c>
+      <c r="C46" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D46" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E46" s="3" t="s">
+        <v>705</v>
+      </c>
+      <c r="F46" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="G46" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="H46" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="I46" t="s">
+        <v>706</v>
+      </c>
+      <c r="J46" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="K46" t="s">
+        <v>122</v>
+      </c>
+      <c r="L46" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="M46" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="N46" t="s">
+        <v>122</v>
+      </c>
+      <c r="O46" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="47" spans="1:15" ht="29" x14ac:dyDescent="0.35">
+      <c r="A47" s="7" t="s">
+        <v>416</v>
+      </c>
+      <c r="B47" s="3" t="s">
+        <v>699</v>
+      </c>
+      <c r="C47" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D47" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E47" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="F47" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="G47" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="H47" s="3" t="s">
+        <v>523</v>
+      </c>
+      <c r="I47" t="s">
+        <v>16</v>
+      </c>
+      <c r="J47" s="1" t="s">
+        <v>522</v>
+      </c>
+      <c r="K47" t="s">
+        <v>122</v>
+      </c>
+      <c r="L47" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="M47" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="N47" t="s">
+        <v>122</v>
+      </c>
+      <c r="O47" t="s">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="48" spans="1:15" ht="29" x14ac:dyDescent="0.35">
+      <c r="A48" s="7" t="s">
+        <v>417</v>
+      </c>
+      <c r="B48" s="3">
+        <v>0</v>
+      </c>
+      <c r="C48" s="3">
+        <v>0</v>
+      </c>
+      <c r="D48" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E48" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="F48" s="3">
+        <v>0</v>
+      </c>
+      <c r="G48" s="3">
+        <v>0</v>
+      </c>
+      <c r="H48" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="I48">
+        <v>0</v>
+      </c>
+      <c r="J48" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="K48" t="s">
+        <v>122</v>
+      </c>
+      <c r="L48" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="M48" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="N48" t="s">
+        <v>122</v>
+      </c>
+      <c r="O48" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="49" spans="1:15" ht="29" x14ac:dyDescent="0.35">
+      <c r="A49" s="7" t="s">
+        <v>415</v>
+      </c>
+      <c r="B49" s="3" t="s">
+        <v>702</v>
+      </c>
+      <c r="C49" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="D49" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E49" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="F49" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="G49" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="H49" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="I49" t="s">
+        <v>707</v>
+      </c>
+      <c r="J49" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="K49" t="s">
+        <v>122</v>
+      </c>
+      <c r="L49" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="M49" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="N49" t="s">
+        <v>122</v>
+      </c>
+      <c r="O49" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="50" spans="1:15" ht="58" x14ac:dyDescent="0.35">
+      <c r="A50" s="7" t="s">
+        <v>415</v>
+      </c>
+      <c r="B50" s="3" t="s">
+        <v>704</v>
+      </c>
+      <c r="C50" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D50" s="3" t="s">
+        <v>708</v>
+      </c>
+      <c r="E50" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="F50" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="G50" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="H50" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="I50" t="s">
+        <v>709</v>
+      </c>
+      <c r="J50" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="K50" t="s">
+        <v>122</v>
+      </c>
+      <c r="L50" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="M50" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="N50" t="s">
+        <v>122</v>
+      </c>
+      <c r="O50" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="51" spans="1:15" ht="29" x14ac:dyDescent="0.35">
+      <c r="A51" s="7" t="s">
+        <v>416</v>
+      </c>
+      <c r="B51" s="3" t="s">
+        <v>710</v>
+      </c>
+      <c r="C51" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D51" s="3" t="s">
+        <v>172</v>
+      </c>
+      <c r="E51" s="3" t="s">
+        <v>249</v>
+      </c>
+      <c r="F51" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="G51" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="H51" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="I51" t="s">
+        <v>247</v>
+      </c>
+      <c r="J51" s="1" t="s">
+        <v>248</v>
+      </c>
+      <c r="K51" t="s">
+        <v>122</v>
+      </c>
+      <c r="L51" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="M51" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="N51" t="s">
+        <v>122</v>
+      </c>
+      <c r="O51" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="52" spans="1:15" ht="29" x14ac:dyDescent="0.35">
+      <c r="A52" s="7" t="s">
+        <v>416</v>
+      </c>
+      <c r="B52" s="3" t="s">
+        <v>711</v>
+      </c>
+      <c r="C52" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D52" s="3" t="s">
+        <v>172</v>
+      </c>
+      <c r="E52" s="3" t="s">
+        <v>173</v>
+      </c>
+      <c r="F52" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="G52" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="H52" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="I52" t="s">
+        <v>170</v>
+      </c>
+      <c r="J52" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="K52" t="s">
+        <v>122</v>
+      </c>
+      <c r="L52" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="M52" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="N52" t="s">
+        <v>122</v>
+      </c>
+      <c r="O52" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="53" spans="1:15" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A53" s="7" t="s">
+        <v>416</v>
+      </c>
+      <c r="B53" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="C53" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D53" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="E53" s="3" t="s">
+        <v>682</v>
+      </c>
+      <c r="F53" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="G53" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="H53" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="I53" t="s">
+        <v>123</v>
+      </c>
+      <c r="J53" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="K53" t="s">
+        <v>122</v>
+      </c>
+      <c r="L53" s="1" t="s">
+        <v>712</v>
+      </c>
+      <c r="M53" s="1" t="s">
+        <v>713</v>
+      </c>
+      <c r="N53" t="s">
+        <v>122</v>
+      </c>
+      <c r="O53" t="s">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="54" spans="1:15" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A54" s="7" t="s">
+        <v>416</v>
+      </c>
+      <c r="B54" s="3" t="s">
+        <v>684</v>
+      </c>
+      <c r="C54" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="D54" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="E54" s="3" t="s">
+        <v>682</v>
+      </c>
+      <c r="F54" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="G54" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="H54" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="I54" t="s">
+        <v>131</v>
+      </c>
+      <c r="J54" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="K54" t="s">
+        <v>438</v>
+      </c>
+      <c r="L54" s="1" t="s">
+        <v>712</v>
+      </c>
+      <c r="M54" s="1" t="s">
+        <v>713</v>
+      </c>
+      <c r="N54" t="s">
+        <v>122</v>
+      </c>
+      <c r="O54" t="s">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="55" spans="1:15" ht="29" x14ac:dyDescent="0.35">
+      <c r="A55" s="7" t="s">
+        <v>415</v>
+      </c>
+      <c r="B55" s="3" t="s">
+        <v>714</v>
+      </c>
+      <c r="C55" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D55" s="3" t="s">
+        <v>528</v>
+      </c>
+      <c r="E55" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="F55" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="G55" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="H55" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="I55" t="s">
+        <v>715</v>
+      </c>
+      <c r="J55" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="K55" t="s">
+        <v>122</v>
+      </c>
+      <c r="L55" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="M55" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="N55" t="s">
+        <v>122</v>
+      </c>
+      <c r="O55" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="56" spans="1:15" ht="29" x14ac:dyDescent="0.35">
+      <c r="A56" s="7" t="s">
+        <v>416</v>
+      </c>
+      <c r="B56" s="3" t="s">
+        <v>128</v>
+      </c>
+      <c r="C56" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D56" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E56" s="3" t="s">
+        <v>682</v>
+      </c>
+      <c r="F56" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="G56" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="H56" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="I56" t="s">
+        <v>127</v>
+      </c>
+      <c r="J56" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="K56" t="s">
+        <v>122</v>
+      </c>
+      <c r="L56" s="1" t="s">
+        <v>716</v>
+      </c>
+      <c r="M56" s="1" t="s">
+        <v>713</v>
+      </c>
+      <c r="N56" t="s">
+        <v>122</v>
+      </c>
+      <c r="O56" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="57" spans="1:15" ht="29" x14ac:dyDescent="0.35">
+      <c r="A57" s="7" t="s">
+        <v>416</v>
+      </c>
+      <c r="B57" s="3" t="s">
+        <v>717</v>
+      </c>
+      <c r="C57" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="D57" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E57" s="3" t="s">
+        <v>682</v>
+      </c>
+      <c r="F57" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="G57" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="H57" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="I57" t="s">
+        <v>129</v>
+      </c>
+      <c r="J57" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="K57" t="s">
+        <v>438</v>
+      </c>
+      <c r="L57" s="1" t="s">
+        <v>716</v>
+      </c>
+      <c r="M57" s="1" t="s">
+        <v>713</v>
+      </c>
+      <c r="N57" t="s">
+        <v>122</v>
+      </c>
+      <c r="O57" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="58" spans="1:15" ht="58" x14ac:dyDescent="0.35">
+      <c r="A58" s="7" t="s">
+        <v>416</v>
+      </c>
+      <c r="B58" s="3" t="s">
+        <v>718</v>
+      </c>
+      <c r="C58" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D58" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E58" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="F58" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="G58" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="H58" s="3" t="s">
+        <v>535</v>
+      </c>
+      <c r="I58" t="s">
+        <v>48</v>
+      </c>
+      <c r="J58" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="K58" t="s">
+        <v>122</v>
+      </c>
+      <c r="L58" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="M58" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="N58" t="s">
+        <v>122</v>
+      </c>
+      <c r="O58" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="59" spans="1:15" ht="29" x14ac:dyDescent="0.35">
+      <c r="A59" s="7" t="s">
+        <v>416</v>
+      </c>
+      <c r="B59" s="3" t="s">
+        <v>527</v>
+      </c>
+      <c r="C59" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D59" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E59" s="3" t="s">
+        <v>719</v>
+      </c>
+      <c r="F59" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="G59" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="H59" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="I59" t="s">
+        <v>529</v>
+      </c>
+      <c r="J59" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="K59" t="s">
+        <v>122</v>
+      </c>
+      <c r="L59" s="1" t="s">
+        <v>720</v>
+      </c>
+      <c r="M59" s="1" t="s">
+        <v>721</v>
+      </c>
+      <c r="N59" t="s">
+        <v>122</v>
+      </c>
+      <c r="O59" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="60" spans="1:15" ht="29" x14ac:dyDescent="0.35">
+      <c r="A60" s="7" t="s">
+        <v>416</v>
+      </c>
+      <c r="B60" s="3" t="s">
+        <v>722</v>
+      </c>
+      <c r="C60" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D60" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E60" s="3" t="s">
+        <v>719</v>
+      </c>
+      <c r="F60" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="G60" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="H60" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="I60" t="s">
+        <v>531</v>
+      </c>
+      <c r="J60" s="1" t="s">
+        <v>530</v>
+      </c>
+      <c r="K60" t="s">
+        <v>122</v>
+      </c>
+      <c r="L60" s="1" t="s">
+        <v>720</v>
+      </c>
+      <c r="M60" s="1" t="s">
+        <v>721</v>
+      </c>
+      <c r="N60" t="s">
+        <v>122</v>
+      </c>
+      <c r="O60" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="61" spans="1:15" ht="29" x14ac:dyDescent="0.35">
+      <c r="A61" s="7" t="s">
+        <v>416</v>
+      </c>
+      <c r="B61" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="C61" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D61" s="3" t="s">
+        <v>723</v>
+      </c>
+      <c r="E61" s="3" t="s">
+        <v>244</v>
+      </c>
+      <c r="F61" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="G61" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="H61" s="3" t="s">
+        <v>466</v>
+      </c>
+      <c r="I61" t="s">
+        <v>36</v>
+      </c>
+      <c r="J61" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="K61" t="s">
+        <v>122</v>
+      </c>
+      <c r="L61" s="1" t="s">
+        <v>724</v>
+      </c>
+      <c r="M61" s="1" t="s">
+        <v>725</v>
+      </c>
+      <c r="N61" t="s">
+        <v>122</v>
+      </c>
+      <c r="O61" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="62" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A62" s="7" t="s">
+        <v>415</v>
+      </c>
+      <c r="B62" s="3" t="s">
+        <v>726</v>
+      </c>
+      <c r="C62" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D62" s="3" t="s">
+        <v>727</v>
+      </c>
+      <c r="E62" s="3" t="s">
+        <v>728</v>
+      </c>
+      <c r="F62" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="G62" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="H62" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="I62" t="s">
+        <v>729</v>
+      </c>
+      <c r="J62" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="K62" t="s">
+        <v>122</v>
+      </c>
+      <c r="L62" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="M62" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="N62" t="s">
+        <v>122</v>
+      </c>
+      <c r="O62" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="63" spans="1:15" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A63" s="7" t="s">
+        <v>416</v>
+      </c>
+      <c r="B63" s="3" t="s">
+        <v>730</v>
+      </c>
+      <c r="C63" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D63" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E63" s="3" t="s">
+        <v>537</v>
+      </c>
+      <c r="F63" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="G63" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="H63" s="3" t="s">
+        <v>731</v>
+      </c>
+      <c r="I63" t="s">
+        <v>538</v>
+      </c>
+      <c r="J63" s="1" t="s">
+        <v>536</v>
+      </c>
+      <c r="K63" t="s">
+        <v>122</v>
+      </c>
+      <c r="L63" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="M63" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="N63" t="s">
+        <v>122</v>
+      </c>
+      <c r="O63" t="s">
+        <v>122</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B456D714-2DB6-4B8B-BC8E-8AA7501F8C79}">
   <dimension ref="A1:O7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J7" sqref="J7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2675,7 +6010,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E53E83C4-68F7-4929-AA83-3F95502173FC}">
   <dimension ref="A1:O195"/>
   <sheetViews>
@@ -4530,7 +7865,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2720FBDC-F538-4F79-9784-827E5ACB3995}">
   <dimension ref="A1:P130"/>
   <sheetViews>

</xml_diff>

<commit_message>
Updated Core rules for amendments #477
</commit_message>
<xml_diff>
--- a/Deliverables/RULES/USDM_CORE_Rules_Changes.xlsx
+++ b/Deliverables/RULES/USDM_CORE_Rules_Changes.xlsx
@@ -5,21 +5,22 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Stack\CL027\Publish\CORE\3.6\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Stack\CL027\Publish\CORE\3.7\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EBCD13D9-6351-442E-A698-9FB1AC7509D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F7B1989-BEAA-49E8-90AB-B631DE2F9D57}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-7620" windowWidth="29040" windowHeight="15720" xr2:uid="{418CF395-400B-43AB-9594-6DFC1F089218}"/>
+    <workbookView xWindow="21015" yWindow="-20925" windowWidth="16035" windowHeight="8625" xr2:uid="{418CF395-400B-43AB-9594-6DFC1F089218}"/>
   </bookViews>
   <sheets>
-    <sheet name="Changes release 3.5-&gt;3.6" sheetId="8" r:id="rId1"/>
-    <sheet name="Changes release 3.4-&gt;3.5" sheetId="7" r:id="rId2"/>
-    <sheet name="Changes release 3.3-&gt;3.4" sheetId="5" r:id="rId3"/>
-    <sheet name="Changes release 3.1-&gt;3.3" sheetId="6" r:id="rId4"/>
+    <sheet name="Changes release 3.6 -&gt; 3.7" sheetId="9" r:id="rId1"/>
+    <sheet name="Changes release 3.5-&gt;3.6" sheetId="8" r:id="rId2"/>
+    <sheet name="Changes release 3.4-&gt;3.5" sheetId="7" r:id="rId3"/>
+    <sheet name="Changes release 3.3-&gt;3.4" sheetId="5" r:id="rId4"/>
+    <sheet name="Changes release 3.1-&gt;3.3" sheetId="6" r:id="rId5"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'Changes release 3.3-&gt;3.4'!$A$1:$O$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'Changes release 3.3-&gt;3.4'!$A$1:$O$1</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -42,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3953" uniqueCount="819">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4058" uniqueCount="833">
   <si>
     <t>All</t>
   </si>
@@ -2499,6 +2500,48 @@
   </si>
   <si>
     <t>CHK0237</t>
+  </si>
+  <si>
+    <t>DDF00045</t>
+  </si>
+  <si>
+    <t>CHK0238</t>
+  </si>
+  <si>
+    <t>CHK0239</t>
+  </si>
+  <si>
+    <t>Each study enrollment must apply to either a geographic scope, a study site, or a study cohort.</t>
+  </si>
+  <si>
+    <t>CHK0240</t>
+  </si>
+  <si>
+    <t>There must be a one-to-one relationship between referenced section number and title within a study amendment.</t>
+  </si>
+  <si>
+    <t>DocumentContentReference</t>
+  </si>
+  <si>
+    <t>sectionNumber, sectionTitle</t>
+  </si>
+  <si>
+    <t>CHK0241</t>
+  </si>
+  <si>
+    <t>A study version is expected to be documented by only one version of a study definition document.</t>
+  </si>
+  <si>
+    <t>CHK0242</t>
+  </si>
+  <si>
+    <t>Each study definition document version is expected to be referenced by either a study version or a study design.</t>
+  </si>
+  <si>
+    <t>StudyVersion, StudyDesign</t>
+  </si>
+  <si>
+    <t>documentVersions, documentVersion</t>
   </si>
 </sst>
 </file>
@@ -2576,7 +2619,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -2602,6 +2645,7 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2935,11 +2979,365 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{067B8281-AB10-416A-8A55-B2F46EB8E8FB}">
+  <dimension ref="A1:O7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="8.453125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="97.90625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.26953125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="24.6328125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="33.36328125" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="10.36328125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.81640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="20.7265625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:15" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>600</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>546</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>547</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>548</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>549</v>
+      </c>
+      <c r="F1" s="8" t="s">
+        <v>550</v>
+      </c>
+      <c r="G1" s="8" t="s">
+        <v>551</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>552</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>775</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>615</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>395</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>545</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>396</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>776</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>777</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A2" s="7" t="s">
+        <v>416</v>
+      </c>
+      <c r="B2" s="11" t="s">
+        <v>114</v>
+      </c>
+      <c r="C2" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="11" t="s">
+        <v>115</v>
+      </c>
+      <c r="E2" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="F2" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="G2" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="H2" s="11" t="s">
+        <v>819</v>
+      </c>
+      <c r="I2" t="s">
+        <v>113</v>
+      </c>
+      <c r="J2" t="s">
+        <v>122</v>
+      </c>
+      <c r="K2" t="s">
+        <v>122</v>
+      </c>
+      <c r="L2" t="s">
+        <v>122</v>
+      </c>
+      <c r="M2" t="s">
+        <v>122</v>
+      </c>
+      <c r="N2" t="s">
+        <v>122</v>
+      </c>
+      <c r="O2" t="s">
+        <v>778</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A3" s="7" t="s">
+        <v>415</v>
+      </c>
+      <c r="B3" s="11" t="s">
+        <v>114</v>
+      </c>
+      <c r="C3" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="D3" s="11" t="s">
+        <v>115</v>
+      </c>
+      <c r="E3" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="F3" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="G3" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="H3" s="11" t="s">
+        <v>122</v>
+      </c>
+      <c r="I3" t="s">
+        <v>820</v>
+      </c>
+      <c r="J3" t="s">
+        <v>122</v>
+      </c>
+      <c r="K3" t="s">
+        <v>122</v>
+      </c>
+      <c r="L3" t="s">
+        <v>122</v>
+      </c>
+      <c r="M3" t="s">
+        <v>122</v>
+      </c>
+      <c r="N3" t="s">
+        <v>122</v>
+      </c>
+      <c r="O3" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A4" s="7" t="s">
+        <v>415</v>
+      </c>
+      <c r="B4" s="11" t="s">
+        <v>822</v>
+      </c>
+      <c r="C4" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="D4" s="11" t="s">
+        <v>715</v>
+      </c>
+      <c r="E4" s="11" t="s">
+        <v>54</v>
+      </c>
+      <c r="F4" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="G4" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="H4" s="11" t="s">
+        <v>122</v>
+      </c>
+      <c r="I4" t="s">
+        <v>821</v>
+      </c>
+      <c r="J4" t="s">
+        <v>122</v>
+      </c>
+      <c r="K4" t="s">
+        <v>122</v>
+      </c>
+      <c r="L4" t="s">
+        <v>122</v>
+      </c>
+      <c r="M4" t="s">
+        <v>122</v>
+      </c>
+      <c r="N4" t="s">
+        <v>122</v>
+      </c>
+      <c r="O4" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A5" s="7" t="s">
+        <v>415</v>
+      </c>
+      <c r="B5" s="11" t="s">
+        <v>824</v>
+      </c>
+      <c r="C5" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="D5" s="11" t="s">
+        <v>825</v>
+      </c>
+      <c r="E5" s="11" t="s">
+        <v>826</v>
+      </c>
+      <c r="F5" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="G5" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="H5" s="11" t="s">
+        <v>122</v>
+      </c>
+      <c r="I5" t="s">
+        <v>823</v>
+      </c>
+      <c r="J5" t="s">
+        <v>122</v>
+      </c>
+      <c r="K5" t="s">
+        <v>122</v>
+      </c>
+      <c r="L5" t="s">
+        <v>122</v>
+      </c>
+      <c r="M5" t="s">
+        <v>122</v>
+      </c>
+      <c r="N5" t="s">
+        <v>122</v>
+      </c>
+      <c r="O5" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A6" s="7" t="s">
+        <v>415</v>
+      </c>
+      <c r="B6" s="11" t="s">
+        <v>828</v>
+      </c>
+      <c r="C6" s="11" t="s">
+        <v>95</v>
+      </c>
+      <c r="D6" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="E6" s="11" t="s">
+        <v>598</v>
+      </c>
+      <c r="F6" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="G6" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="H6" s="11" t="s">
+        <v>122</v>
+      </c>
+      <c r="I6" t="s">
+        <v>827</v>
+      </c>
+      <c r="J6" t="s">
+        <v>122</v>
+      </c>
+      <c r="K6" t="s">
+        <v>122</v>
+      </c>
+      <c r="L6" t="s">
+        <v>122</v>
+      </c>
+      <c r="M6" t="s">
+        <v>122</v>
+      </c>
+      <c r="N6" t="s">
+        <v>122</v>
+      </c>
+      <c r="O6" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A7" s="7" t="s">
+        <v>415</v>
+      </c>
+      <c r="B7" s="11" t="s">
+        <v>830</v>
+      </c>
+      <c r="C7" s="11" t="s">
+        <v>95</v>
+      </c>
+      <c r="D7" s="11" t="s">
+        <v>831</v>
+      </c>
+      <c r="E7" s="11" t="s">
+        <v>832</v>
+      </c>
+      <c r="F7" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="G7" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="H7" s="11" t="s">
+        <v>122</v>
+      </c>
+      <c r="I7" t="s">
+        <v>829</v>
+      </c>
+      <c r="J7" t="s">
+        <v>122</v>
+      </c>
+      <c r="K7" t="s">
+        <v>122</v>
+      </c>
+      <c r="L7" t="s">
+        <v>122</v>
+      </c>
+      <c r="M7" t="s">
+        <v>122</v>
+      </c>
+      <c r="N7" t="s">
+        <v>122</v>
+      </c>
+      <c r="O7" t="s">
+        <v>122</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A424D0F2-3B88-4770-93C0-98D49DE8D516}">
   <dimension ref="A1:O104"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4600,7 +4998,7 @@
         <v>783</v>
       </c>
     </row>
-    <row r="36" spans="1:15" ht="29" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A36" s="7" t="s">
         <v>415</v>
       </c>
@@ -4647,7 +5045,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="37" spans="1:15" ht="29" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A37" s="7" t="s">
         <v>415</v>
       </c>
@@ -5117,7 +5515,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="47" spans="1:15" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:15" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A47" s="7" t="s">
         <v>416</v>
       </c>
@@ -6151,7 +6549,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="69" spans="1:15" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:15" ht="29" x14ac:dyDescent="0.35">
       <c r="A69" s="7" t="s">
         <v>416</v>
       </c>
@@ -7232,7 +7630,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="92" spans="1:15" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:15" ht="29" x14ac:dyDescent="0.35">
       <c r="A92" s="7" t="s">
         <v>416</v>
       </c>
@@ -7279,7 +7677,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="93" spans="1:15" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:15" ht="29" x14ac:dyDescent="0.35">
       <c r="A93" s="7" t="s">
         <v>416</v>
       </c>
@@ -7373,7 +7771,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="95" spans="1:15" ht="29" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A95" s="7" t="s">
         <v>416</v>
       </c>
@@ -7420,7 +7818,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="96" spans="1:15" ht="29" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A96" s="7" t="s">
         <v>416</v>
       </c>
@@ -7853,7 +8251,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B456D714-2DB6-4B8B-BC8E-8AA7501F8C79}">
   <dimension ref="A1:O7"/>
   <sheetViews>
@@ -8204,7 +8602,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E53E83C4-68F7-4929-AA83-3F95502173FC}">
   <dimension ref="A1:O195"/>
   <sheetViews>
@@ -10059,7 +10457,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2720FBDC-F538-4F79-9784-827E5ACB3995}">
   <dimension ref="A1:P130"/>
   <sheetViews>

</xml_diff>

<commit_message>
Updated rules according to #504, #507 and public review CORE v3 tickets
</commit_message>
<xml_diff>
--- a/Deliverables/RULES/USDM_CORE_Rules_Changes.xlsx
+++ b/Deliverables/RULES/USDM_CORE_Rules_Changes.xlsx
@@ -1,26 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Stack\CL027\Publish\CORE\3.7\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Stack\CL027\Publish\CORE\3.8\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F7B1989-BEAA-49E8-90AB-B631DE2F9D57}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41A0C30B-BC8E-4D50-A193-A14D409AD687}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="21015" yWindow="-20925" windowWidth="16035" windowHeight="8625" xr2:uid="{418CF395-400B-43AB-9594-6DFC1F089218}"/>
+    <workbookView xWindow="-2220" yWindow="-19020" windowWidth="22350" windowHeight="15165" xr2:uid="{418CF395-400B-43AB-9594-6DFC1F089218}"/>
   </bookViews>
   <sheets>
-    <sheet name="Changes release 3.6 -&gt; 3.7" sheetId="9" r:id="rId1"/>
-    <sheet name="Changes release 3.5-&gt;3.6" sheetId="8" r:id="rId2"/>
-    <sheet name="Changes release 3.4-&gt;3.5" sheetId="7" r:id="rId3"/>
-    <sheet name="Changes release 3.3-&gt;3.4" sheetId="5" r:id="rId4"/>
-    <sheet name="Changes release 3.1-&gt;3.3" sheetId="6" r:id="rId5"/>
+    <sheet name="Changes release 3.7 -&gt; 3.8" sheetId="10" r:id="rId1"/>
+    <sheet name="Changes release 3.6 -&gt; 3.7" sheetId="9" r:id="rId2"/>
+    <sheet name="Changes release 3.5-&gt;3.6" sheetId="8" r:id="rId3"/>
+    <sheet name="Changes release 3.4-&gt;3.5" sheetId="7" r:id="rId4"/>
+    <sheet name="Changes release 3.3-&gt;3.4" sheetId="5" r:id="rId5"/>
+    <sheet name="Changes release 3.1-&gt;3.3" sheetId="6" r:id="rId6"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'Changes release 3.3-&gt;3.4'!$A$1:$O$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">'Changes release 3.3-&gt;3.4'!$A$1:$O$1</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -43,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4058" uniqueCount="833">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4276" uniqueCount="859">
   <si>
     <t>All</t>
   </si>
@@ -2542,6 +2543,84 @@
   </si>
   <si>
     <t>documentVersions, documentVersion</t>
+  </si>
+  <si>
+    <t>If timing type is not "Fixed Reference" then it must point to two scheduled instances (e.g. the relativeFromScheduledInstance and relativeToScheduledInstance attributes must not be missing and must not be equal to each other).</t>
+  </si>
+  <si>
+    <t>A standard code alias is not expected to be equal to the standard code (e.g. no equal code for the same coding system version is expected).</t>
+  </si>
+  <si>
+    <t>DDF00063</t>
+  </si>
+  <si>
+    <t>Anchor timings (e.g. type is "Fixed Reference") must be related to a scheduled activity instance.</t>
+  </si>
+  <si>
+    <t>relativeFromScheduledInstance</t>
+  </si>
+  <si>
+    <t>relativeToScheduledInstance=&gt;relativeFromScheduledInstance</t>
+  </si>
+  <si>
+    <t>There must be exactly one sponsor study identifier (i.e., a study identifier whose scope is an organization that is identified as the organization for the sponsor study role).</t>
+  </si>
+  <si>
+    <t>A study definition document version must not be referenced more than once by the same study design.</t>
+  </si>
+  <si>
+    <t>StudyVersion=&gt;StudyDesign</t>
+  </si>
+  <si>
+    <t>documentVersions, documentVersion=&gt;documentVersions</t>
+  </si>
+  <si>
+    <t>An study impact type must be specified according to the extensible study amendment impact type (Cxxxx) DDF codelist (e.g. an entry with a code or decode used from the codelist should be consistent with the full entry in the codelist).</t>
+  </si>
+  <si>
+    <t>StudyAmendmentImpact</t>
+  </si>
+  <si>
+    <t>CHK0243</t>
+  </si>
+  <si>
+    <t>Organization</t>
+  </si>
+  <si>
+    <t>CHK0244</t>
+  </si>
+  <si>
+    <t xml:space="preserve">There must be exactly one study role with a code of sponsor. </t>
+  </si>
+  <si>
+    <t>CHK0245</t>
+  </si>
+  <si>
+    <t>The sponsor study role must point to exactly one organization.</t>
+  </si>
+  <si>
+    <t>organizations</t>
+  </si>
+  <si>
+    <t>CHK0246</t>
+  </si>
+  <si>
+    <t>The sponsor study role must be applicable to a study version.</t>
+  </si>
+  <si>
+    <t>CHK0247</t>
+  </si>
+  <si>
+    <t>CORE v3.0 Public Review change</t>
+  </si>
+  <si>
+    <t>Warning/ Error change</t>
+  </si>
+  <si>
+    <t>Version 4.0 (Version 3.8)</t>
+  </si>
+  <si>
+    <t>V4 (V3.8) change</t>
   </si>
 </sst>
 </file>
@@ -2650,7 +2729,15 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="1">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -2979,11 +3066,695 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8EF31D4B-F1B8-4E5E-A34A-AF6E16EC4595}">
+  <dimension ref="A1:P13"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N2" sqref="N2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="8.453125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.7265625" customWidth="1"/>
+    <col min="3" max="3" width="63.6328125" customWidth="1"/>
+    <col min="4" max="4" width="9.26953125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="32.26953125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="27.90625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.36328125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.7265625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="50.7265625" style="1" customWidth="1"/>
+    <col min="12" max="12" width="11.36328125" customWidth="1"/>
+    <col min="13" max="13" width="24.54296875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="54.90625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:16" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="A1" s="8" t="s">
+        <v>600</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>855</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>546</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>547</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>548</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>549</v>
+      </c>
+      <c r="G1" s="8" t="s">
+        <v>550</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>857</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>552</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>775</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>615</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>856</v>
+      </c>
+      <c r="M1" s="5" t="s">
+        <v>545</v>
+      </c>
+      <c r="N1" s="5" t="s">
+        <v>396</v>
+      </c>
+      <c r="O1" s="5" t="s">
+        <v>776</v>
+      </c>
+      <c r="P1" s="5" t="s">
+        <v>858</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="A2" s="7" t="s">
+        <v>416</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>833</v>
+      </c>
+      <c r="D2" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="F2" s="11" t="s">
+        <v>69</v>
+      </c>
+      <c r="G2" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="H2" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="I2" s="11" t="s">
+        <v>542</v>
+      </c>
+      <c r="J2" t="s">
+        <v>70</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="L2" t="s">
+        <v>122</v>
+      </c>
+      <c r="M2" t="s">
+        <v>122</v>
+      </c>
+      <c r="N2" t="s">
+        <v>122</v>
+      </c>
+      <c r="O2" t="s">
+        <v>122</v>
+      </c>
+      <c r="P2" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" ht="58" x14ac:dyDescent="0.35">
+      <c r="A3" s="7" t="s">
+        <v>416</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>834</v>
+      </c>
+      <c r="D3" s="11" t="s">
+        <v>95</v>
+      </c>
+      <c r="E3" s="11" t="s">
+        <v>118</v>
+      </c>
+      <c r="F3" s="11" t="s">
+        <v>119</v>
+      </c>
+      <c r="G3" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="H3" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="I3" s="11" t="s">
+        <v>835</v>
+      </c>
+      <c r="J3" t="s">
+        <v>255</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>437</v>
+      </c>
+      <c r="L3" t="s">
+        <v>122</v>
+      </c>
+      <c r="M3" t="s">
+        <v>122</v>
+      </c>
+      <c r="N3" t="s">
+        <v>122</v>
+      </c>
+      <c r="O3" t="s">
+        <v>122</v>
+      </c>
+      <c r="P3" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A4" s="7" t="s">
+        <v>416</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>836</v>
+      </c>
+      <c r="D4" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="E4" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="F4" s="11" t="s">
+        <v>837</v>
+      </c>
+      <c r="G4" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="H4" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="I4" s="11" t="s">
+        <v>497</v>
+      </c>
+      <c r="J4" t="s">
+        <v>259</v>
+      </c>
+      <c r="K4" s="1" t="s">
+        <v>260</v>
+      </c>
+      <c r="L4" t="s">
+        <v>122</v>
+      </c>
+      <c r="M4" t="s">
+        <v>122</v>
+      </c>
+      <c r="N4" t="s">
+        <v>838</v>
+      </c>
+      <c r="O4" t="s">
+        <v>122</v>
+      </c>
+      <c r="P4" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" ht="58" x14ac:dyDescent="0.35">
+      <c r="A5" s="7" t="s">
+        <v>416</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>839</v>
+      </c>
+      <c r="D5" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="E5" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="F5" s="11" t="s">
+        <v>697</v>
+      </c>
+      <c r="G5" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="H5" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="I5" s="11" t="s">
+        <v>122</v>
+      </c>
+      <c r="J5" t="s">
+        <v>698</v>
+      </c>
+      <c r="K5" s="1" t="s">
+        <v>696</v>
+      </c>
+      <c r="L5" t="s">
+        <v>122</v>
+      </c>
+      <c r="M5" t="s">
+        <v>122</v>
+      </c>
+      <c r="N5" t="s">
+        <v>122</v>
+      </c>
+      <c r="O5" t="s">
+        <v>122</v>
+      </c>
+      <c r="P5" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" ht="58" x14ac:dyDescent="0.35">
+      <c r="A6" s="7" t="s">
+        <v>416</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>658</v>
+      </c>
+      <c r="D6" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="E6" s="11" t="s">
+        <v>659</v>
+      </c>
+      <c r="F6" s="11" t="s">
+        <v>660</v>
+      </c>
+      <c r="G6" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="H6" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="I6" s="11" t="s">
+        <v>122</v>
+      </c>
+      <c r="J6" t="s">
+        <v>661</v>
+      </c>
+      <c r="K6" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="L6" t="s">
+        <v>122</v>
+      </c>
+      <c r="M6" t="s">
+        <v>122</v>
+      </c>
+      <c r="N6" t="s">
+        <v>122</v>
+      </c>
+      <c r="O6" t="s">
+        <v>122</v>
+      </c>
+      <c r="P6" t="s">
+        <v>778</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A7" s="7" t="s">
+        <v>416</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>840</v>
+      </c>
+      <c r="D7" s="11" t="s">
+        <v>95</v>
+      </c>
+      <c r="E7" s="11" t="s">
+        <v>191</v>
+      </c>
+      <c r="F7" s="11" t="s">
+        <v>598</v>
+      </c>
+      <c r="G7" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="H7" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="I7" s="11" t="s">
+        <v>122</v>
+      </c>
+      <c r="J7" t="s">
+        <v>827</v>
+      </c>
+      <c r="K7" s="1" t="s">
+        <v>828</v>
+      </c>
+      <c r="L7" t="s">
+        <v>122</v>
+      </c>
+      <c r="M7" t="s">
+        <v>841</v>
+      </c>
+      <c r="N7" t="s">
+        <v>122</v>
+      </c>
+      <c r="O7" t="s">
+        <v>122</v>
+      </c>
+      <c r="P7" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" ht="29" x14ac:dyDescent="0.35">
+      <c r="A8" s="7" t="s">
+        <v>416</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>830</v>
+      </c>
+      <c r="D8" s="11" t="s">
+        <v>95</v>
+      </c>
+      <c r="E8" s="11" t="s">
+        <v>831</v>
+      </c>
+      <c r="F8" s="11" t="s">
+        <v>598</v>
+      </c>
+      <c r="G8" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="H8" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="I8" s="11" t="s">
+        <v>122</v>
+      </c>
+      <c r="J8" t="s">
+        <v>829</v>
+      </c>
+      <c r="K8" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="L8" t="s">
+        <v>122</v>
+      </c>
+      <c r="M8" t="s">
+        <v>122</v>
+      </c>
+      <c r="N8" t="s">
+        <v>842</v>
+      </c>
+      <c r="O8" t="s">
+        <v>122</v>
+      </c>
+      <c r="P8" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" ht="58" x14ac:dyDescent="0.35">
+      <c r="A9" s="7" t="s">
+        <v>415</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>843</v>
+      </c>
+      <c r="D9" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="E9" s="11" t="s">
+        <v>844</v>
+      </c>
+      <c r="F9" s="11" t="s">
+        <v>66</v>
+      </c>
+      <c r="G9" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="H9" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="I9" s="11" t="s">
+        <v>122</v>
+      </c>
+      <c r="J9" t="s">
+        <v>845</v>
+      </c>
+      <c r="K9" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="L9" t="s">
+        <v>122</v>
+      </c>
+      <c r="M9" t="s">
+        <v>122</v>
+      </c>
+      <c r="N9" t="s">
+        <v>122</v>
+      </c>
+      <c r="O9" t="s">
+        <v>122</v>
+      </c>
+      <c r="P9" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" ht="58" x14ac:dyDescent="0.35">
+      <c r="A10" s="7" t="s">
+        <v>415</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>658</v>
+      </c>
+      <c r="D10" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="E10" s="11" t="s">
+        <v>846</v>
+      </c>
+      <c r="F10" s="11" t="s">
+        <v>66</v>
+      </c>
+      <c r="G10" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="H10" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="I10" s="11" t="s">
+        <v>122</v>
+      </c>
+      <c r="J10" t="s">
+        <v>847</v>
+      </c>
+      <c r="K10" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="L10" t="s">
+        <v>122</v>
+      </c>
+      <c r="M10" t="s">
+        <v>122</v>
+      </c>
+      <c r="N10" t="s">
+        <v>122</v>
+      </c>
+      <c r="O10" t="s">
+        <v>122</v>
+      </c>
+      <c r="P10" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A11" s="7" t="s">
+        <v>415</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>848</v>
+      </c>
+      <c r="D11" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="E11" s="11" t="s">
+        <v>807</v>
+      </c>
+      <c r="F11" s="11" t="s">
+        <v>675</v>
+      </c>
+      <c r="G11" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="H11" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="I11" s="11" t="s">
+        <v>122</v>
+      </c>
+      <c r="J11" t="s">
+        <v>849</v>
+      </c>
+      <c r="K11" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="L11" t="s">
+        <v>122</v>
+      </c>
+      <c r="M11" t="s">
+        <v>122</v>
+      </c>
+      <c r="N11" t="s">
+        <v>122</v>
+      </c>
+      <c r="O11" t="s">
+        <v>122</v>
+      </c>
+      <c r="P11" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A12" s="7" t="s">
+        <v>415</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>850</v>
+      </c>
+      <c r="D12" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="E12" s="11" t="s">
+        <v>807</v>
+      </c>
+      <c r="F12" s="11" t="s">
+        <v>851</v>
+      </c>
+      <c r="G12" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="H12" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="I12" s="11" t="s">
+        <v>122</v>
+      </c>
+      <c r="J12" t="s">
+        <v>852</v>
+      </c>
+      <c r="K12" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="L12" t="s">
+        <v>122</v>
+      </c>
+      <c r="M12" t="s">
+        <v>122</v>
+      </c>
+      <c r="N12" t="s">
+        <v>122</v>
+      </c>
+      <c r="O12" t="s">
+        <v>122</v>
+      </c>
+      <c r="P12" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A13" s="7" t="s">
+        <v>415</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>853</v>
+      </c>
+      <c r="D13" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="E13" s="11" t="s">
+        <v>807</v>
+      </c>
+      <c r="F13" s="11" t="s">
+        <v>54</v>
+      </c>
+      <c r="G13" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="H13" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="I13" s="11" t="s">
+        <v>122</v>
+      </c>
+      <c r="J13" t="s">
+        <v>854</v>
+      </c>
+      <c r="K13" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="L13" t="s">
+        <v>122</v>
+      </c>
+      <c r="M13" t="s">
+        <v>122</v>
+      </c>
+      <c r="N13" t="s">
+        <v>122</v>
+      </c>
+      <c r="O13" t="s">
+        <v>122</v>
+      </c>
+      <c r="P13" t="s">
+        <v>122</v>
+      </c>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="B2:B13">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="notEqual">
+      <formula>""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{067B8281-AB10-416A-8A55-B2F46EB8E8FB}">
   <dimension ref="A1:O7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3332,7 +4103,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A424D0F2-3B88-4770-93C0-98D49DE8D516}">
   <dimension ref="A1:O104"/>
   <sheetViews>
@@ -8251,7 +9022,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B456D714-2DB6-4B8B-BC8E-8AA7501F8C79}">
   <dimension ref="A1:O7"/>
   <sheetViews>
@@ -8602,7 +9373,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E53E83C4-68F7-4929-AA83-3F95502173FC}">
   <dimension ref="A1:O195"/>
   <sheetViews>
@@ -10457,7 +11228,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2720FBDC-F538-4F79-9784-827E5ACB3995}">
   <dimension ref="A1:P130"/>
   <sheetViews>

</xml_diff>

<commit_message>
updated rules, See #532
</commit_message>
<xml_diff>
--- a/Deliverables/RULES/USDM_CORE_Rules_Changes.xlsx
+++ b/Deliverables/RULES/USDM_CORE_Rules_Changes.xlsx
@@ -5,24 +5,25 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Stack\CL027\Publish\CORE\3.9\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Stack\CL027\Publish\CORE\3.10\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{89D4C58F-A760-46A5-B0FD-5269F2849C4B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{5CA2923E-2C1F-4FAA-A675-FDB71525A4E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2280" yWindow="0" windowWidth="14650" windowHeight="12160" xr2:uid="{418CF395-400B-43AB-9594-6DFC1F089218}"/>
+    <workbookView xWindow="-13560" yWindow="-21720" windowWidth="51840" windowHeight="21120" xr2:uid="{418CF395-400B-43AB-9594-6DFC1F089218}"/>
   </bookViews>
   <sheets>
-    <sheet name="Changes release 3.8 -&gt; 3.9" sheetId="11" r:id="rId1"/>
-    <sheet name="Changes release 3.7 -&gt; 3.8" sheetId="10" r:id="rId2"/>
-    <sheet name="Changes release 3.6 -&gt; 3.7" sheetId="9" r:id="rId3"/>
-    <sheet name="Changes release 3.5-&gt;3.6" sheetId="8" r:id="rId4"/>
-    <sheet name="Changes release 3.4-&gt;3.5" sheetId="7" r:id="rId5"/>
-    <sheet name="Changes release 3.3-&gt;3.4" sheetId="5" r:id="rId6"/>
-    <sheet name="Changes release 3.1-&gt;3.3" sheetId="6" r:id="rId7"/>
+    <sheet name="Changes release 3.9 -&gt; 3.10" sheetId="12" r:id="rId1"/>
+    <sheet name="Changes release 3.8 -&gt; 3.9" sheetId="11" r:id="rId2"/>
+    <sheet name="Changes release 3.7 -&gt; 3.8" sheetId="10" r:id="rId3"/>
+    <sheet name="Changes release 3.6 -&gt; 3.7" sheetId="9" r:id="rId4"/>
+    <sheet name="Changes release 3.5-&gt;3.6" sheetId="8" r:id="rId5"/>
+    <sheet name="Changes release 3.4-&gt;3.5" sheetId="7" r:id="rId6"/>
+    <sheet name="Changes release 3.3-&gt;3.4" sheetId="5" r:id="rId7"/>
+    <sheet name="Changes release 3.1-&gt;3.3" sheetId="6" r:id="rId8"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">'Changes release 3.3-&gt;3.4'!$A$1:$O$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">'Changes release 3.3-&gt;3.4'!$A$1:$O$1</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -45,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5050" uniqueCount="1060">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5610" uniqueCount="1132">
   <si>
     <t>All</t>
   </si>
@@ -51000,6 +51001,451 @@
         <scheme val="minor"/>
       </rPr>
       <t>.</t>
+    </r>
+  </si>
+  <si>
+    <t>A study version's study phase must be specified according to the extensible Trial Phase Response (C66737) SDTM codelist (e.g. an entry with a code or decode used from the codelist should be consistent with the full entry in the codelist).</t>
+  </si>
+  <si>
+    <t>If the intervention model indicates a single group design then only one intervention is expected. In all other cases more interventions are expected.</t>
+  </si>
+  <si>
+    <t>A study version's study type must be specified using the Study Type Response (C99077) SDTM codelist.</t>
+  </si>
+  <si>
+    <t>A study design's trial intent types must be specified according to the extensible Trial Intent Type Response (C66736) SDTM codelist (e.g. an entry with a code or decode used from the codelist should be consistent with the full entry in the codelist).</t>
+  </si>
+  <si>
+    <t>DDF00118</t>
+  </si>
+  <si>
+    <t>A study design's trial types must be specified according to the extensible Trial Type Response (C66739) SDTM codelist (e.g. an entry with a code or decode used from the codelist should be consistent with the full entry in the codelist).</t>
+  </si>
+  <si>
+    <t>DDF00119</t>
+  </si>
+  <si>
+    <t>A study design's intervention model must be specified according to the extensible Intervention Model Response (C99076) SDTM codelist (e.g. an entry with a code or decode used from the codelist should be consistent with the full entry in the codelist).</t>
+  </si>
+  <si>
+    <t>DDF00120</t>
+  </si>
+  <si>
+    <t>A study design's blinding schema must be specified according to the extensible Trial Blinding Schema Response (C66735) SDTM codelist (e.g. an entry with a code or decode used from the codelist should be consistent with the full entry in the codelist).</t>
+  </si>
+  <si>
+    <t>DDF00121</t>
+  </si>
+  <si>
+    <t>A study design's characteristics must be specified according to the Study design characteristics (C207416) DDF codelist (e.g. an entry with a code or decode used from the codelist should be consistent with the full entry in the codelist).</t>
+  </si>
+  <si>
+    <t>Within a study design, if more characteristics are defined, they must be distinct.</t>
+  </si>
+  <si>
+    <t>DDF00134</t>
+  </si>
+  <si>
+    <t>Within a study design, if more trial types are defined, they must be distinct.</t>
+  </si>
+  <si>
+    <t>DDF00055</t>
+  </si>
+  <si>
+    <t>Within a study design, if more therapeutic areas are defined, they must be distinct.</t>
+  </si>
+  <si>
+    <t>DDF00056</t>
+  </si>
+  <si>
+    <t>Within a study design, if more trial intent types are defined, they must be distinct.</t>
+  </si>
+  <si>
+    <t>DDF00057</t>
+  </si>
+  <si>
+    <t>DDF00070</t>
+  </si>
+  <si>
+    <t>A study definition document version must not be referenced more than once by the same study design.</t>
+  </si>
+  <si>
+    <t>ObservationalStudyDesign, InterventionalStudyDesign</t>
+  </si>
+  <si>
+    <t>StudyDesign=&gt;ObservationalStudyDesign, InterventionalStudyDesign</t>
+  </si>
+  <si>
+    <t>StudyVersion, ObservationalStudyDesign, InterventionalStudyDesign</t>
+  </si>
+  <si>
+    <t>StudyVersion, StudyDesign=&gt;StudyVersion, ObservationalStudyDesign, InterventionalStudyDesign</t>
+  </si>
+  <si>
+    <t>CHK0257</t>
+  </si>
+  <si>
+    <t>InterventionalStudyDesign</t>
+  </si>
+  <si>
+    <t>model</t>
+  </si>
+  <si>
+    <t>CHK0258</t>
+  </si>
+  <si>
+    <t>An interventional study design's intent types must be specified according to the extensible Trial Intent Type Response (C66736) SDTM codelist (e.g. an entry with a code or decode used from the codelist should be consistent with the full entry in the codelist).</t>
+  </si>
+  <si>
+    <t>intentTypes</t>
+  </si>
+  <si>
+    <t>CHK0259</t>
+  </si>
+  <si>
+    <t>An interventional study design's sub types must be specified according to the extensible Trial Type Response (C66739) SDTM codelist (e.g. an entry with a code or decode used from the codelist should be consistent with the full entry in the codelist).</t>
+  </si>
+  <si>
+    <t>subTypes</t>
+  </si>
+  <si>
+    <t>CHK0260</t>
+  </si>
+  <si>
+    <t>CHK0261</t>
+  </si>
+  <si>
+    <t>CHK0262</t>
+  </si>
+  <si>
+    <t>A study design's characteristics must be specified according to the study design characteristics (C207416) DDF codelist (e.g. an entry with a code or decode used from the codelist should be consistent with the full entry in the codelist).</t>
+  </si>
+  <si>
+    <t>InterventionalStudyDesign, ObservationalStudyDesign</t>
+  </si>
+  <si>
+    <t>CHK0263</t>
+  </si>
+  <si>
+    <t>CHK0264</t>
+  </si>
+  <si>
+    <t>Within a study design, if more sub types are defined, they must be distinct.</t>
+  </si>
+  <si>
+    <t>CHK0265</t>
+  </si>
+  <si>
+    <t>CHK0266</t>
+  </si>
+  <si>
+    <t>Within a study design, if more intent types are defined, they must be distinct.</t>
+  </si>
+  <si>
+    <t>CHK0267</t>
+  </si>
+  <si>
+    <t>A study design's observational model must be specified according to the extensible Observational Study Model (C127259) SDTM codelist (e.g. an entry with a code or decode used from the codelist should be consistent with the full entry in the codelist).</t>
+  </si>
+  <si>
+    <t>ObservationalStudyDesign</t>
+  </si>
+  <si>
+    <t>CHK0268</t>
+  </si>
+  <si>
+    <t>An observational study design's time perspective must be specified according to the extensible Observational Study Time Perspective (C127261) SDTM codelist (e.g. an entry with a code or decode used from the codelist should be consistent with the full entry in the codelist).</t>
+  </si>
+  <si>
+    <t>timePerspective</t>
+  </si>
+  <si>
+    <t>CHK0269</t>
+  </si>
+  <si>
+    <t>An observational study design's sampling method must be specified according to the extensible Observational Study Sampling Method (C127260) SDTM codelist (e.g. an entry with a code or decode used from the codelist should be consistent with the full entry in the codelist).</t>
+  </si>
+  <si>
+    <t>samplingMethod</t>
+  </si>
+  <si>
+    <t>CHK0270</t>
+  </si>
+  <si>
+    <t>A observational study design's sub types must be specified according to the (Cxxxx) DDF codelist (e.g. an entry with a code or decode used from the codelist should be consistent with the full entry in the codelist).</t>
+  </si>
+  <si>
+    <t>CHK0271</t>
+  </si>
+  <si>
+    <t xml:space="preserve">An interventional study must be specified using the InterventionalStudyDesign class. </t>
+  </si>
+  <si>
+    <t>CHK0272</t>
+  </si>
+  <si>
+    <t>An observational study (including patient registries) must be specified using the ObservationalStudyDesign class.</t>
+  </si>
+  <si>
+    <t>CHK0273</t>
+  </si>
+  <si>
+    <t>A study design's study phase must be specified according to the extensible Trial Phase Response (C66737) SDTM codelist (e.g. an entry with a code or decode used from the codelist should be consistent with the full entry in the codelist).</t>
+  </si>
+  <si>
+    <t>CHK0274</t>
+  </si>
+  <si>
+    <t>A study design's study type must be specified using the Study Type Response (C99077) SDTM codelist.</t>
+  </si>
+  <si>
+    <t>CHK0275</t>
+  </si>
+  <si>
+    <t>If a biospecimen retention indicates that a type of biospecimen is retained, then there must be an indication of whether the type of biospecimen includes DNA.</t>
+  </si>
+  <si>
+    <t>BiospecimenRetention</t>
+  </si>
+  <si>
+    <t>includesDNA</t>
+  </si>
+  <si>
+    <t>Version 4.0 (Version 3.10)</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">The minimum value of a range must be less than </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>the</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>maximum</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>value</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>of</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>the</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> range.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">The minimum value of a range must be less than </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF0000FF"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>or</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF0000FF"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>equal</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF0000FF"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>to</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF0000FF"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>the</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF0000FF"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>maximum</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF0000FF"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>value</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF0000FF"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>of the range.</t>
     </r>
   </si>
 </sst>
@@ -51149,7 +51595,14 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="2">
+  <dxfs count="3">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -51493,12 +51946,1799 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DA56E3A9-6AF6-4F10-BAF1-2E2148AC6531}">
+  <sheetPr codeName="Sheet8"/>
+  <dimension ref="A1:P35"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K8" sqref="K8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="2" max="2" width="12" customWidth="1"/>
+    <col min="3" max="3" width="49.1796875" customWidth="1"/>
+    <col min="4" max="4" width="9.26953125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="25" style="1" customWidth="1"/>
+    <col min="6" max="6" width="18.54296875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.36328125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.81640625" customWidth="1"/>
+    <col min="9" max="9" width="11.453125" customWidth="1"/>
+    <col min="10" max="10" width="8.36328125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="44.453125" style="1" customWidth="1"/>
+    <col min="12" max="12" width="19.7265625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="36.90625" style="1" customWidth="1"/>
+    <col min="14" max="14" width="15.26953125" bestFit="1" customWidth="1"/>
+    <col min="15" max="16" width="9.54296875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:16" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="A1" s="8" t="s">
+        <v>394</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>602</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>344</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>345</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>346</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>347</v>
+      </c>
+      <c r="G1" s="8" t="s">
+        <v>348</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>1129</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>350</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>531</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>406</v>
+      </c>
+      <c r="L1" s="8" t="s">
+        <v>240</v>
+      </c>
+      <c r="M1" s="5" t="s">
+        <v>343</v>
+      </c>
+      <c r="N1" s="7" t="s">
+        <v>241</v>
+      </c>
+      <c r="O1" s="7" t="s">
+        <v>532</v>
+      </c>
+      <c r="P1" s="7" t="s">
+        <v>533</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="A2" s="7" t="s">
+        <v>254</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>1060</v>
+      </c>
+      <c r="D2" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="F2" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="G2" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="H2" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="I2" s="11" t="s">
+        <v>335</v>
+      </c>
+      <c r="J2" t="s">
+        <v>39</v>
+      </c>
+      <c r="K2" s="13" t="s">
+        <v>98</v>
+      </c>
+      <c r="L2" t="s">
+        <v>98</v>
+      </c>
+      <c r="M2" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="N2" t="s">
+        <v>98</v>
+      </c>
+      <c r="O2" t="s">
+        <v>98</v>
+      </c>
+      <c r="P2" t="s">
+        <v>534</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A3" s="7" t="s">
+        <v>254</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>1061</v>
+      </c>
+      <c r="D3" s="11" t="s">
+        <v>74</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>153</v>
+      </c>
+      <c r="F3" s="11" t="s">
+        <v>132</v>
+      </c>
+      <c r="G3" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="H3" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="I3" s="11" t="s">
+        <v>608</v>
+      </c>
+      <c r="J3" t="s">
+        <v>609</v>
+      </c>
+      <c r="K3" s="13" t="s">
+        <v>98</v>
+      </c>
+      <c r="L3" t="s">
+        <v>98</v>
+      </c>
+      <c r="M3" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="N3" t="s">
+        <v>98</v>
+      </c>
+      <c r="O3" t="s">
+        <v>98</v>
+      </c>
+      <c r="P3" t="s">
+        <v>534</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" ht="29" x14ac:dyDescent="0.35">
+      <c r="A4" s="7" t="s">
+        <v>254</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>1062</v>
+      </c>
+      <c r="D4" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="F4" s="11" t="s">
+        <v>145</v>
+      </c>
+      <c r="G4" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="H4" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="I4" s="11" t="s">
+        <v>623</v>
+      </c>
+      <c r="J4" t="s">
+        <v>144</v>
+      </c>
+      <c r="K4" s="13" t="s">
+        <v>98</v>
+      </c>
+      <c r="L4" t="s">
+        <v>98</v>
+      </c>
+      <c r="M4" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="N4" t="s">
+        <v>98</v>
+      </c>
+      <c r="O4" t="s">
+        <v>98</v>
+      </c>
+      <c r="P4" t="s">
+        <v>534</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="A5" s="7" t="s">
+        <v>254</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>1063</v>
+      </c>
+      <c r="D5" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>153</v>
+      </c>
+      <c r="F5" s="11" t="s">
+        <v>154</v>
+      </c>
+      <c r="G5" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="H5" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="I5" s="11" t="s">
+        <v>1064</v>
+      </c>
+      <c r="J5" t="s">
+        <v>152</v>
+      </c>
+      <c r="K5" s="13" t="s">
+        <v>98</v>
+      </c>
+      <c r="L5" t="s">
+        <v>98</v>
+      </c>
+      <c r="M5" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="N5" t="s">
+        <v>98</v>
+      </c>
+      <c r="O5" t="s">
+        <v>98</v>
+      </c>
+      <c r="P5" t="s">
+        <v>534</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" ht="58" x14ac:dyDescent="0.35">
+      <c r="A6" s="7" t="s">
+        <v>254</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>1065</v>
+      </c>
+      <c r="D6" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>153</v>
+      </c>
+      <c r="F6" s="11" t="s">
+        <v>156</v>
+      </c>
+      <c r="G6" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="H6" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="I6" s="11" t="s">
+        <v>1066</v>
+      </c>
+      <c r="J6" t="s">
+        <v>155</v>
+      </c>
+      <c r="K6" s="13" t="s">
+        <v>98</v>
+      </c>
+      <c r="L6" t="s">
+        <v>98</v>
+      </c>
+      <c r="M6" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="N6" t="s">
+        <v>98</v>
+      </c>
+      <c r="O6" t="s">
+        <v>98</v>
+      </c>
+      <c r="P6" t="s">
+        <v>534</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="A7" s="7" t="s">
+        <v>254</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>1067</v>
+      </c>
+      <c r="D7" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>153</v>
+      </c>
+      <c r="F7" s="11" t="s">
+        <v>158</v>
+      </c>
+      <c r="G7" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="H7" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="I7" s="11" t="s">
+        <v>1068</v>
+      </c>
+      <c r="J7" t="s">
+        <v>157</v>
+      </c>
+      <c r="K7" s="13" t="s">
+        <v>98</v>
+      </c>
+      <c r="L7" t="s">
+        <v>98</v>
+      </c>
+      <c r="M7" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="N7" t="s">
+        <v>98</v>
+      </c>
+      <c r="O7" t="s">
+        <v>98</v>
+      </c>
+      <c r="P7" t="s">
+        <v>534</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="A8" s="7" t="s">
+        <v>254</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>1069</v>
+      </c>
+      <c r="D8" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>153</v>
+      </c>
+      <c r="F8" s="11" t="s">
+        <v>160</v>
+      </c>
+      <c r="G8" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="H8" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="I8" s="11" t="s">
+        <v>1070</v>
+      </c>
+      <c r="J8" t="s">
+        <v>159</v>
+      </c>
+      <c r="K8" s="13" t="s">
+        <v>98</v>
+      </c>
+      <c r="L8" t="s">
+        <v>98</v>
+      </c>
+      <c r="M8" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="N8" t="s">
+        <v>98</v>
+      </c>
+      <c r="O8" t="s">
+        <v>98</v>
+      </c>
+      <c r="P8" t="s">
+        <v>534</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="A9" s="7" t="s">
+        <v>254</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>1071</v>
+      </c>
+      <c r="D9" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>153</v>
+      </c>
+      <c r="F9" s="11" t="s">
+        <v>162</v>
+      </c>
+      <c r="G9" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="H9" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="I9" s="11" t="s">
+        <v>625</v>
+      </c>
+      <c r="J9" t="s">
+        <v>161</v>
+      </c>
+      <c r="K9" s="13" t="s">
+        <v>98</v>
+      </c>
+      <c r="L9" t="s">
+        <v>98</v>
+      </c>
+      <c r="M9" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="N9" t="s">
+        <v>98</v>
+      </c>
+      <c r="O9" t="s">
+        <v>98</v>
+      </c>
+      <c r="P9" t="s">
+        <v>534</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" ht="29" x14ac:dyDescent="0.35">
+      <c r="A10" s="7" t="s">
+        <v>254</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>1072</v>
+      </c>
+      <c r="D10" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>153</v>
+      </c>
+      <c r="F10" s="11" t="s">
+        <v>162</v>
+      </c>
+      <c r="G10" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="H10" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="I10" s="11" t="s">
+        <v>1073</v>
+      </c>
+      <c r="J10" t="s">
+        <v>207</v>
+      </c>
+      <c r="K10" s="13" t="s">
+        <v>98</v>
+      </c>
+      <c r="L10" t="s">
+        <v>98</v>
+      </c>
+      <c r="M10" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="N10" t="s">
+        <v>98</v>
+      </c>
+      <c r="O10" t="s">
+        <v>98</v>
+      </c>
+      <c r="P10" t="s">
+        <v>534</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" ht="29" x14ac:dyDescent="0.35">
+      <c r="A11" s="7" t="s">
+        <v>254</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>1074</v>
+      </c>
+      <c r="D11" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>153</v>
+      </c>
+      <c r="F11" s="11" t="s">
+        <v>156</v>
+      </c>
+      <c r="G11" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="H11" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="I11" s="11" t="s">
+        <v>1075</v>
+      </c>
+      <c r="J11" t="s">
+        <v>208</v>
+      </c>
+      <c r="K11" s="13" t="s">
+        <v>98</v>
+      </c>
+      <c r="L11" t="s">
+        <v>98</v>
+      </c>
+      <c r="M11" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="N11" t="s">
+        <v>98</v>
+      </c>
+      <c r="O11" t="s">
+        <v>98</v>
+      </c>
+      <c r="P11" t="s">
+        <v>534</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" ht="29" x14ac:dyDescent="0.35">
+      <c r="A12" s="7" t="s">
+        <v>254</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>1076</v>
+      </c>
+      <c r="D12" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>153</v>
+      </c>
+      <c r="F12" s="11" t="s">
+        <v>210</v>
+      </c>
+      <c r="G12" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="H12" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="I12" s="11" t="s">
+        <v>1077</v>
+      </c>
+      <c r="J12" t="s">
+        <v>209</v>
+      </c>
+      <c r="K12" s="13" t="s">
+        <v>98</v>
+      </c>
+      <c r="L12" t="s">
+        <v>98</v>
+      </c>
+      <c r="M12" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="N12" t="s">
+        <v>98</v>
+      </c>
+      <c r="O12" t="s">
+        <v>98</v>
+      </c>
+      <c r="P12" t="s">
+        <v>534</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" ht="29" x14ac:dyDescent="0.35">
+      <c r="A13" s="7" t="s">
+        <v>254</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>1078</v>
+      </c>
+      <c r="D13" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>153</v>
+      </c>
+      <c r="F13" s="11" t="s">
+        <v>154</v>
+      </c>
+      <c r="G13" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="H13" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="I13" s="11" t="s">
+        <v>1079</v>
+      </c>
+      <c r="J13" t="s">
+        <v>211</v>
+      </c>
+      <c r="K13" s="13" t="s">
+        <v>98</v>
+      </c>
+      <c r="L13" t="s">
+        <v>98</v>
+      </c>
+      <c r="M13" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="N13" t="s">
+        <v>98</v>
+      </c>
+      <c r="O13" t="s">
+        <v>98</v>
+      </c>
+      <c r="P13" t="s">
+        <v>534</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" ht="29" x14ac:dyDescent="0.35">
+      <c r="A14" s="7" t="s">
+        <v>254</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>1131</v>
+      </c>
+      <c r="D14" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="E14" s="3" t="s">
+        <v>291</v>
+      </c>
+      <c r="F14" s="11" t="s">
+        <v>296</v>
+      </c>
+      <c r="G14" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="H14" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="I14" s="11" t="s">
+        <v>1080</v>
+      </c>
+      <c r="J14" t="s">
+        <v>448</v>
+      </c>
+      <c r="K14" s="13" t="s">
+        <v>1130</v>
+      </c>
+      <c r="L14" t="s">
+        <v>98</v>
+      </c>
+      <c r="M14" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="N14" t="s">
+        <v>98</v>
+      </c>
+      <c r="O14" t="s">
+        <v>98</v>
+      </c>
+      <c r="P14" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" ht="29" x14ac:dyDescent="0.35">
+      <c r="A15" s="7" t="s">
+        <v>254</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>1081</v>
+      </c>
+      <c r="D15" s="11" t="s">
+        <v>74</v>
+      </c>
+      <c r="E15" s="3" t="s">
+        <v>1082</v>
+      </c>
+      <c r="F15" s="11" t="s">
+        <v>392</v>
+      </c>
+      <c r="G15" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="H15" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="I15" s="11" t="s">
+        <v>98</v>
+      </c>
+      <c r="J15" t="s">
+        <v>578</v>
+      </c>
+      <c r="K15" s="13" t="s">
+        <v>98</v>
+      </c>
+      <c r="L15" t="s">
+        <v>98</v>
+      </c>
+      <c r="M15" s="1" t="s">
+        <v>1083</v>
+      </c>
+      <c r="N15" t="s">
+        <v>98</v>
+      </c>
+      <c r="O15" t="s">
+        <v>98</v>
+      </c>
+      <c r="P15" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A16" s="7" t="s">
+        <v>254</v>
+      </c>
+      <c r="B16" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>581</v>
+      </c>
+      <c r="D16" s="11" t="s">
+        <v>74</v>
+      </c>
+      <c r="E16" s="3" t="s">
+        <v>1084</v>
+      </c>
+      <c r="F16" s="11" t="s">
+        <v>392</v>
+      </c>
+      <c r="G16" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="H16" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="I16" s="11" t="s">
+        <v>98</v>
+      </c>
+      <c r="J16" t="s">
+        <v>580</v>
+      </c>
+      <c r="K16" s="13" t="s">
+        <v>98</v>
+      </c>
+      <c r="L16" t="s">
+        <v>98</v>
+      </c>
+      <c r="M16" s="1" t="s">
+        <v>1085</v>
+      </c>
+      <c r="N16" t="s">
+        <v>98</v>
+      </c>
+      <c r="O16" t="s">
+        <v>98</v>
+      </c>
+      <c r="P16" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="17" spans="1:16" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A17" s="7" t="s">
+        <v>253</v>
+      </c>
+      <c r="B17" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>1061</v>
+      </c>
+      <c r="D17" s="11" t="s">
+        <v>74</v>
+      </c>
+      <c r="E17" s="3" t="s">
+        <v>1087</v>
+      </c>
+      <c r="F17" s="11" t="s">
+        <v>1088</v>
+      </c>
+      <c r="G17" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="H17" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="I17" s="11" t="s">
+        <v>98</v>
+      </c>
+      <c r="J17" t="s">
+        <v>1086</v>
+      </c>
+      <c r="K17" s="13" t="s">
+        <v>98</v>
+      </c>
+      <c r="L17" t="s">
+        <v>98</v>
+      </c>
+      <c r="M17" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="N17" t="s">
+        <v>98</v>
+      </c>
+      <c r="O17" t="s">
+        <v>98</v>
+      </c>
+      <c r="P17" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="18" spans="1:16" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="A18" s="7" t="s">
+        <v>253</v>
+      </c>
+      <c r="B18" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>1090</v>
+      </c>
+      <c r="D18" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="E18" s="3" t="s">
+        <v>1087</v>
+      </c>
+      <c r="F18" s="11" t="s">
+        <v>1091</v>
+      </c>
+      <c r="G18" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="H18" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="I18" s="11" t="s">
+        <v>98</v>
+      </c>
+      <c r="J18" t="s">
+        <v>1089</v>
+      </c>
+      <c r="K18" s="13" t="s">
+        <v>98</v>
+      </c>
+      <c r="L18" t="s">
+        <v>98</v>
+      </c>
+      <c r="M18" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="N18" t="s">
+        <v>98</v>
+      </c>
+      <c r="O18" t="s">
+        <v>98</v>
+      </c>
+      <c r="P18" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="19" spans="1:16" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="A19" s="7" t="s">
+        <v>253</v>
+      </c>
+      <c r="B19" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>1093</v>
+      </c>
+      <c r="D19" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="E19" s="3" t="s">
+        <v>1087</v>
+      </c>
+      <c r="F19" s="11" t="s">
+        <v>1094</v>
+      </c>
+      <c r="G19" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="H19" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="I19" s="11" t="s">
+        <v>98</v>
+      </c>
+      <c r="J19" t="s">
+        <v>1092</v>
+      </c>
+      <c r="K19" s="13" t="s">
+        <v>98</v>
+      </c>
+      <c r="L19" t="s">
+        <v>98</v>
+      </c>
+      <c r="M19" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="N19" t="s">
+        <v>98</v>
+      </c>
+      <c r="O19" t="s">
+        <v>98</v>
+      </c>
+      <c r="P19" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="20" spans="1:16" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="A20" s="7" t="s">
+        <v>253</v>
+      </c>
+      <c r="B20" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>1067</v>
+      </c>
+      <c r="D20" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="E20" s="3" t="s">
+        <v>1087</v>
+      </c>
+      <c r="F20" s="11" t="s">
+        <v>1088</v>
+      </c>
+      <c r="G20" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="H20" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="I20" s="11" t="s">
+        <v>98</v>
+      </c>
+      <c r="J20" t="s">
+        <v>1095</v>
+      </c>
+      <c r="K20" s="13" t="s">
+        <v>98</v>
+      </c>
+      <c r="L20" t="s">
+        <v>98</v>
+      </c>
+      <c r="M20" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="N20" t="s">
+        <v>98</v>
+      </c>
+      <c r="O20" t="s">
+        <v>98</v>
+      </c>
+      <c r="P20" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="21" spans="1:16" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="A21" s="7" t="s">
+        <v>253</v>
+      </c>
+      <c r="B21" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>1069</v>
+      </c>
+      <c r="D21" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="E21" s="3" t="s">
+        <v>1087</v>
+      </c>
+      <c r="F21" s="11" t="s">
+        <v>160</v>
+      </c>
+      <c r="G21" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="H21" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="I21" s="11" t="s">
+        <v>98</v>
+      </c>
+      <c r="J21" t="s">
+        <v>1096</v>
+      </c>
+      <c r="K21" s="13" t="s">
+        <v>98</v>
+      </c>
+      <c r="L21" t="s">
+        <v>98</v>
+      </c>
+      <c r="M21" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="N21" t="s">
+        <v>98</v>
+      </c>
+      <c r="O21" t="s">
+        <v>98</v>
+      </c>
+      <c r="P21" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="22" spans="1:16" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="A22" s="7" t="s">
+        <v>253</v>
+      </c>
+      <c r="B22" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="C22" s="3" t="s">
+        <v>1098</v>
+      </c>
+      <c r="D22" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="E22" s="3" t="s">
+        <v>1099</v>
+      </c>
+      <c r="F22" s="11" t="s">
+        <v>162</v>
+      </c>
+      <c r="G22" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="H22" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="I22" s="11" t="s">
+        <v>98</v>
+      </c>
+      <c r="J22" t="s">
+        <v>1097</v>
+      </c>
+      <c r="K22" s="13" t="s">
+        <v>98</v>
+      </c>
+      <c r="L22" t="s">
+        <v>98</v>
+      </c>
+      <c r="M22" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="N22" t="s">
+        <v>98</v>
+      </c>
+      <c r="O22" t="s">
+        <v>98</v>
+      </c>
+      <c r="P22" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="23" spans="1:16" ht="29" x14ac:dyDescent="0.35">
+      <c r="A23" s="7" t="s">
+        <v>253</v>
+      </c>
+      <c r="B23" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>1072</v>
+      </c>
+      <c r="D23" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="E23" s="3" t="s">
+        <v>1099</v>
+      </c>
+      <c r="F23" s="11" t="s">
+        <v>162</v>
+      </c>
+      <c r="G23" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="H23" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="I23" s="11" t="s">
+        <v>98</v>
+      </c>
+      <c r="J23" t="s">
+        <v>1100</v>
+      </c>
+      <c r="K23" s="13" t="s">
+        <v>98</v>
+      </c>
+      <c r="L23" t="s">
+        <v>98</v>
+      </c>
+      <c r="M23" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="N23" t="s">
+        <v>98</v>
+      </c>
+      <c r="O23" t="s">
+        <v>98</v>
+      </c>
+      <c r="P23" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="24" spans="1:16" ht="29" x14ac:dyDescent="0.35">
+      <c r="A24" s="7" t="s">
+        <v>253</v>
+      </c>
+      <c r="B24" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="C24" s="3" t="s">
+        <v>1102</v>
+      </c>
+      <c r="D24" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="E24" s="3" t="s">
+        <v>1099</v>
+      </c>
+      <c r="F24" s="11" t="s">
+        <v>1094</v>
+      </c>
+      <c r="G24" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="H24" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="I24" s="11" t="s">
+        <v>98</v>
+      </c>
+      <c r="J24" t="s">
+        <v>1101</v>
+      </c>
+      <c r="K24" s="13" t="s">
+        <v>98</v>
+      </c>
+      <c r="L24" t="s">
+        <v>98</v>
+      </c>
+      <c r="M24" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="N24" t="s">
+        <v>98</v>
+      </c>
+      <c r="O24" t="s">
+        <v>98</v>
+      </c>
+      <c r="P24" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="25" spans="1:16" ht="29" x14ac:dyDescent="0.35">
+      <c r="A25" s="7" t="s">
+        <v>253</v>
+      </c>
+      <c r="B25" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="C25" s="3" t="s">
+        <v>1076</v>
+      </c>
+      <c r="D25" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="E25" s="3" t="s">
+        <v>1099</v>
+      </c>
+      <c r="F25" s="11" t="s">
+        <v>210</v>
+      </c>
+      <c r="G25" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="H25" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="I25" s="11" t="s">
+        <v>98</v>
+      </c>
+      <c r="J25" t="s">
+        <v>1103</v>
+      </c>
+      <c r="K25" s="13" t="s">
+        <v>98</v>
+      </c>
+      <c r="L25" t="s">
+        <v>98</v>
+      </c>
+      <c r="M25" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="N25" t="s">
+        <v>98</v>
+      </c>
+      <c r="O25" t="s">
+        <v>98</v>
+      </c>
+      <c r="P25" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="26" spans="1:16" ht="29" x14ac:dyDescent="0.35">
+      <c r="A26" s="7" t="s">
+        <v>253</v>
+      </c>
+      <c r="B26" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="C26" s="3" t="s">
+        <v>1105</v>
+      </c>
+      <c r="D26" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="E26" s="3" t="s">
+        <v>1087</v>
+      </c>
+      <c r="F26" s="11" t="s">
+        <v>1091</v>
+      </c>
+      <c r="G26" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="H26" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="I26" s="11" t="s">
+        <v>98</v>
+      </c>
+      <c r="J26" t="s">
+        <v>1104</v>
+      </c>
+      <c r="K26" s="13" t="s">
+        <v>98</v>
+      </c>
+      <c r="L26" t="s">
+        <v>98</v>
+      </c>
+      <c r="M26" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="N26" t="s">
+        <v>98</v>
+      </c>
+      <c r="O26" t="s">
+        <v>98</v>
+      </c>
+      <c r="P26" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="27" spans="1:16" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="A27" s="7" t="s">
+        <v>253</v>
+      </c>
+      <c r="B27" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="C27" s="3" t="s">
+        <v>1107</v>
+      </c>
+      <c r="D27" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="E27" s="3" t="s">
+        <v>1108</v>
+      </c>
+      <c r="F27" s="11" t="s">
+        <v>1088</v>
+      </c>
+      <c r="G27" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="H27" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="I27" s="11" t="s">
+        <v>98</v>
+      </c>
+      <c r="J27" t="s">
+        <v>1106</v>
+      </c>
+      <c r="K27" s="13" t="s">
+        <v>98</v>
+      </c>
+      <c r="L27" t="s">
+        <v>98</v>
+      </c>
+      <c r="M27" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="N27" t="s">
+        <v>98</v>
+      </c>
+      <c r="O27" t="s">
+        <v>98</v>
+      </c>
+      <c r="P27" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="28" spans="1:16" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="A28" s="7" t="s">
+        <v>253</v>
+      </c>
+      <c r="B28" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="C28" s="3" t="s">
+        <v>1110</v>
+      </c>
+      <c r="D28" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="E28" s="3" t="s">
+        <v>1108</v>
+      </c>
+      <c r="F28" s="11" t="s">
+        <v>1111</v>
+      </c>
+      <c r="G28" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="H28" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="I28" s="11" t="s">
+        <v>98</v>
+      </c>
+      <c r="J28" t="s">
+        <v>1109</v>
+      </c>
+      <c r="K28" s="13" t="s">
+        <v>98</v>
+      </c>
+      <c r="L28" t="s">
+        <v>98</v>
+      </c>
+      <c r="M28" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="N28" t="s">
+        <v>98</v>
+      </c>
+      <c r="O28" t="s">
+        <v>98</v>
+      </c>
+      <c r="P28" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="29" spans="1:16" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="A29" s="7" t="s">
+        <v>253</v>
+      </c>
+      <c r="B29" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="C29" s="3" t="s">
+        <v>1113</v>
+      </c>
+      <c r="D29" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="E29" s="3" t="s">
+        <v>1108</v>
+      </c>
+      <c r="F29" s="11" t="s">
+        <v>1114</v>
+      </c>
+      <c r="G29" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="H29" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="I29" s="11" t="s">
+        <v>98</v>
+      </c>
+      <c r="J29" t="s">
+        <v>1112</v>
+      </c>
+      <c r="K29" s="13" t="s">
+        <v>98</v>
+      </c>
+      <c r="L29" t="s">
+        <v>98</v>
+      </c>
+      <c r="M29" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="N29" t="s">
+        <v>98</v>
+      </c>
+      <c r="O29" t="s">
+        <v>98</v>
+      </c>
+      <c r="P29" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="30" spans="1:16" ht="58" x14ac:dyDescent="0.35">
+      <c r="A30" s="7" t="s">
+        <v>253</v>
+      </c>
+      <c r="B30" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="C30" s="3" t="s">
+        <v>1116</v>
+      </c>
+      <c r="D30" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="E30" s="3" t="s">
+        <v>1108</v>
+      </c>
+      <c r="F30" s="11" t="s">
+        <v>1094</v>
+      </c>
+      <c r="G30" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="H30" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="I30" s="11" t="s">
+        <v>98</v>
+      </c>
+      <c r="J30" t="s">
+        <v>1115</v>
+      </c>
+      <c r="K30" s="13" t="s">
+        <v>98</v>
+      </c>
+      <c r="L30" t="s">
+        <v>98</v>
+      </c>
+      <c r="M30" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="N30" t="s">
+        <v>98</v>
+      </c>
+      <c r="O30" t="s">
+        <v>98</v>
+      </c>
+      <c r="P30" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="31" spans="1:16" ht="29" x14ac:dyDescent="0.35">
+      <c r="A31" s="7" t="s">
+        <v>253</v>
+      </c>
+      <c r="B31" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="C31" s="3" t="s">
+        <v>1118</v>
+      </c>
+      <c r="D31" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="E31" s="3" t="s">
+        <v>1087</v>
+      </c>
+      <c r="F31" s="11" t="s">
+        <v>145</v>
+      </c>
+      <c r="G31" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="H31" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="I31" s="11" t="s">
+        <v>98</v>
+      </c>
+      <c r="J31" t="s">
+        <v>1117</v>
+      </c>
+      <c r="K31" s="13" t="s">
+        <v>98</v>
+      </c>
+      <c r="L31" t="s">
+        <v>98</v>
+      </c>
+      <c r="M31" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="N31" t="s">
+        <v>98</v>
+      </c>
+      <c r="O31" t="s">
+        <v>98</v>
+      </c>
+      <c r="P31" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="32" spans="1:16" ht="29" x14ac:dyDescent="0.35">
+      <c r="A32" s="7" t="s">
+        <v>253</v>
+      </c>
+      <c r="B32" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="C32" s="3" t="s">
+        <v>1120</v>
+      </c>
+      <c r="D32" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="E32" s="3" t="s">
+        <v>1108</v>
+      </c>
+      <c r="F32" s="11" t="s">
+        <v>145</v>
+      </c>
+      <c r="G32" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="H32" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="I32" s="11" t="s">
+        <v>98</v>
+      </c>
+      <c r="J32" t="s">
+        <v>1119</v>
+      </c>
+      <c r="K32" s="13" t="s">
+        <v>98</v>
+      </c>
+      <c r="L32" t="s">
+        <v>98</v>
+      </c>
+      <c r="M32" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="N32" t="s">
+        <v>98</v>
+      </c>
+      <c r="O32" t="s">
+        <v>98</v>
+      </c>
+      <c r="P32" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="33" spans="1:16" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="A33" s="7" t="s">
+        <v>253</v>
+      </c>
+      <c r="B33" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="C33" s="3" t="s">
+        <v>1122</v>
+      </c>
+      <c r="D33" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="E33" s="3" t="s">
+        <v>1082</v>
+      </c>
+      <c r="F33" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="G33" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="H33" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="I33" s="11" t="s">
+        <v>98</v>
+      </c>
+      <c r="J33" t="s">
+        <v>1121</v>
+      </c>
+      <c r="K33" s="13" t="s">
+        <v>98</v>
+      </c>
+      <c r="L33" t="s">
+        <v>98</v>
+      </c>
+      <c r="M33" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="N33" t="s">
+        <v>98</v>
+      </c>
+      <c r="O33" t="s">
+        <v>98</v>
+      </c>
+      <c r="P33" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="34" spans="1:16" ht="29" x14ac:dyDescent="0.35">
+      <c r="A34" s="7" t="s">
+        <v>253</v>
+      </c>
+      <c r="B34" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="C34" s="3" t="s">
+        <v>1124</v>
+      </c>
+      <c r="D34" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="E34" s="3" t="s">
+        <v>1082</v>
+      </c>
+      <c r="F34" s="11" t="s">
+        <v>145</v>
+      </c>
+      <c r="G34" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="H34" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="I34" s="11" t="s">
+        <v>98</v>
+      </c>
+      <c r="J34" t="s">
+        <v>1123</v>
+      </c>
+      <c r="K34" s="13" t="s">
+        <v>98</v>
+      </c>
+      <c r="L34" t="s">
+        <v>98</v>
+      </c>
+      <c r="M34" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="N34" t="s">
+        <v>98</v>
+      </c>
+      <c r="O34" t="s">
+        <v>98</v>
+      </c>
+      <c r="P34" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="35" spans="1:16" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A35" s="7" t="s">
+        <v>253</v>
+      </c>
+      <c r="B35" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="C35" s="3" t="s">
+        <v>1126</v>
+      </c>
+      <c r="D35" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="E35" s="3" t="s">
+        <v>1127</v>
+      </c>
+      <c r="F35" s="11" t="s">
+        <v>1128</v>
+      </c>
+      <c r="G35" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="H35" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="I35" s="11" t="s">
+        <v>98</v>
+      </c>
+      <c r="J35" t="s">
+        <v>1125</v>
+      </c>
+      <c r="K35" s="13" t="s">
+        <v>98</v>
+      </c>
+      <c r="L35" t="s">
+        <v>98</v>
+      </c>
+      <c r="M35" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="N35" t="s">
+        <v>98</v>
+      </c>
+      <c r="O35" t="s">
+        <v>98</v>
+      </c>
+      <c r="P35" t="s">
+        <v>98</v>
+      </c>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="B2:B35">
+    <cfRule type="cellIs" dxfId="2" priority="1" operator="notEqual">
+      <formula>""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{04922479-DC74-45C1-A6FB-8A5685DCA4C3}">
   <sheetPr codeName="Sheet7"/>
   <dimension ref="A1:Q49"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K11" sqref="K11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -54015,7 +56255,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8EF31D4B-F1B8-4E5E-A34A-AF6E16EC4595}">
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:P13"/>
@@ -54700,7 +56940,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{067B8281-AB10-416A-8A55-B2F46EB8E8FB}">
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:O7"/>
@@ -55055,7 +57295,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A424D0F2-3B88-4770-93C0-98D49DE8D516}">
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:O104"/>
@@ -59975,7 +62215,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B456D714-2DB6-4B8B-BC8E-8AA7501F8C79}">
   <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:O7"/>
@@ -60327,7 +62567,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E53E83C4-68F7-4929-AA83-3F95502173FC}">
   <sheetPr codeName="Sheet5"/>
   <dimension ref="A1:O195"/>
@@ -62183,7 +64423,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2720FBDC-F538-4F79-9784-827E5ACB3995}">
   <sheetPr codeName="Sheet6"/>
   <dimension ref="A1:P130"/>

</xml_diff>

<commit_message>
Rules updates acc to #575, #561, #556, #569
</commit_message>
<xml_diff>
--- a/Deliverables/RULES/USDM_CORE_Rules_Changes.xlsx
+++ b/Deliverables/RULES/USDM_CORE_Rules_Changes.xlsx
@@ -1,29 +1,30 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Stack\CL027\Publish\CORE\3.10\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Stack\CL027\Publish\CORE\3.11\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{882D2D0D-135C-4C3D-92A6-5AA0784E194F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{2B9777CA-54F9-4760-99D4-FF84EB69137A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3180" yWindow="-19095" windowWidth="24360" windowHeight="17400" xr2:uid="{418CF395-400B-43AB-9594-6DFC1F089218}"/>
+    <workbookView xWindow="-165" yWindow="-19080" windowWidth="23295" windowHeight="18015" xr2:uid="{418CF395-400B-43AB-9594-6DFC1F089218}"/>
   </bookViews>
   <sheets>
-    <sheet name="Changes release 3.9 -&gt; 3.10" sheetId="12" r:id="rId1"/>
-    <sheet name="Changes release 3.8 -&gt; 3.9" sheetId="11" r:id="rId2"/>
-    <sheet name="Changes release 3.7 -&gt; 3.8" sheetId="10" r:id="rId3"/>
-    <sheet name="Changes release 3.6 -&gt; 3.7" sheetId="9" r:id="rId4"/>
-    <sheet name="Changes release 3.5-&gt;3.6" sheetId="8" r:id="rId5"/>
-    <sheet name="Changes release 3.4-&gt;3.5" sheetId="7" r:id="rId6"/>
-    <sheet name="Changes release 3.3-&gt;3.4" sheetId="5" r:id="rId7"/>
-    <sheet name="Changes release 3.1-&gt;3.3" sheetId="6" r:id="rId8"/>
+    <sheet name="Changes release 3.10 -&gt; 3.11" sheetId="13" r:id="rId1"/>
+    <sheet name="Changes release 3.9 -&gt; 3.10" sheetId="12" r:id="rId2"/>
+    <sheet name="Changes release 3.8 -&gt; 3.9" sheetId="11" r:id="rId3"/>
+    <sheet name="Changes release 3.7 -&gt; 3.8" sheetId="10" r:id="rId4"/>
+    <sheet name="Changes release 3.6 -&gt; 3.7" sheetId="9" r:id="rId5"/>
+    <sheet name="Changes release 3.5-&gt;3.6" sheetId="8" r:id="rId6"/>
+    <sheet name="Changes release 3.4-&gt;3.5" sheetId="7" r:id="rId7"/>
+    <sheet name="Changes release 3.3-&gt;3.4" sheetId="5" r:id="rId8"/>
+    <sheet name="Changes release 3.1-&gt;3.3" sheetId="6" r:id="rId9"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">'Changes release 3.3-&gt;3.4'!$A$1:$O$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="7" hidden="1">'Changes release 3.3-&gt;3.4'!$A$1:$O$1</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -46,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5626" uniqueCount="1134">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6061" uniqueCount="1186">
   <si>
     <t>All</t>
   </si>
@@ -51453,6 +51454,517 @@
   </si>
   <si>
     <t>CHK0276</t>
+  </si>
+  <si>
+    <t>EligibilityCriterionItem, Characteristic, Condition, Objective, Endpoint</t>
+  </si>
+  <si>
+    <t>EligibilityCriterion, Characteristic, Condition, Objective, Endpoint=&gt;EligibilityCriterionItem, Characteristic, Condition, Objective, Endpoint</t>
+  </si>
+  <si>
+    <t>Any parameter name referenced in a tag in the text should be specified in the data dictionary parameter maps.</t>
+  </si>
+  <si>
+    <t>DDF00089</t>
+  </si>
+  <si>
+    <t>The unit of a planned age is expected to be specified using terms from the Age Unit (C66781) SDTM codelist.</t>
+  </si>
+  <si>
+    <t>Within a study design, if a planned completion number is defined, it must be specified either in the study population or in all cohorts.</t>
+  </si>
+  <si>
+    <t>DDF00132</t>
+  </si>
+  <si>
+    <t>Within a study design, if a planned enrollment number is defined, it must be specified either in the study population or in all cohorts.</t>
+  </si>
+  <si>
+    <t>DDF00133</t>
+  </si>
+  <si>
+    <t>DDF00067</t>
+  </si>
+  <si>
+    <t>?=&gt;N</t>
+  </si>
+  <si>
+    <t>The minimum value of a range must be less than or equal to the maximum value of the range.</t>
+  </si>
+  <si>
+    <t>denominator</t>
+  </si>
+  <si>
+    <t>numerator, denominator=&gt;denominator</t>
+  </si>
+  <si>
+    <t>DDF00086</t>
+  </si>
+  <si>
+    <t>forStudyCohort, forStudySite, forGeographicScope</t>
+  </si>
+  <si>
+    <t>appliesTo=&gt;forStudyCohort, forStudySite, forGeographicScope</t>
+  </si>
+  <si>
+    <t>CHK0277</t>
+  </si>
+  <si>
+    <t>CHK0278</t>
+  </si>
+  <si>
+    <t>A unit must not be specified for a planned enrollment number.</t>
+  </si>
+  <si>
+    <t>plannedEnrollmentNumberQuantity, plannedEnrollmentNumberRange</t>
+  </si>
+  <si>
+    <t>CHK0279</t>
+  </si>
+  <si>
+    <t>plannedCompletionNumberRange, plannedCompletionNumberQuantity</t>
+  </si>
+  <si>
+    <t>CHK0280</t>
+  </si>
+  <si>
+    <t>plannedEnrollmentNumberRange, plannedEnrollmentNumberQuantity</t>
+  </si>
+  <si>
+    <t>CHK0281</t>
+  </si>
+  <si>
+    <t>CHK0282</t>
+  </si>
+  <si>
+    <t>If a strength numerator quantity is specified, it must have a unit.</t>
+  </si>
+  <si>
+    <t>numeratorQuantity</t>
+  </si>
+  <si>
+    <t>CHK0283</t>
+  </si>
+  <si>
+    <t>If a strength numerator range is specified, both the minValue and maxValue must have a unit.</t>
+  </si>
+  <si>
+    <t>numeratorRange</t>
+  </si>
+  <si>
+    <t>CHK0284</t>
+  </si>
+  <si>
+    <t>For each strength, either a numerator quantity or range must be specified.</t>
+  </si>
+  <si>
+    <t>numeratorQuantity, numeratorRange</t>
+  </si>
+  <si>
+    <t>CHK0285</t>
+  </si>
+  <si>
+    <t>If the unit is the same (or missing) for both the minimum and maximum value, then the minimum value must be less than the maximum value.</t>
+  </si>
+  <si>
+    <t>CHK0286</t>
+  </si>
+  <si>
+    <t>For each range, a unit must be specified either for both the minimum and the maximum value, or for neither of them.</t>
+  </si>
+  <si>
+    <t>CHK0287</t>
+  </si>
+  <si>
+    <t>A unit must not be specified for a planned completion number.</t>
+  </si>
+  <si>
+    <t>CHK0288</t>
+  </si>
+  <si>
+    <t>For planned enrollment number, both a quantity and a range must not be specified for the same study design population or study cohort.</t>
+  </si>
+  <si>
+    <t>CHK0289</t>
+  </si>
+  <si>
+    <t>For planned completion number, both a quantity and a range must not be specified for the same study design population or study cohort.</t>
+  </si>
+  <si>
+    <t>CHK0290</t>
+  </si>
+  <si>
+    <t>CHK0291</t>
+  </si>
+  <si>
+    <t>CHK0292</t>
+  </si>
+  <si>
+    <t>An eligibility criterion item must not be used more than once within a study design.</t>
+  </si>
+  <si>
+    <t>EligibilityCriterionItem</t>
+  </si>
+  <si>
+    <r>
+      <t>If</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF0000FF"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>a</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF0000FF"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>strength</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF0000FF"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>denominator</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF0000FF"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>is</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF0000FF"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>specified,</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF0000FF"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>it</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF0000FF"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>must</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF0000FF"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>have</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> a unit.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>A</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>unit</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>must</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>be</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>specified</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>for</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>every</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>strength</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>denominator</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>and</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>numerator</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -51601,21 +52113,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="5">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="3">
     <dxf>
       <fill>
         <patternFill>
@@ -51966,12 +52464,1403 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5F073237-C241-4A12-AF73-84AEF043C739}">
+  <sheetPr codeName="Sheet9"/>
+  <dimension ref="A1:O29"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="2" max="2" width="62.36328125" customWidth="1"/>
+    <col min="3" max="3" width="14.36328125" customWidth="1"/>
+    <col min="4" max="4" width="30.1796875" style="1" customWidth="1"/>
+    <col min="5" max="5" width="31.54296875" style="1" customWidth="1"/>
+    <col min="8" max="8" width="12.08984375" customWidth="1"/>
+    <col min="9" max="9" width="11.36328125" customWidth="1"/>
+    <col min="10" max="10" width="41.08984375" style="1" customWidth="1"/>
+    <col min="12" max="12" width="47.6328125" style="1" customWidth="1"/>
+    <col min="13" max="13" width="19.81640625" style="1" customWidth="1"/>
+    <col min="14" max="15" width="9.54296875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:15" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A1" s="8" t="s">
+        <v>394</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>344</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>345</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>346</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>347</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>348</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>349</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>350</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>531</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>406</v>
+      </c>
+      <c r="K1" s="8" t="s">
+        <v>240</v>
+      </c>
+      <c r="L1" s="5" t="s">
+        <v>343</v>
+      </c>
+      <c r="M1" s="5" t="s">
+        <v>241</v>
+      </c>
+      <c r="N1" s="7" t="s">
+        <v>532</v>
+      </c>
+      <c r="O1" s="7" t="s">
+        <v>533</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" ht="58" x14ac:dyDescent="0.35">
+      <c r="A2" s="7" t="s">
+        <v>254</v>
+      </c>
+      <c r="B2" s="16" t="s">
+        <v>76</v>
+      </c>
+      <c r="C2" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>1134</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="F2" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="G2" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="H2" s="11" t="s">
+        <v>286</v>
+      </c>
+      <c r="I2" t="s">
+        <v>75</v>
+      </c>
+      <c r="J2" s="13" t="s">
+        <v>98</v>
+      </c>
+      <c r="K2" t="s">
+        <v>98</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>1135</v>
+      </c>
+      <c r="M2" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="N2" t="s">
+        <v>98</v>
+      </c>
+      <c r="O2" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" ht="29" x14ac:dyDescent="0.35">
+      <c r="A3" s="7" t="s">
+        <v>254</v>
+      </c>
+      <c r="B3" s="16" t="s">
+        <v>1136</v>
+      </c>
+      <c r="C3" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="F3" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="G3" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="H3" s="11" t="s">
+        <v>1137</v>
+      </c>
+      <c r="I3" t="s">
+        <v>79</v>
+      </c>
+      <c r="J3" s="13" t="s">
+        <v>98</v>
+      </c>
+      <c r="K3" t="s">
+        <v>98</v>
+      </c>
+      <c r="L3" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="M3" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="N3" t="s">
+        <v>98</v>
+      </c>
+      <c r="O3" t="s">
+        <v>534</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" ht="29" x14ac:dyDescent="0.35">
+      <c r="A4" s="7" t="s">
+        <v>254</v>
+      </c>
+      <c r="B4" s="16" t="s">
+        <v>298</v>
+      </c>
+      <c r="C4" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>469</v>
+      </c>
+      <c r="F4" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="G4" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="H4" s="11" t="s">
+        <v>470</v>
+      </c>
+      <c r="I4" t="s">
+        <v>299</v>
+      </c>
+      <c r="J4" s="13" t="s">
+        <v>98</v>
+      </c>
+      <c r="K4" t="s">
+        <v>98</v>
+      </c>
+      <c r="L4" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="M4" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="N4" t="s">
+        <v>98</v>
+      </c>
+      <c r="O4" t="s">
+        <v>534</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" ht="29" x14ac:dyDescent="0.35">
+      <c r="A5" s="7" t="s">
+        <v>254</v>
+      </c>
+      <c r="B5" s="16" t="s">
+        <v>1138</v>
+      </c>
+      <c r="C5" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="F5" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="G5" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="H5" s="11" t="s">
+        <v>616</v>
+      </c>
+      <c r="I5" t="s">
+        <v>301</v>
+      </c>
+      <c r="J5" s="13" t="s">
+        <v>98</v>
+      </c>
+      <c r="K5" t="s">
+        <v>98</v>
+      </c>
+      <c r="L5" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="M5" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="N5" t="s">
+        <v>98</v>
+      </c>
+      <c r="O5" t="s">
+        <v>534</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" ht="29" x14ac:dyDescent="0.35">
+      <c r="A6" s="7" t="s">
+        <v>254</v>
+      </c>
+      <c r="B6" s="16" t="s">
+        <v>1139</v>
+      </c>
+      <c r="C6" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>204</v>
+      </c>
+      <c r="F6" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="G6" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="H6" s="11" t="s">
+        <v>1140</v>
+      </c>
+      <c r="I6" t="s">
+        <v>203</v>
+      </c>
+      <c r="J6" s="13" t="s">
+        <v>98</v>
+      </c>
+      <c r="K6" t="s">
+        <v>98</v>
+      </c>
+      <c r="L6" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="M6" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="N6" t="s">
+        <v>98</v>
+      </c>
+      <c r="O6" t="s">
+        <v>534</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" ht="29" x14ac:dyDescent="0.35">
+      <c r="A7" s="7" t="s">
+        <v>254</v>
+      </c>
+      <c r="B7" s="16" t="s">
+        <v>1141</v>
+      </c>
+      <c r="C7" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>206</v>
+      </c>
+      <c r="F7" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="G7" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="H7" s="11" t="s">
+        <v>1142</v>
+      </c>
+      <c r="I7" t="s">
+        <v>205</v>
+      </c>
+      <c r="J7" s="13" t="s">
+        <v>98</v>
+      </c>
+      <c r="K7" t="s">
+        <v>98</v>
+      </c>
+      <c r="L7" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="M7" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="N7" t="s">
+        <v>98</v>
+      </c>
+      <c r="O7" t="s">
+        <v>534</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A8" s="7" t="s">
+        <v>254</v>
+      </c>
+      <c r="B8" s="16" t="s">
+        <v>379</v>
+      </c>
+      <c r="C8" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="F8" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="G8" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="H8" s="11" t="s">
+        <v>1143</v>
+      </c>
+      <c r="I8" t="s">
+        <v>380</v>
+      </c>
+      <c r="J8" s="13" t="s">
+        <v>98</v>
+      </c>
+      <c r="K8" t="s">
+        <v>98</v>
+      </c>
+      <c r="L8" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="M8" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="N8" t="s">
+        <v>98</v>
+      </c>
+      <c r="O8" t="s">
+        <v>1144</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" ht="29" x14ac:dyDescent="0.35">
+      <c r="A9" s="7" t="s">
+        <v>254</v>
+      </c>
+      <c r="B9" s="16" t="s">
+        <v>1145</v>
+      </c>
+      <c r="C9" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>291</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>296</v>
+      </c>
+      <c r="F9" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="G9" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="H9" s="11" t="s">
+        <v>1080</v>
+      </c>
+      <c r="I9" t="s">
+        <v>448</v>
+      </c>
+      <c r="J9" s="13" t="s">
+        <v>98</v>
+      </c>
+      <c r="K9" t="s">
+        <v>98</v>
+      </c>
+      <c r="L9" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="M9" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="N9" t="s">
+        <v>98</v>
+      </c>
+      <c r="O9" t="s">
+        <v>534</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A10" s="7" t="s">
+        <v>254</v>
+      </c>
+      <c r="B10" s="16" t="s">
+        <v>1036</v>
+      </c>
+      <c r="C10" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>450</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="F10" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="G10" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="H10" s="11" t="s">
+        <v>1037</v>
+      </c>
+      <c r="I10" t="s">
+        <v>451</v>
+      </c>
+      <c r="J10" s="13" t="s">
+        <v>98</v>
+      </c>
+      <c r="K10" t="s">
+        <v>98</v>
+      </c>
+      <c r="L10" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="M10" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="N10" t="s">
+        <v>98</v>
+      </c>
+      <c r="O10" t="s">
+        <v>534</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A11" s="7" t="s">
+        <v>254</v>
+      </c>
+      <c r="B11" s="15" t="s">
+        <v>1184</v>
+      </c>
+      <c r="C11" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>456</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>1146</v>
+      </c>
+      <c r="F11" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="G11" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="H11" s="11" t="s">
+        <v>98</v>
+      </c>
+      <c r="I11" t="s">
+        <v>458</v>
+      </c>
+      <c r="J11" s="14" t="s">
+        <v>1185</v>
+      </c>
+      <c r="K11" t="s">
+        <v>98</v>
+      </c>
+      <c r="L11" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="M11" s="1" t="s">
+        <v>1147</v>
+      </c>
+      <c r="N11" t="s">
+        <v>98</v>
+      </c>
+      <c r="O11" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" ht="29" x14ac:dyDescent="0.35">
+      <c r="A12" s="7" t="s">
+        <v>254</v>
+      </c>
+      <c r="B12" s="16" t="s">
+        <v>505</v>
+      </c>
+      <c r="C12" s="11" t="s">
+        <v>74</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="F12" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="G12" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="H12" s="11" t="s">
+        <v>1148</v>
+      </c>
+      <c r="I12" t="s">
+        <v>506</v>
+      </c>
+      <c r="J12" s="13" t="s">
+        <v>98</v>
+      </c>
+      <c r="K12" t="s">
+        <v>98</v>
+      </c>
+      <c r="L12" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="M12" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="N12" t="s">
+        <v>98</v>
+      </c>
+      <c r="O12" t="s">
+        <v>534</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A13" s="7" t="s">
+        <v>254</v>
+      </c>
+      <c r="B13" s="16" t="s">
+        <v>573</v>
+      </c>
+      <c r="C13" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>487</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>1149</v>
+      </c>
+      <c r="F13" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="G13" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="H13" s="11" t="s">
+        <v>98</v>
+      </c>
+      <c r="I13" t="s">
+        <v>572</v>
+      </c>
+      <c r="J13" s="13" t="s">
+        <v>98</v>
+      </c>
+      <c r="K13" t="s">
+        <v>98</v>
+      </c>
+      <c r="L13" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="M13" s="1" t="s">
+        <v>1150</v>
+      </c>
+      <c r="N13" t="s">
+        <v>98</v>
+      </c>
+      <c r="O13" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A14" s="7" t="s">
+        <v>253</v>
+      </c>
+      <c r="B14" s="16" t="s">
+        <v>1036</v>
+      </c>
+      <c r="C14" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="E14" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="F14" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="G14" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="H14" s="11" t="s">
+        <v>98</v>
+      </c>
+      <c r="I14" t="s">
+        <v>1151</v>
+      </c>
+      <c r="J14" s="13" t="s">
+        <v>98</v>
+      </c>
+      <c r="K14" t="s">
+        <v>98</v>
+      </c>
+      <c r="L14" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="M14" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="N14" t="s">
+        <v>98</v>
+      </c>
+      <c r="O14" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" ht="29" x14ac:dyDescent="0.35">
+      <c r="A15" s="7" t="s">
+        <v>253</v>
+      </c>
+      <c r="B15" s="16" t="s">
+        <v>1153</v>
+      </c>
+      <c r="C15" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E15" s="3" t="s">
+        <v>1154</v>
+      </c>
+      <c r="F15" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="G15" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="H15" s="11" t="s">
+        <v>98</v>
+      </c>
+      <c r="I15" t="s">
+        <v>1152</v>
+      </c>
+      <c r="J15" s="13" t="s">
+        <v>98</v>
+      </c>
+      <c r="K15" t="s">
+        <v>98</v>
+      </c>
+      <c r="L15" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="M15" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="N15" t="s">
+        <v>98</v>
+      </c>
+      <c r="O15" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" ht="29" x14ac:dyDescent="0.35">
+      <c r="A16" s="7" t="s">
+        <v>253</v>
+      </c>
+      <c r="B16" s="16" t="s">
+        <v>1139</v>
+      </c>
+      <c r="C16" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E16" s="3" t="s">
+        <v>1156</v>
+      </c>
+      <c r="F16" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="G16" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="H16" s="11" t="s">
+        <v>98</v>
+      </c>
+      <c r="I16" t="s">
+        <v>1155</v>
+      </c>
+      <c r="J16" s="13" t="s">
+        <v>98</v>
+      </c>
+      <c r="K16" t="s">
+        <v>98</v>
+      </c>
+      <c r="L16" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="M16" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="N16" t="s">
+        <v>98</v>
+      </c>
+      <c r="O16" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15" ht="29" x14ac:dyDescent="0.35">
+      <c r="A17" s="7" t="s">
+        <v>253</v>
+      </c>
+      <c r="B17" s="16" t="s">
+        <v>1141</v>
+      </c>
+      <c r="C17" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E17" s="3" t="s">
+        <v>1158</v>
+      </c>
+      <c r="F17" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="G17" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="H17" s="11" t="s">
+        <v>98</v>
+      </c>
+      <c r="I17" t="s">
+        <v>1157</v>
+      </c>
+      <c r="J17" s="13" t="s">
+        <v>98</v>
+      </c>
+      <c r="K17" t="s">
+        <v>98</v>
+      </c>
+      <c r="L17" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="M17" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="N17" t="s">
+        <v>98</v>
+      </c>
+      <c r="O17" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15" ht="29" x14ac:dyDescent="0.35">
+      <c r="A18" s="7" t="s">
+        <v>253</v>
+      </c>
+      <c r="B18" s="16" t="s">
+        <v>1138</v>
+      </c>
+      <c r="C18" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="D18" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E18" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="F18" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="G18" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="H18" s="11" t="s">
+        <v>98</v>
+      </c>
+      <c r="I18" t="s">
+        <v>1159</v>
+      </c>
+      <c r="J18" s="13" t="s">
+        <v>98</v>
+      </c>
+      <c r="K18" t="s">
+        <v>98</v>
+      </c>
+      <c r="L18" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="M18" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="N18" t="s">
+        <v>98</v>
+      </c>
+      <c r="O18" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A19" s="7" t="s">
+        <v>253</v>
+      </c>
+      <c r="B19" s="16" t="s">
+        <v>1161</v>
+      </c>
+      <c r="C19" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="D19" s="3" t="s">
+        <v>456</v>
+      </c>
+      <c r="E19" s="3" t="s">
+        <v>1162</v>
+      </c>
+      <c r="F19" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="G19" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="H19" s="11" t="s">
+        <v>98</v>
+      </c>
+      <c r="I19" t="s">
+        <v>1160</v>
+      </c>
+      <c r="J19" s="13" t="s">
+        <v>98</v>
+      </c>
+      <c r="K19" t="s">
+        <v>98</v>
+      </c>
+      <c r="L19" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="M19" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="N19" t="s">
+        <v>98</v>
+      </c>
+      <c r="O19" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15" ht="29" x14ac:dyDescent="0.35">
+      <c r="A20" s="7" t="s">
+        <v>253</v>
+      </c>
+      <c r="B20" s="16" t="s">
+        <v>1164</v>
+      </c>
+      <c r="C20" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="D20" s="3" t="s">
+        <v>456</v>
+      </c>
+      <c r="E20" s="3" t="s">
+        <v>1165</v>
+      </c>
+      <c r="F20" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="G20" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="H20" s="11" t="s">
+        <v>98</v>
+      </c>
+      <c r="I20" t="s">
+        <v>1163</v>
+      </c>
+      <c r="J20" s="13" t="s">
+        <v>98</v>
+      </c>
+      <c r="K20" t="s">
+        <v>98</v>
+      </c>
+      <c r="L20" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="M20" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="N20" t="s">
+        <v>98</v>
+      </c>
+      <c r="O20" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A21" s="7" t="s">
+        <v>253</v>
+      </c>
+      <c r="B21" s="16" t="s">
+        <v>1167</v>
+      </c>
+      <c r="C21" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="D21" s="3" t="s">
+        <v>456</v>
+      </c>
+      <c r="E21" s="3" t="s">
+        <v>1168</v>
+      </c>
+      <c r="F21" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="G21" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="H21" s="11" t="s">
+        <v>98</v>
+      </c>
+      <c r="I21" t="s">
+        <v>1166</v>
+      </c>
+      <c r="J21" s="13" t="s">
+        <v>98</v>
+      </c>
+      <c r="K21" t="s">
+        <v>98</v>
+      </c>
+      <c r="L21" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="M21" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="N21" t="s">
+        <v>98</v>
+      </c>
+      <c r="O21" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="22" spans="1:15" ht="29" x14ac:dyDescent="0.35">
+      <c r="A22" s="7" t="s">
+        <v>253</v>
+      </c>
+      <c r="B22" s="16" t="s">
+        <v>1170</v>
+      </c>
+      <c r="C22" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="D22" s="3" t="s">
+        <v>291</v>
+      </c>
+      <c r="E22" s="3" t="s">
+        <v>296</v>
+      </c>
+      <c r="F22" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="G22" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="H22" s="11" t="s">
+        <v>98</v>
+      </c>
+      <c r="I22" t="s">
+        <v>1169</v>
+      </c>
+      <c r="J22" s="13" t="s">
+        <v>98</v>
+      </c>
+      <c r="K22" t="s">
+        <v>98</v>
+      </c>
+      <c r="L22" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="M22" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="N22" t="s">
+        <v>98</v>
+      </c>
+      <c r="O22" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="23" spans="1:15" ht="29" x14ac:dyDescent="0.35">
+      <c r="A23" s="7" t="s">
+        <v>253</v>
+      </c>
+      <c r="B23" s="16" t="s">
+        <v>1172</v>
+      </c>
+      <c r="C23" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="D23" s="3" t="s">
+        <v>291</v>
+      </c>
+      <c r="E23" s="3" t="s">
+        <v>296</v>
+      </c>
+      <c r="F23" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="G23" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="H23" s="11" t="s">
+        <v>98</v>
+      </c>
+      <c r="I23" t="s">
+        <v>1171</v>
+      </c>
+      <c r="J23" s="13" t="s">
+        <v>98</v>
+      </c>
+      <c r="K23" t="s">
+        <v>98</v>
+      </c>
+      <c r="L23" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="M23" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="N23" t="s">
+        <v>98</v>
+      </c>
+      <c r="O23" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="24" spans="1:15" ht="29" x14ac:dyDescent="0.35">
+      <c r="A24" s="7" t="s">
+        <v>253</v>
+      </c>
+      <c r="B24" s="16" t="s">
+        <v>1174</v>
+      </c>
+      <c r="C24" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="D24" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E24" s="3" t="s">
+        <v>1156</v>
+      </c>
+      <c r="F24" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="G24" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="H24" s="11" t="s">
+        <v>98</v>
+      </c>
+      <c r="I24" t="s">
+        <v>1173</v>
+      </c>
+      <c r="J24" s="13" t="s">
+        <v>98</v>
+      </c>
+      <c r="K24" t="s">
+        <v>98</v>
+      </c>
+      <c r="L24" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="M24" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="N24" t="s">
+        <v>98</v>
+      </c>
+      <c r="O24" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="25" spans="1:15" ht="29" x14ac:dyDescent="0.35">
+      <c r="A25" s="7" t="s">
+        <v>253</v>
+      </c>
+      <c r="B25" s="16" t="s">
+        <v>1176</v>
+      </c>
+      <c r="C25" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="D25" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E25" s="3" t="s">
+        <v>1154</v>
+      </c>
+      <c r="F25" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="G25" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="H25" s="11" t="s">
+        <v>98</v>
+      </c>
+      <c r="I25" t="s">
+        <v>1175</v>
+      </c>
+      <c r="J25" s="13" t="s">
+        <v>98</v>
+      </c>
+      <c r="K25" t="s">
+        <v>98</v>
+      </c>
+      <c r="L25" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="M25" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="N25" t="s">
+        <v>98</v>
+      </c>
+      <c r="O25" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="26" spans="1:15" ht="29" x14ac:dyDescent="0.35">
+      <c r="A26" s="7" t="s">
+        <v>253</v>
+      </c>
+      <c r="B26" s="16" t="s">
+        <v>1178</v>
+      </c>
+      <c r="C26" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="D26" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E26" s="3" t="s">
+        <v>1156</v>
+      </c>
+      <c r="F26" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="G26" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="H26" s="11" t="s">
+        <v>98</v>
+      </c>
+      <c r="I26" t="s">
+        <v>1177</v>
+      </c>
+      <c r="J26" s="13" t="s">
+        <v>98</v>
+      </c>
+      <c r="K26" t="s">
+        <v>98</v>
+      </c>
+      <c r="L26" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="M26" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="N26" t="s">
+        <v>98</v>
+      </c>
+      <c r="O26" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="27" spans="1:15" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A27" s="7" t="s">
+        <v>253</v>
+      </c>
+      <c r="B27" s="16" t="s">
+        <v>1136</v>
+      </c>
+      <c r="C27" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="D27" s="3" t="s">
+        <v>1134</v>
+      </c>
+      <c r="E27" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="F27" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="G27" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="H27" s="11" t="s">
+        <v>98</v>
+      </c>
+      <c r="I27" t="s">
+        <v>1179</v>
+      </c>
+      <c r="J27" s="13" t="s">
+        <v>98</v>
+      </c>
+      <c r="K27" t="s">
+        <v>98</v>
+      </c>
+      <c r="L27" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="M27" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="N27" t="s">
+        <v>98</v>
+      </c>
+      <c r="O27" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="28" spans="1:15" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A28" s="7" t="s">
+        <v>253</v>
+      </c>
+      <c r="B28" s="16" t="s">
+        <v>505</v>
+      </c>
+      <c r="C28" s="11" t="s">
+        <v>74</v>
+      </c>
+      <c r="D28" s="3" t="s">
+        <v>1134</v>
+      </c>
+      <c r="E28" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="F28" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="G28" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="H28" s="11" t="s">
+        <v>98</v>
+      </c>
+      <c r="I28" t="s">
+        <v>1180</v>
+      </c>
+      <c r="J28" s="13" t="s">
+        <v>98</v>
+      </c>
+      <c r="K28" t="s">
+        <v>98</v>
+      </c>
+      <c r="L28" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="M28" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="N28" t="s">
+        <v>98</v>
+      </c>
+      <c r="O28" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="29" spans="1:15" ht="29" x14ac:dyDescent="0.35">
+      <c r="A29" s="7" t="s">
+        <v>253</v>
+      </c>
+      <c r="B29" s="16" t="s">
+        <v>1182</v>
+      </c>
+      <c r="C29" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="D29" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="E29" s="3" t="s">
+        <v>1183</v>
+      </c>
+      <c r="F29" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="G29" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="H29" s="11" t="s">
+        <v>98</v>
+      </c>
+      <c r="I29" t="s">
+        <v>1181</v>
+      </c>
+      <c r="J29" s="13" t="s">
+        <v>98</v>
+      </c>
+      <c r="K29" t="s">
+        <v>98</v>
+      </c>
+      <c r="L29" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="M29" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="N29" t="s">
+        <v>98</v>
+      </c>
+      <c r="O29" t="s">
+        <v>98</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DA56E3A9-6AF6-4F10-BAF1-2E2148AC6531}">
   <sheetPr codeName="Sheet8"/>
   <dimension ref="A1:P36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K5" sqref="K5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -53794,7 +55683,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B2:B36">
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="notEqual">
+    <cfRule type="cellIs" dxfId="2" priority="1" operator="notEqual">
       <formula>""</formula>
     </cfRule>
   </conditionalFormatting>
@@ -53802,7 +55691,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{04922479-DC74-45C1-A6FB-8A5685DCA4C3}">
   <sheetPr codeName="Sheet7"/>
   <dimension ref="A1:Q49"/>
@@ -56317,7 +58206,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B2:B49">
-    <cfRule type="cellIs" dxfId="3" priority="1" operator="notEqual">
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="notEqual">
       <formula>""</formula>
     </cfRule>
   </conditionalFormatting>
@@ -56325,7 +58214,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8EF31D4B-F1B8-4E5E-A34A-AF6E16EC4595}">
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:P13"/>
@@ -57002,7 +58891,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B2:B13">
-    <cfRule type="cellIs" dxfId="2" priority="1" operator="notEqual">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="notEqual">
       <formula>""</formula>
     </cfRule>
   </conditionalFormatting>
@@ -57010,7 +58899,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{067B8281-AB10-416A-8A55-B2F46EB8E8FB}">
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:O7"/>
@@ -57365,7 +59254,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A424D0F2-3B88-4770-93C0-98D49DE8D516}">
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:O104"/>
@@ -62285,7 +64174,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B456D714-2DB6-4B8B-BC8E-8AA7501F8C79}">
   <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:O7"/>
@@ -62637,7 +64526,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E53E83C4-68F7-4929-AA83-3F95502173FC}">
   <sheetPr codeName="Sheet5"/>
   <dimension ref="A1:O195"/>
@@ -64493,7 +66382,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2720FBDC-F538-4F79-9784-827E5ACB3995}">
   <sheetPr codeName="Sheet6"/>
   <dimension ref="A1:P130"/>

</xml_diff>

<commit_message>
changes acc to ticket #587
</commit_message>
<xml_diff>
--- a/Deliverables/RULES/USDM_CORE_Rules_Changes.xlsx
+++ b/Deliverables/RULES/USDM_CORE_Rules_Changes.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Stack\CL027\Publish\CORE\3.11\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Stack\CL027\Publish\CORE\3.11b\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{2B9777CA-54F9-4760-99D4-FF84EB69137A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{B11B03E9-4984-41F5-9D2A-EC10426EF327}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-165" yWindow="-19080" windowWidth="23295" windowHeight="18015" xr2:uid="{418CF395-400B-43AB-9594-6DFC1F089218}"/>
+    <workbookView xWindow="2400" yWindow="-19740" windowWidth="24375" windowHeight="15915" xr2:uid="{418CF395-400B-43AB-9594-6DFC1F089218}"/>
   </bookViews>
   <sheets>
     <sheet name="Changes release 3.10 -&gt; 3.11" sheetId="13" r:id="rId1"/>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6061" uniqueCount="1186">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="355" uniqueCount="1201">
   <si>
     <t>All</t>
   </si>
@@ -51607,11 +51607,252 @@
   </si>
   <si>
     <r>
+      <t>A</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>unit</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>must</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>be</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>specified</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>for</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>every</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>strength</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>denominator</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>and</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>numerator</t>
+    </r>
+  </si>
+  <si>
+    <t>A study element must only reference study interventions that are defined within the same study design as the study element.</t>
+  </si>
+  <si>
+    <t>DDF00109</t>
+  </si>
+  <si>
+    <t>CHK0293</t>
+  </si>
+  <si>
+    <t>An eligibility criterion item is expected to be used in at least one study design.</t>
+  </si>
+  <si>
+    <t>CHK0294</t>
+  </si>
+  <si>
+    <t>An eligibility criterion must be referenced by either a study design population or cohorts, not both.</t>
+  </si>
+  <si>
+    <t>CHK0295</t>
+  </si>
+  <si>
+    <t>A study cohort must only reference indications that are  defined within the same study design.</t>
+  </si>
+  <si>
+    <t>StudyCohort</t>
+  </si>
+  <si>
+    <t>indications</t>
+  </si>
+  <si>
+    <t>CHK0296</t>
+  </si>
+  <si>
+    <t>A study element must only reference study interventions that are referenced by the same study design as the study element.</t>
+  </si>
+  <si>
+    <t>CHK0297</t>
+  </si>
+  <si>
+    <t>CHK0298</t>
+  </si>
+  <si>
+    <t>An activity must only reference child activities that are specified within the same study design.</t>
+  </si>
+  <si>
+    <r>
       <t>If</t>
     </r>
     <r>
       <rPr>
         <sz val="11"/>
+        <color theme="1"/>
         <rFont val="Aptos Narrow"/>
         <family val="2"/>
         <scheme val="minor"/>
@@ -51631,6 +51872,7 @@
     <r>
       <rPr>
         <sz val="11"/>
+        <color theme="1"/>
         <rFont val="Aptos Narrow"/>
         <family val="2"/>
         <scheme val="minor"/>
@@ -51650,6 +51892,7 @@
     <r>
       <rPr>
         <sz val="11"/>
+        <color theme="1"/>
         <rFont val="Aptos Narrow"/>
         <family val="2"/>
         <scheme val="minor"/>
@@ -51669,6 +51912,7 @@
     <r>
       <rPr>
         <sz val="11"/>
+        <color theme="1"/>
         <rFont val="Aptos Narrow"/>
         <family val="2"/>
         <scheme val="minor"/>
@@ -51688,6 +51932,7 @@
     <r>
       <rPr>
         <sz val="11"/>
+        <color theme="1"/>
         <rFont val="Aptos Narrow"/>
         <family val="2"/>
         <scheme val="minor"/>
@@ -51707,6 +51952,7 @@
     <r>
       <rPr>
         <sz val="11"/>
+        <color theme="1"/>
         <rFont val="Aptos Narrow"/>
         <family val="2"/>
         <scheme val="minor"/>
@@ -51726,6 +51972,7 @@
     <r>
       <rPr>
         <sz val="11"/>
+        <color theme="1"/>
         <rFont val="Aptos Narrow"/>
         <family val="2"/>
         <scheme val="minor"/>
@@ -51745,6 +51992,7 @@
     <r>
       <rPr>
         <sz val="11"/>
+        <color theme="1"/>
         <rFont val="Aptos Narrow"/>
         <family val="2"/>
         <scheme val="minor"/>
@@ -51764,206 +52012,12 @@
     <r>
       <rPr>
         <sz val="11"/>
+        <color theme="1"/>
         <rFont val="Aptos Narrow"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve"> a unit.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>A</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>unit</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>must</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>be</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>specified</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>for</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>every</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>strength</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>denominator</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>and</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>numerator</t>
     </r>
   </si>
 </sst>
@@ -52466,23 +52520,25 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5F073237-C241-4A12-AF73-84AEF043C739}">
   <sheetPr codeName="Sheet9"/>
-  <dimension ref="A1:O29"/>
+  <dimension ref="A1:O36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="62.36328125" customWidth="1"/>
-    <col min="3" max="3" width="14.36328125" customWidth="1"/>
-    <col min="4" max="4" width="30.1796875" style="1" customWidth="1"/>
-    <col min="5" max="5" width="31.54296875" style="1" customWidth="1"/>
-    <col min="8" max="8" width="12.08984375" customWidth="1"/>
-    <col min="9" max="9" width="11.36328125" customWidth="1"/>
-    <col min="10" max="10" width="41.08984375" style="1" customWidth="1"/>
-    <col min="12" max="12" width="47.6328125" style="1" customWidth="1"/>
-    <col min="13" max="13" width="19.81640625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="9.7265625" customWidth="1"/>
+    <col min="2" max="2" width="71.453125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="13.453125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="24.26953125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="26" style="1" customWidth="1"/>
+    <col min="6" max="7" width="10.36328125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.6328125" style="1" customWidth="1"/>
+    <col min="10" max="10" width="47.6328125" style="1" customWidth="1"/>
+    <col min="11" max="11" width="12.7265625" style="1" customWidth="1"/>
+    <col min="12" max="12" width="27.54296875" style="1" customWidth="1"/>
+    <col min="13" max="13" width="17.1796875" style="1" customWidth="1"/>
     <col min="14" max="15" width="9.54296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -52502,10 +52558,10 @@
       <c r="E1" s="2" t="s">
         <v>347</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="8" t="s">
         <v>348</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G1" s="8" t="s">
         <v>349</v>
       </c>
       <c r="H1" s="2" t="s">
@@ -52520,24 +52576,24 @@
       <c r="K1" s="8" t="s">
         <v>240</v>
       </c>
-      <c r="L1" s="5" t="s">
+      <c r="L1" s="2" t="s">
         <v>343</v>
       </c>
-      <c r="M1" s="5" t="s">
+      <c r="M1" s="2" t="s">
         <v>241</v>
       </c>
-      <c r="N1" s="7" t="s">
+      <c r="N1" s="8" t="s">
         <v>532</v>
       </c>
-      <c r="O1" s="7" t="s">
+      <c r="O1" s="8" t="s">
         <v>533</v>
       </c>
     </row>
-    <row r="2" spans="1:15" ht="58" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:15" ht="87" x14ac:dyDescent="0.35">
       <c r="A2" s="7" t="s">
         <v>254</v>
       </c>
-      <c r="B2" s="16" t="s">
+      <c r="B2" s="3" t="s">
         <v>76</v>
       </c>
       <c r="C2" s="11" t="s">
@@ -52580,11 +52636,11 @@
         <v>98</v>
       </c>
     </row>
-    <row r="3" spans="1:15" ht="29" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:15" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A3" s="7" t="s">
         <v>254</v>
       </c>
-      <c r="B3" s="16" t="s">
+      <c r="B3" s="3" t="s">
         <v>1136</v>
       </c>
       <c r="C3" s="11" t="s">
@@ -52631,17 +52687,17 @@
       <c r="A4" s="7" t="s">
         <v>254</v>
       </c>
-      <c r="B4" s="16" t="s">
-        <v>298</v>
+      <c r="B4" s="3" t="s">
+        <v>1185</v>
       </c>
       <c r="C4" s="11" t="s">
         <v>1</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>6</v>
+        <v>131</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>469</v>
+        <v>132</v>
       </c>
       <c r="F4" s="11" t="s">
         <v>2</v>
@@ -52650,10 +52706,10 @@
         <v>8</v>
       </c>
       <c r="H4" s="11" t="s">
-        <v>470</v>
+        <v>1186</v>
       </c>
       <c r="I4" t="s">
-        <v>299</v>
+        <v>130</v>
       </c>
       <c r="J4" s="13" t="s">
         <v>98</v>
@@ -52678,8 +52734,8 @@
       <c r="A5" s="7" t="s">
         <v>254</v>
       </c>
-      <c r="B5" s="16" t="s">
-        <v>1138</v>
+      <c r="B5" s="3" t="s">
+        <v>298</v>
       </c>
       <c r="C5" s="11" t="s">
         <v>1</v>
@@ -52688,7 +52744,7 @@
         <v>6</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>28</v>
+        <v>469</v>
       </c>
       <c r="F5" s="11" t="s">
         <v>2</v>
@@ -52697,10 +52753,10 @@
         <v>8</v>
       </c>
       <c r="H5" s="11" t="s">
-        <v>616</v>
+        <v>470</v>
       </c>
       <c r="I5" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="J5" s="13" t="s">
         <v>98</v>
@@ -52725,8 +52781,8 @@
       <c r="A6" s="7" t="s">
         <v>254</v>
       </c>
-      <c r="B6" s="16" t="s">
-        <v>1139</v>
+      <c r="B6" s="3" t="s">
+        <v>1138</v>
       </c>
       <c r="C6" s="11" t="s">
         <v>1</v>
@@ -52735,7 +52791,7 @@
         <v>6</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>204</v>
+        <v>28</v>
       </c>
       <c r="F6" s="11" t="s">
         <v>2</v>
@@ -52744,10 +52800,10 @@
         <v>8</v>
       </c>
       <c r="H6" s="11" t="s">
-        <v>1140</v>
+        <v>616</v>
       </c>
       <c r="I6" t="s">
-        <v>203</v>
+        <v>301</v>
       </c>
       <c r="J6" s="13" t="s">
         <v>98</v>
@@ -52772,8 +52828,8 @@
       <c r="A7" s="7" t="s">
         <v>254</v>
       </c>
-      <c r="B7" s="16" t="s">
-        <v>1141</v>
+      <c r="B7" s="3" t="s">
+        <v>1139</v>
       </c>
       <c r="C7" s="11" t="s">
         <v>1</v>
@@ -52782,7 +52838,7 @@
         <v>6</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="F7" s="11" t="s">
         <v>2</v>
@@ -52791,10 +52847,10 @@
         <v>8</v>
       </c>
       <c r="H7" s="11" t="s">
-        <v>1142</v>
+        <v>1140</v>
       </c>
       <c r="I7" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="J7" s="13" t="s">
         <v>98</v>
@@ -52815,21 +52871,21 @@
         <v>534</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:15" ht="29" x14ac:dyDescent="0.35">
       <c r="A8" s="7" t="s">
         <v>254</v>
       </c>
-      <c r="B8" s="16" t="s">
-        <v>379</v>
+      <c r="B8" s="3" t="s">
+        <v>1141</v>
       </c>
       <c r="C8" s="11" t="s">
         <v>1</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>65</v>
+        <v>6</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>66</v>
+        <v>206</v>
       </c>
       <c r="F8" s="11" t="s">
         <v>2</v>
@@ -52838,10 +52894,10 @@
         <v>8</v>
       </c>
       <c r="H8" s="11" t="s">
-        <v>1143</v>
+        <v>1142</v>
       </c>
       <c r="I8" t="s">
-        <v>380</v>
+        <v>205</v>
       </c>
       <c r="J8" s="13" t="s">
         <v>98</v>
@@ -52859,24 +52915,24 @@
         <v>98</v>
       </c>
       <c r="O8" t="s">
-        <v>1144</v>
+        <v>534</v>
       </c>
     </row>
-    <row r="9" spans="1:15" ht="29" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A9" s="7" t="s">
         <v>254</v>
       </c>
-      <c r="B9" s="16" t="s">
-        <v>1145</v>
+      <c r="B9" s="3" t="s">
+        <v>379</v>
       </c>
       <c r="C9" s="11" t="s">
         <v>1</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>291</v>
+        <v>65</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>296</v>
+        <v>66</v>
       </c>
       <c r="F9" s="11" t="s">
         <v>2</v>
@@ -52885,10 +52941,10 @@
         <v>8</v>
       </c>
       <c r="H9" s="11" t="s">
-        <v>1080</v>
+        <v>1143</v>
       </c>
       <c r="I9" t="s">
-        <v>448</v>
+        <v>380</v>
       </c>
       <c r="J9" s="13" t="s">
         <v>98</v>
@@ -52906,24 +52962,24 @@
         <v>98</v>
       </c>
       <c r="O9" t="s">
-        <v>534</v>
+        <v>1144</v>
       </c>
     </row>
-    <row r="10" spans="1:15" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:15" ht="29" x14ac:dyDescent="0.35">
       <c r="A10" s="7" t="s">
         <v>254</v>
       </c>
-      <c r="B10" s="16" t="s">
-        <v>1036</v>
+      <c r="B10" s="3" t="s">
+        <v>1145</v>
       </c>
       <c r="C10" s="11" t="s">
         <v>1</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>450</v>
+        <v>291</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>32</v>
+        <v>296</v>
       </c>
       <c r="F10" s="11" t="s">
         <v>2</v>
@@ -52932,10 +52988,10 @@
         <v>8</v>
       </c>
       <c r="H10" s="11" t="s">
-        <v>1037</v>
+        <v>1080</v>
       </c>
       <c r="I10" t="s">
-        <v>451</v>
+        <v>448</v>
       </c>
       <c r="J10" s="13" t="s">
         <v>98</v>
@@ -52960,32 +53016,32 @@
       <c r="A11" s="7" t="s">
         <v>254</v>
       </c>
-      <c r="B11" s="15" t="s">
-        <v>1184</v>
+      <c r="B11" s="3" t="s">
+        <v>1036</v>
       </c>
       <c r="C11" s="11" t="s">
         <v>1</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>456</v>
+        <v>450</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>1146</v>
+        <v>32</v>
       </c>
       <c r="F11" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="G11" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="G11" s="11" t="s">
-        <v>2</v>
-      </c>
       <c r="H11" s="11" t="s">
-        <v>98</v>
+        <v>1037</v>
       </c>
       <c r="I11" t="s">
-        <v>458</v>
-      </c>
-      <c r="J11" s="14" t="s">
-        <v>1185</v>
+        <v>451</v>
+      </c>
+      <c r="J11" s="13" t="s">
+        <v>98</v>
       </c>
       <c r="K11" t="s">
         <v>98</v>
@@ -52994,45 +53050,45 @@
         <v>98</v>
       </c>
       <c r="M11" s="1" t="s">
-        <v>1147</v>
+        <v>98</v>
       </c>
       <c r="N11" t="s">
         <v>98</v>
       </c>
       <c r="O11" t="s">
-        <v>98</v>
+        <v>534</v>
       </c>
     </row>
-    <row r="12" spans="1:15" ht="29" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:15" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A12" s="7" t="s">
         <v>254</v>
       </c>
-      <c r="B12" s="16" t="s">
-        <v>505</v>
+      <c r="B12" s="15" t="s">
+        <v>1200</v>
       </c>
       <c r="C12" s="11" t="s">
-        <v>74</v>
+        <v>1</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>77</v>
+        <v>456</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>78</v>
+        <v>1146</v>
       </c>
       <c r="F12" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="G12" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="G12" s="11" t="s">
-        <v>8</v>
-      </c>
       <c r="H12" s="11" t="s">
-        <v>1148</v>
+        <v>98</v>
       </c>
       <c r="I12" t="s">
-        <v>506</v>
-      </c>
-      <c r="J12" s="13" t="s">
-        <v>98</v>
+        <v>458</v>
+      </c>
+      <c r="J12" s="14" t="s">
+        <v>1184</v>
       </c>
       <c r="K12" t="s">
         <v>98</v>
@@ -53041,77 +53097,77 @@
         <v>98</v>
       </c>
       <c r="M12" s="1" t="s">
-        <v>98</v>
+        <v>1147</v>
       </c>
       <c r="N12" t="s">
         <v>98</v>
       </c>
       <c r="O12" t="s">
-        <v>534</v>
+        <v>98</v>
       </c>
     </row>
     <row r="13" spans="1:15" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A13" s="7" t="s">
         <v>254</v>
       </c>
-      <c r="B13" s="16" t="s">
+      <c r="B13" s="3" t="s">
+        <v>505</v>
+      </c>
+      <c r="C13" s="11" t="s">
+        <v>74</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="F13" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="G13" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="H13" s="11" t="s">
+        <v>1148</v>
+      </c>
+      <c r="I13" t="s">
+        <v>506</v>
+      </c>
+      <c r="J13" s="13" t="s">
+        <v>98</v>
+      </c>
+      <c r="K13" t="s">
+        <v>98</v>
+      </c>
+      <c r="L13" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="M13" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="N13" t="s">
+        <v>98</v>
+      </c>
+      <c r="O13" t="s">
+        <v>534</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="A14" s="7" t="s">
+        <v>254</v>
+      </c>
+      <c r="B14" s="3" t="s">
         <v>573</v>
-      </c>
-      <c r="C13" s="11" t="s">
-        <v>1</v>
-      </c>
-      <c r="D13" s="3" t="s">
-        <v>487</v>
-      </c>
-      <c r="E13" s="3" t="s">
-        <v>1149</v>
-      </c>
-      <c r="F13" s="11" t="s">
-        <v>8</v>
-      </c>
-      <c r="G13" s="11" t="s">
-        <v>2</v>
-      </c>
-      <c r="H13" s="11" t="s">
-        <v>98</v>
-      </c>
-      <c r="I13" t="s">
-        <v>572</v>
-      </c>
-      <c r="J13" s="13" t="s">
-        <v>98</v>
-      </c>
-      <c r="K13" t="s">
-        <v>98</v>
-      </c>
-      <c r="L13" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="M13" s="1" t="s">
-        <v>1150</v>
-      </c>
-      <c r="N13" t="s">
-        <v>98</v>
-      </c>
-      <c r="O13" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="14" spans="1:15" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A14" s="7" t="s">
-        <v>253</v>
-      </c>
-      <c r="B14" s="16" t="s">
-        <v>1036</v>
       </c>
       <c r="C14" s="11" t="s">
         <v>1</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>31</v>
+        <v>487</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>32</v>
+        <v>1149</v>
       </c>
       <c r="F14" s="11" t="s">
         <v>8</v>
@@ -53123,7 +53179,7 @@
         <v>98</v>
       </c>
       <c r="I14" t="s">
-        <v>1151</v>
+        <v>572</v>
       </c>
       <c r="J14" s="13" t="s">
         <v>98</v>
@@ -53135,7 +53191,7 @@
         <v>98</v>
       </c>
       <c r="M14" s="1" t="s">
-        <v>98</v>
+        <v>1150</v>
       </c>
       <c r="N14" t="s">
         <v>98</v>
@@ -53144,21 +53200,21 @@
         <v>98</v>
       </c>
     </row>
-    <row r="15" spans="1:15" ht="29" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:15" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A15" s="7" t="s">
         <v>253</v>
       </c>
-      <c r="B15" s="16" t="s">
-        <v>1153</v>
+      <c r="B15" s="3" t="s">
+        <v>1036</v>
       </c>
       <c r="C15" s="11" t="s">
         <v>1</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>6</v>
+        <v>31</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>1154</v>
+        <v>32</v>
       </c>
       <c r="F15" s="11" t="s">
         <v>8</v>
@@ -53170,7 +53226,7 @@
         <v>98</v>
       </c>
       <c r="I15" t="s">
-        <v>1152</v>
+        <v>1151</v>
       </c>
       <c r="J15" s="13" t="s">
         <v>98</v>
@@ -53191,12 +53247,12 @@
         <v>98</v>
       </c>
     </row>
-    <row r="16" spans="1:15" ht="29" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:15" ht="58" x14ac:dyDescent="0.35">
       <c r="A16" s="7" t="s">
         <v>253</v>
       </c>
-      <c r="B16" s="16" t="s">
-        <v>1139</v>
+      <c r="B16" s="3" t="s">
+        <v>1153</v>
       </c>
       <c r="C16" s="11" t="s">
         <v>1</v>
@@ -53205,7 +53261,7 @@
         <v>6</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>1156</v>
+        <v>1154</v>
       </c>
       <c r="F16" s="11" t="s">
         <v>8</v>
@@ -53217,7 +53273,7 @@
         <v>98</v>
       </c>
       <c r="I16" t="s">
-        <v>1155</v>
+        <v>1152</v>
       </c>
       <c r="J16" s="13" t="s">
         <v>98</v>
@@ -53238,12 +53294,12 @@
         <v>98</v>
       </c>
     </row>
-    <row r="17" spans="1:15" ht="29" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:15" ht="58" x14ac:dyDescent="0.35">
       <c r="A17" s="7" t="s">
         <v>253</v>
       </c>
-      <c r="B17" s="16" t="s">
-        <v>1141</v>
+      <c r="B17" s="3" t="s">
+        <v>1139</v>
       </c>
       <c r="C17" s="11" t="s">
         <v>1</v>
@@ -53252,7 +53308,7 @@
         <v>6</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>1158</v>
+        <v>1156</v>
       </c>
       <c r="F17" s="11" t="s">
         <v>8</v>
@@ -53264,7 +53320,7 @@
         <v>98</v>
       </c>
       <c r="I17" t="s">
-        <v>1157</v>
+        <v>1155</v>
       </c>
       <c r="J17" s="13" t="s">
         <v>98</v>
@@ -53285,12 +53341,12 @@
         <v>98</v>
       </c>
     </row>
-    <row r="18" spans="1:15" ht="29" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:15" ht="58" x14ac:dyDescent="0.35">
       <c r="A18" s="7" t="s">
         <v>253</v>
       </c>
-      <c r="B18" s="16" t="s">
-        <v>1138</v>
+      <c r="B18" s="3" t="s">
+        <v>1141</v>
       </c>
       <c r="C18" s="11" t="s">
         <v>1</v>
@@ -53299,7 +53355,7 @@
         <v>6</v>
       </c>
       <c r="E18" s="3" t="s">
-        <v>28</v>
+        <v>1158</v>
       </c>
       <c r="F18" s="11" t="s">
         <v>8</v>
@@ -53311,7 +53367,7 @@
         <v>98</v>
       </c>
       <c r="I18" t="s">
-        <v>1159</v>
+        <v>1157</v>
       </c>
       <c r="J18" s="13" t="s">
         <v>98</v>
@@ -53332,21 +53388,21 @@
         <v>98</v>
       </c>
     </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:15" ht="29" x14ac:dyDescent="0.35">
       <c r="A19" s="7" t="s">
         <v>253</v>
       </c>
-      <c r="B19" s="16" t="s">
-        <v>1161</v>
+      <c r="B19" s="3" t="s">
+        <v>1138</v>
       </c>
       <c r="C19" s="11" t="s">
         <v>1</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>456</v>
+        <v>6</v>
       </c>
       <c r="E19" s="3" t="s">
-        <v>1162</v>
+        <v>28</v>
       </c>
       <c r="F19" s="11" t="s">
         <v>8</v>
@@ -53358,7 +53414,7 @@
         <v>98</v>
       </c>
       <c r="I19" t="s">
-        <v>1160</v>
+        <v>1159</v>
       </c>
       <c r="J19" s="13" t="s">
         <v>98</v>
@@ -53379,12 +53435,12 @@
         <v>98</v>
       </c>
     </row>
-    <row r="20" spans="1:15" ht="29" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A20" s="7" t="s">
         <v>253</v>
       </c>
-      <c r="B20" s="16" t="s">
-        <v>1164</v>
+      <c r="B20" s="3" t="s">
+        <v>1161</v>
       </c>
       <c r="C20" s="11" t="s">
         <v>1</v>
@@ -53393,7 +53449,7 @@
         <v>456</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>1165</v>
+        <v>1162</v>
       </c>
       <c r="F20" s="11" t="s">
         <v>8</v>
@@ -53405,7 +53461,7 @@
         <v>98</v>
       </c>
       <c r="I20" t="s">
-        <v>1163</v>
+        <v>1160</v>
       </c>
       <c r="J20" s="13" t="s">
         <v>98</v>
@@ -53426,12 +53482,12 @@
         <v>98</v>
       </c>
     </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:15" ht="29" x14ac:dyDescent="0.35">
       <c r="A21" s="7" t="s">
         <v>253</v>
       </c>
-      <c r="B21" s="16" t="s">
-        <v>1167</v>
+      <c r="B21" s="3" t="s">
+        <v>1164</v>
       </c>
       <c r="C21" s="11" t="s">
         <v>1</v>
@@ -53440,7 +53496,7 @@
         <v>456</v>
       </c>
       <c r="E21" s="3" t="s">
-        <v>1168</v>
+        <v>1165</v>
       </c>
       <c r="F21" s="11" t="s">
         <v>8</v>
@@ -53452,7 +53508,7 @@
         <v>98</v>
       </c>
       <c r="I21" t="s">
-        <v>1166</v>
+        <v>1163</v>
       </c>
       <c r="J21" s="13" t="s">
         <v>98</v>
@@ -53477,17 +53533,17 @@
       <c r="A22" s="7" t="s">
         <v>253</v>
       </c>
-      <c r="B22" s="16" t="s">
-        <v>1170</v>
+      <c r="B22" s="3" t="s">
+        <v>1167</v>
       </c>
       <c r="C22" s="11" t="s">
         <v>1</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>291</v>
+        <v>456</v>
       </c>
       <c r="E22" s="3" t="s">
-        <v>296</v>
+        <v>1168</v>
       </c>
       <c r="F22" s="11" t="s">
         <v>8</v>
@@ -53499,7 +53555,7 @@
         <v>98</v>
       </c>
       <c r="I22" t="s">
-        <v>1169</v>
+        <v>1166</v>
       </c>
       <c r="J22" s="13" t="s">
         <v>98</v>
@@ -53524,8 +53580,8 @@
       <c r="A23" s="7" t="s">
         <v>253</v>
       </c>
-      <c r="B23" s="16" t="s">
-        <v>1172</v>
+      <c r="B23" s="3" t="s">
+        <v>1170</v>
       </c>
       <c r="C23" s="11" t="s">
         <v>1</v>
@@ -53546,7 +53602,7 @@
         <v>98</v>
       </c>
       <c r="I23" t="s">
-        <v>1171</v>
+        <v>1169</v>
       </c>
       <c r="J23" s="13" t="s">
         <v>98</v>
@@ -53571,17 +53627,17 @@
       <c r="A24" s="7" t="s">
         <v>253</v>
       </c>
-      <c r="B24" s="16" t="s">
-        <v>1174</v>
+      <c r="B24" s="3" t="s">
+        <v>1172</v>
       </c>
       <c r="C24" s="11" t="s">
         <v>1</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>6</v>
+        <v>291</v>
       </c>
       <c r="E24" s="3" t="s">
-        <v>1156</v>
+        <v>296</v>
       </c>
       <c r="F24" s="11" t="s">
         <v>8</v>
@@ -53593,7 +53649,7 @@
         <v>98</v>
       </c>
       <c r="I24" t="s">
-        <v>1173</v>
+        <v>1171</v>
       </c>
       <c r="J24" s="13" t="s">
         <v>98</v>
@@ -53614,12 +53670,12 @@
         <v>98</v>
       </c>
     </row>
-    <row r="25" spans="1:15" ht="29" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:15" ht="58" x14ac:dyDescent="0.35">
       <c r="A25" s="7" t="s">
         <v>253</v>
       </c>
-      <c r="B25" s="16" t="s">
-        <v>1176</v>
+      <c r="B25" s="3" t="s">
+        <v>1174</v>
       </c>
       <c r="C25" s="11" t="s">
         <v>1</v>
@@ -53628,7 +53684,7 @@
         <v>6</v>
       </c>
       <c r="E25" s="3" t="s">
-        <v>1154</v>
+        <v>1156</v>
       </c>
       <c r="F25" s="11" t="s">
         <v>8</v>
@@ -53640,7 +53696,7 @@
         <v>98</v>
       </c>
       <c r="I25" t="s">
-        <v>1175</v>
+        <v>1173</v>
       </c>
       <c r="J25" s="13" t="s">
         <v>98</v>
@@ -53661,12 +53717,12 @@
         <v>98</v>
       </c>
     </row>
-    <row r="26" spans="1:15" ht="29" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:15" ht="58" x14ac:dyDescent="0.35">
       <c r="A26" s="7" t="s">
         <v>253</v>
       </c>
-      <c r="B26" s="16" t="s">
-        <v>1178</v>
+      <c r="B26" s="3" t="s">
+        <v>1176</v>
       </c>
       <c r="C26" s="11" t="s">
         <v>1</v>
@@ -53675,7 +53731,7 @@
         <v>6</v>
       </c>
       <c r="E26" s="3" t="s">
-        <v>1156</v>
+        <v>1154</v>
       </c>
       <c r="F26" s="11" t="s">
         <v>8</v>
@@ -53687,7 +53743,7 @@
         <v>98</v>
       </c>
       <c r="I26" t="s">
-        <v>1177</v>
+        <v>1175</v>
       </c>
       <c r="J26" s="13" t="s">
         <v>98</v>
@@ -53708,21 +53764,21 @@
         <v>98</v>
       </c>
     </row>
-    <row r="27" spans="1:15" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:15" ht="58" x14ac:dyDescent="0.35">
       <c r="A27" s="7" t="s">
         <v>253</v>
       </c>
-      <c r="B27" s="16" t="s">
-        <v>1136</v>
+      <c r="B27" s="3" t="s">
+        <v>1178</v>
       </c>
       <c r="C27" s="11" t="s">
         <v>1</v>
       </c>
       <c r="D27" s="3" t="s">
-        <v>1134</v>
+        <v>6</v>
       </c>
       <c r="E27" s="3" t="s">
-        <v>78</v>
+        <v>1156</v>
       </c>
       <c r="F27" s="11" t="s">
         <v>8</v>
@@ -53734,7 +53790,7 @@
         <v>98</v>
       </c>
       <c r="I27" t="s">
-        <v>1179</v>
+        <v>1177</v>
       </c>
       <c r="J27" s="13" t="s">
         <v>98</v>
@@ -53759,11 +53815,11 @@
       <c r="A28" s="7" t="s">
         <v>253</v>
       </c>
-      <c r="B28" s="16" t="s">
-        <v>505</v>
+      <c r="B28" s="3" t="s">
+        <v>1136</v>
       </c>
       <c r="C28" s="11" t="s">
-        <v>74</v>
+        <v>1</v>
       </c>
       <c r="D28" s="3" t="s">
         <v>1134</v>
@@ -53781,7 +53837,7 @@
         <v>98</v>
       </c>
       <c r="I28" t="s">
-        <v>1180</v>
+        <v>1179</v>
       </c>
       <c r="J28" s="13" t="s">
         <v>98</v>
@@ -53802,21 +53858,21 @@
         <v>98</v>
       </c>
     </row>
-    <row r="29" spans="1:15" ht="29" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:15" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A29" s="7" t="s">
         <v>253</v>
       </c>
-      <c r="B29" s="16" t="s">
-        <v>1182</v>
+      <c r="B29" s="3" t="s">
+        <v>505</v>
       </c>
       <c r="C29" s="11" t="s">
-        <v>1</v>
+        <v>74</v>
       </c>
       <c r="D29" s="3" t="s">
-        <v>112</v>
+        <v>1134</v>
       </c>
       <c r="E29" s="3" t="s">
-        <v>1183</v>
+        <v>78</v>
       </c>
       <c r="F29" s="11" t="s">
         <v>8</v>
@@ -53828,24 +53884,353 @@
         <v>98</v>
       </c>
       <c r="I29" t="s">
+        <v>1180</v>
+      </c>
+      <c r="J29" s="13" t="s">
+        <v>98</v>
+      </c>
+      <c r="K29" t="s">
+        <v>98</v>
+      </c>
+      <c r="L29" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="M29" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="N29" t="s">
+        <v>98</v>
+      </c>
+      <c r="O29" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="30" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A30" s="7" t="s">
+        <v>253</v>
+      </c>
+      <c r="B30" s="3" t="s">
+        <v>1182</v>
+      </c>
+      <c r="C30" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="D30" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="E30" s="3" t="s">
+        <v>1183</v>
+      </c>
+      <c r="F30" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="G30" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="H30" s="11" t="s">
+        <v>98</v>
+      </c>
+      <c r="I30" t="s">
         <v>1181</v>
       </c>
-      <c r="J29" s="13" t="s">
-        <v>98</v>
-      </c>
-      <c r="K29" t="s">
-        <v>98</v>
-      </c>
-      <c r="L29" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="M29" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="N29" t="s">
-        <v>98</v>
-      </c>
-      <c r="O29" t="s">
+      <c r="J30" s="13" t="s">
+        <v>98</v>
+      </c>
+      <c r="K30" t="s">
+        <v>98</v>
+      </c>
+      <c r="L30" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="M30" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="N30" t="s">
+        <v>98</v>
+      </c>
+      <c r="O30" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="31" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A31" s="7" t="s">
+        <v>253</v>
+      </c>
+      <c r="B31" s="3" t="s">
+        <v>1188</v>
+      </c>
+      <c r="C31" s="11" t="s">
+        <v>74</v>
+      </c>
+      <c r="D31" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="E31" s="3" t="s">
+        <v>1183</v>
+      </c>
+      <c r="F31" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="G31" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="H31" s="11" t="s">
+        <v>98</v>
+      </c>
+      <c r="I31" t="s">
+        <v>1187</v>
+      </c>
+      <c r="J31" s="13" t="s">
+        <v>98</v>
+      </c>
+      <c r="K31" t="s">
+        <v>98</v>
+      </c>
+      <c r="L31" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="M31" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="N31" t="s">
+        <v>98</v>
+      </c>
+      <c r="O31" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="32" spans="1:15" ht="29" x14ac:dyDescent="0.35">
+      <c r="A32" s="7" t="s">
+        <v>253</v>
+      </c>
+      <c r="B32" s="3" t="s">
+        <v>1190</v>
+      </c>
+      <c r="C32" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="D32" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E32" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="F32" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="G32" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="H32" s="11" t="s">
+        <v>98</v>
+      </c>
+      <c r="I32" t="s">
+        <v>1189</v>
+      </c>
+      <c r="J32" s="13" t="s">
+        <v>98</v>
+      </c>
+      <c r="K32" t="s">
+        <v>98</v>
+      </c>
+      <c r="L32" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="M32" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="N32" t="s">
+        <v>98</v>
+      </c>
+      <c r="O32" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="33" spans="1:15" ht="29" x14ac:dyDescent="0.35">
+      <c r="A33" s="7" t="s">
+        <v>253</v>
+      </c>
+      <c r="B33" s="3" t="s">
+        <v>1192</v>
+      </c>
+      <c r="C33" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="D33" s="3" t="s">
+        <v>1193</v>
+      </c>
+      <c r="E33" s="3" t="s">
+        <v>1194</v>
+      </c>
+      <c r="F33" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="G33" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="H33" s="11" t="s">
+        <v>98</v>
+      </c>
+      <c r="I33" t="s">
+        <v>1191</v>
+      </c>
+      <c r="J33" s="13" t="s">
+        <v>98</v>
+      </c>
+      <c r="K33" t="s">
+        <v>98</v>
+      </c>
+      <c r="L33" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="M33" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="N33" t="s">
+        <v>98</v>
+      </c>
+      <c r="O33" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="34" spans="1:15" ht="29" x14ac:dyDescent="0.35">
+      <c r="A34" s="7" t="s">
+        <v>253</v>
+      </c>
+      <c r="B34" s="3" t="s">
+        <v>1196</v>
+      </c>
+      <c r="C34" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="D34" s="3" t="s">
+        <v>131</v>
+      </c>
+      <c r="E34" s="3" t="s">
+        <v>132</v>
+      </c>
+      <c r="F34" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="G34" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="H34" s="11" t="s">
+        <v>98</v>
+      </c>
+      <c r="I34" t="s">
+        <v>1195</v>
+      </c>
+      <c r="J34" s="13" t="s">
+        <v>98</v>
+      </c>
+      <c r="K34" t="s">
+        <v>98</v>
+      </c>
+      <c r="L34" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="M34" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="N34" t="s">
+        <v>98</v>
+      </c>
+      <c r="O34" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="35" spans="1:15" ht="29" x14ac:dyDescent="0.35">
+      <c r="A35" s="7" t="s">
+        <v>253</v>
+      </c>
+      <c r="B35" s="3" t="s">
+        <v>1061</v>
+      </c>
+      <c r="C35" s="11" t="s">
+        <v>74</v>
+      </c>
+      <c r="D35" s="3" t="s">
+        <v>153</v>
+      </c>
+      <c r="E35" s="3" t="s">
+        <v>132</v>
+      </c>
+      <c r="F35" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="G35" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="H35" s="11" t="s">
+        <v>98</v>
+      </c>
+      <c r="I35" t="s">
+        <v>1197</v>
+      </c>
+      <c r="J35" s="13" t="s">
+        <v>98</v>
+      </c>
+      <c r="K35" t="s">
+        <v>98</v>
+      </c>
+      <c r="L35" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="M35" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="N35" t="s">
+        <v>98</v>
+      </c>
+      <c r="O35" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="36" spans="1:15" ht="29" x14ac:dyDescent="0.35">
+      <c r="A36" s="7" t="s">
+        <v>253</v>
+      </c>
+      <c r="B36" s="3" t="s">
+        <v>1199</v>
+      </c>
+      <c r="C36" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="D36" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="E36" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="F36" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="G36" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="H36" s="11" t="s">
+        <v>98</v>
+      </c>
+      <c r="I36" t="s">
+        <v>1198</v>
+      </c>
+      <c r="J36" s="13" t="s">
+        <v>98</v>
+      </c>
+      <c r="K36" t="s">
+        <v>98</v>
+      </c>
+      <c r="L36" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="M36" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="N36" t="s">
+        <v>98</v>
+      </c>
+      <c r="O36" t="s">
         <v>98</v>
       </c>
     </row>
@@ -53860,7 +54245,7 @@
   <dimension ref="A1:P36"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="K3" sqref="K3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -53915,19 +54300,19 @@
       <c r="K1" s="2" t="s">
         <v>406</v>
       </c>
-      <c r="L1" s="8" t="s">
+      <c r="L1" s="2" t="s">
         <v>240</v>
       </c>
-      <c r="M1" s="5" t="s">
+      <c r="M1" s="2" t="s">
         <v>343</v>
       </c>
-      <c r="N1" s="7" t="s">
+      <c r="N1" s="2" t="s">
         <v>241</v>
       </c>
-      <c r="O1" s="7" t="s">
+      <c r="O1" s="8" t="s">
         <v>532</v>
       </c>
-      <c r="P1" s="7" t="s">
+      <c r="P1" s="8" t="s">
         <v>533</v>
       </c>
     </row>
@@ -55696,7 +56081,7 @@
   <sheetPr codeName="Sheet7"/>
   <dimension ref="A1:Q49"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="C1" workbookViewId="0">
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
reviewed version 4 optional rules and updated accordingly
</commit_message>
<xml_diff>
--- a/Deliverables/RULES/USDM_CORE_Rules_Changes.xlsx
+++ b/Deliverables/RULES/USDM_CORE_Rules_Changes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Stack\CL027\Publish\CORE\3.11b\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{FE94A9BB-5110-4B7A-822A-57812D9E0826}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68E89AF2-9EE9-4512-A3A4-F07939E72E8E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-8820" yWindow="-20565" windowWidth="20070" windowHeight="18600" xr2:uid="{418CF395-400B-43AB-9594-6DFC1F089218}"/>
+    <workbookView xWindow="-13560" yWindow="-21720" windowWidth="51840" windowHeight="21120" xr2:uid="{418CF395-400B-43AB-9594-6DFC1F089218}"/>
   </bookViews>
   <sheets>
     <sheet name="Changes release 3.10 -&gt; 3.11" sheetId="13" r:id="rId1"/>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6226" uniqueCount="1208">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6319" uniqueCount="1209">
   <si>
     <t>All</t>
   </si>
@@ -51456,12 +51456,6 @@
     <t>CHK0276</t>
   </si>
   <si>
-    <t>EligibilityCriterionItem, Characteristic, Condition, Objective, Endpoint</t>
-  </si>
-  <si>
-    <t>EligibilityCriterion, Characteristic, Condition, Objective, Endpoint=&gt;EligibilityCriterionItem, Characteristic, Condition, Objective, Endpoint</t>
-  </si>
-  <si>
     <t>Any parameter name referenced in a tag in the text should be specified in the data dictionary parameter maps.</t>
   </si>
   <si>
@@ -51606,201 +51600,6 @@
     <t>EligibilityCriterionItem</t>
   </si>
   <si>
-    <r>
-      <t>A</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>unit</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>must</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>be</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>specified</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>for</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>every</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>strength</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>denominator</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>and</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>numerator</t>
-    </r>
-  </si>
-  <si>
     <t>A study element must only reference study interventions that are defined within the same study design as the study element.</t>
   </si>
   <si>
@@ -51846,181 +51645,6 @@
     <t>An activity must only reference child activities that are specified within the same study design.</t>
   </si>
   <si>
-    <r>
-      <t>If</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF0000FF"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>a</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF0000FF"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>strength</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF0000FF"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>denominator</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF0000FF"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>is</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF0000FF"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>specified,</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF0000FF"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>it</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF0000FF"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>must</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF0000FF"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>have</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> a unit.</t>
-    </r>
-  </si>
-  <si>
     <t>If the reason for a study amendment is 'Other' then this must be specified (attribute reasonOther must be completed)</t>
   </si>
   <si>
@@ -52040,6 +51664,21 @@
   </si>
   <si>
     <t>The same reason is not expected to be given as a primary and secondary reason.</t>
+  </si>
+  <si>
+    <t>Within a study design, there must be at least 1 eligibility criterion that is referenced by either a study population or a cohort.</t>
+  </si>
+  <si>
+    <t>When included in text, references to items stored elsewhere in the data model must be specified in the correct format. They must start with '&lt;usdm:ref', end with either '/&gt;' or '&gt;&lt;/usdm:ref&gt;', and must contain 'klass="klassName"',  'id="idValue"', and 'attribute="attributeName"/&gt;' in any order (where "klassName" and "attributeName" contain only letters in upper or lower case).</t>
+  </si>
+  <si>
+    <t>For a specified range at least a minimum or maximum value is expected.</t>
+  </si>
+  <si>
+    <t>If a strength denominator is specified, it must have a unit.</t>
+  </si>
+  <si>
+    <t>EligibilityCriterionItem, Characteristic, Condition, Objective, Endpoint, IntercurrentEvent</t>
   </si>
 </sst>
 </file>
@@ -52097,7 +51736,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -52133,11 +51772,33 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -52184,6 +51845,15 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -52541,27 +52211,28 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5F073237-C241-4A12-AF73-84AEF043C739}">
   <sheetPr codeName="Sheet9"/>
-  <dimension ref="A1:O40"/>
+  <dimension ref="A1:O47"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="L8" sqref="L8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="58.85546875" style="1" customWidth="1"/>
-    <col min="3" max="3" width="26" style="1" customWidth="1"/>
-    <col min="4" max="4" width="28.85546875" style="1" customWidth="1"/>
-    <col min="5" max="5" width="27.7109375" style="1" customWidth="1"/>
-    <col min="6" max="6" width="8.42578125" style="1" customWidth="1"/>
-    <col min="7" max="7" width="7.85546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="47.5703125" style="1" customWidth="1"/>
-    <col min="9" max="9" width="12.7109375" style="1" customWidth="1"/>
-    <col min="10" max="10" width="35.85546875" style="1" customWidth="1"/>
-    <col min="11" max="11" width="17.140625" style="1" customWidth="1"/>
-    <col min="12" max="12" width="34.42578125" style="1" customWidth="1"/>
-    <col min="13" max="13" width="29.5703125" customWidth="1"/>
+    <col min="1" max="1" width="9.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="55.85546875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="9.42578125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="31.140625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="31" style="1" customWidth="1"/>
+    <col min="6" max="6" width="7.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.42578125" style="1" customWidth="1"/>
+    <col min="8" max="8" width="12.7109375" style="1" customWidth="1"/>
+    <col min="9" max="9" width="9.5703125" style="1" customWidth="1"/>
+    <col min="10" max="10" width="39.5703125" style="22" customWidth="1"/>
+    <col min="11" max="11" width="16.7109375" style="1" customWidth="1"/>
+    <col min="12" max="12" width="30.140625" style="22" customWidth="1"/>
+    <col min="13" max="13" width="27.7109375" style="1" customWidth="1"/>
+    <col min="14" max="15" width="9.140625" style="22"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="45" x14ac:dyDescent="0.25">
@@ -52589,19 +52260,19 @@
       <c r="H1" s="2" t="s">
         <v>350</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="I1" s="9" t="s">
         <v>531</v>
       </c>
       <c r="J1" s="2" t="s">
         <v>406</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="K1" s="20" t="s">
         <v>240</v>
       </c>
       <c r="L1" s="2" t="s">
         <v>343</v>
       </c>
-      <c r="M1" s="2" t="s">
+      <c r="M1" s="20" t="s">
         <v>241</v>
       </c>
       <c r="N1" s="2" t="s">
@@ -52611,108 +52282,104 @@
         <v>533</v>
       </c>
     </row>
-    <row r="2" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" ht="45" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>1201</v>
-      </c>
-      <c r="C2" s="11" t="s">
+        <v>1204</v>
+      </c>
+      <c r="C2" s="3" t="s">
         <v>1</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>45</v>
+        <v>6</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>313</v>
-      </c>
-      <c r="F2" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="F2" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="G2" s="11" t="s">
-        <v>2</v>
+      <c r="G2" s="3" t="s">
+        <v>9</v>
       </c>
       <c r="H2" s="11" t="s">
-        <v>314</v>
+        <v>98</v>
       </c>
       <c r="I2" t="s">
-        <v>44</v>
-      </c>
-      <c r="J2" s="13" t="s">
-        <v>98</v>
-      </c>
-      <c r="K2" t="s">
-        <v>98</v>
-      </c>
-      <c r="L2" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="M2" t="s">
-        <v>98</v>
-      </c>
-      <c r="N2" t="s">
-        <v>98</v>
-      </c>
-      <c r="O2" t="s">
-        <v>554</v>
+        <v>5</v>
+      </c>
+      <c r="J2" s="21"/>
+      <c r="K2" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="L2" s="22" t="s">
+        <v>98</v>
+      </c>
+      <c r="M2" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="N2" s="22" t="s">
+        <v>98</v>
+      </c>
+      <c r="O2" s="22" t="s">
+        <v>98</v>
       </c>
     </row>
-    <row r="3" spans="1:15" ht="75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
         <v>254</v>
       </c>
       <c r="B3" s="3" t="s">
+        <v>1197</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>313</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="H3" s="11" t="s">
+        <v>314</v>
+      </c>
+      <c r="I3" t="s">
+        <v>44</v>
+      </c>
+      <c r="J3" s="21"/>
+      <c r="K3" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="L3" s="22" t="s">
+        <v>98</v>
+      </c>
+      <c r="M3" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="N3" s="22" t="s">
+        <v>98</v>
+      </c>
+      <c r="O3" s="22" t="s">
+        <v>554</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" ht="75" x14ac:dyDescent="0.25">
+      <c r="A4" s="7" t="s">
+        <v>255</v>
+      </c>
+      <c r="B4" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="C3" s="11" t="s">
-        <v>1</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>1134</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="F3" s="11" t="s">
-        <v>8</v>
-      </c>
-      <c r="G3" s="11" t="s">
-        <v>9</v>
-      </c>
-      <c r="H3" s="11" t="s">
-        <v>286</v>
-      </c>
-      <c r="I3" t="s">
-        <v>75</v>
-      </c>
-      <c r="J3" s="13" t="s">
-        <v>98</v>
-      </c>
-      <c r="K3" t="s">
-        <v>98</v>
-      </c>
-      <c r="L3" s="1" t="s">
-        <v>1135</v>
-      </c>
-      <c r="M3" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="N3" t="s">
-        <v>98</v>
-      </c>
-      <c r="O3" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="4" spans="1:15" ht="45" x14ac:dyDescent="0.25">
-      <c r="A4" s="7" t="s">
-        <v>254</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>1136</v>
-      </c>
-      <c r="C4" s="11" t="s">
+      <c r="C4" s="3" t="s">
         <v>1</v>
       </c>
       <c r="D4" s="3" t="s">
@@ -52721,35 +52388,32 @@
       <c r="E4" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="F4" s="11" t="s">
-        <v>2</v>
-      </c>
-      <c r="G4" s="11" t="s">
+      <c r="F4" s="3" t="s">
         <v>8</v>
       </c>
+      <c r="G4" s="3" t="s">
+        <v>9</v>
+      </c>
       <c r="H4" s="11" t="s">
-        <v>1137</v>
+        <v>98</v>
       </c>
       <c r="I4" t="s">
-        <v>79</v>
-      </c>
-      <c r="J4" s="13" t="s">
-        <v>98</v>
-      </c>
-      <c r="K4" t="s">
-        <v>98</v>
-      </c>
-      <c r="L4" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="K4" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="L4" s="22" t="s">
         <v>98</v>
       </c>
       <c r="M4" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="N4" t="s">
-        <v>98</v>
-      </c>
-      <c r="O4" t="s">
-        <v>534</v>
+      <c r="N4" s="22" t="s">
+        <v>98</v>
+      </c>
+      <c r="O4" s="22" t="s">
+        <v>98</v>
       </c>
     </row>
     <row r="5" spans="1:15" ht="30" x14ac:dyDescent="0.25">
@@ -52757,328 +52421,307 @@
         <v>254</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>1185</v>
-      </c>
-      <c r="C5" s="11" t="s">
+        <v>1134</v>
+      </c>
+      <c r="C5" s="3" t="s">
         <v>1</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>131</v>
+        <v>77</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>132</v>
-      </c>
-      <c r="F5" s="11" t="s">
+        <v>78</v>
+      </c>
+      <c r="F5" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="G5" s="11" t="s">
+      <c r="G5" s="3" t="s">
         <v>8</v>
       </c>
       <c r="H5" s="11" t="s">
-        <v>1186</v>
+        <v>1135</v>
       </c>
       <c r="I5" t="s">
-        <v>130</v>
-      </c>
-      <c r="J5" s="13" t="s">
-        <v>98</v>
-      </c>
-      <c r="K5" t="s">
-        <v>98</v>
-      </c>
-      <c r="L5" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="K5" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="L5" s="22" t="s">
         <v>98</v>
       </c>
       <c r="M5" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="N5" t="s">
-        <v>98</v>
-      </c>
-      <c r="O5" t="s">
+      <c r="N5" s="22" t="s">
+        <v>98</v>
+      </c>
+      <c r="O5" s="22" t="s">
         <v>534</v>
       </c>
     </row>
-    <row r="6" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:15" ht="105" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>1202</v>
-      </c>
-      <c r="C6" s="11" t="s">
-        <v>74</v>
+        <v>1205</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>1</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>318</v>
+        <v>82</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>319</v>
-      </c>
-      <c r="F6" s="11" t="s">
-        <v>2</v>
-      </c>
-      <c r="G6" s="11" t="s">
+        <v>78</v>
+      </c>
+      <c r="F6" s="3" t="s">
         <v>8</v>
       </c>
+      <c r="G6" s="3" t="s">
+        <v>9</v>
+      </c>
       <c r="H6" s="11" t="s">
-        <v>1203</v>
+        <v>98</v>
       </c>
       <c r="I6" t="s">
-        <v>320</v>
-      </c>
-      <c r="J6" s="13" t="s">
-        <v>98</v>
-      </c>
-      <c r="K6" t="s">
-        <v>98</v>
-      </c>
-      <c r="L6" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="M6" t="s">
-        <v>98</v>
-      </c>
-      <c r="N6" t="s">
-        <v>98</v>
-      </c>
-      <c r="O6" t="s">
-        <v>534</v>
+        <v>80</v>
+      </c>
+      <c r="K6" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="L6" s="22" t="s">
+        <v>98</v>
+      </c>
+      <c r="M6" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="N6" s="22" t="s">
+        <v>98</v>
+      </c>
+      <c r="O6" s="22" t="s">
+        <v>98</v>
       </c>
     </row>
     <row r="7" spans="1:15" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>298</v>
-      </c>
-      <c r="C7" s="11" t="s">
-        <v>1</v>
+        <v>493</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>74</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>6</v>
+        <v>86</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>469</v>
-      </c>
-      <c r="F7" s="11" t="s">
-        <v>2</v>
-      </c>
-      <c r="G7" s="11" t="s">
+        <v>87</v>
+      </c>
+      <c r="F7" s="3" t="s">
         <v>8</v>
       </c>
+      <c r="G7" s="3" t="s">
+        <v>9</v>
+      </c>
       <c r="H7" s="11" t="s">
-        <v>470</v>
+        <v>98</v>
       </c>
       <c r="I7" t="s">
-        <v>299</v>
-      </c>
-      <c r="J7" s="13" t="s">
-        <v>98</v>
-      </c>
-      <c r="K7" t="s">
-        <v>98</v>
-      </c>
-      <c r="L7" s="1" t="s">
+        <v>494</v>
+      </c>
+      <c r="K7" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="L7" s="22" t="s">
         <v>98</v>
       </c>
       <c r="M7" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="N7" t="s">
-        <v>98</v>
-      </c>
-      <c r="O7" t="s">
-        <v>534</v>
+      <c r="N7" s="22" t="s">
+        <v>98</v>
+      </c>
+      <c r="O7" s="22" t="s">
+        <v>98</v>
       </c>
     </row>
     <row r="8" spans="1:15" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>1138</v>
-      </c>
-      <c r="C8" s="11" t="s">
-        <v>1</v>
+        <v>498</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>74</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>6</v>
+        <v>86</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="F8" s="11" t="s">
-        <v>2</v>
-      </c>
-      <c r="G8" s="11" t="s">
+        <v>499</v>
+      </c>
+      <c r="F8" s="3" t="s">
         <v>8</v>
       </c>
+      <c r="G8" s="3" t="s">
+        <v>9</v>
+      </c>
       <c r="H8" s="11" t="s">
-        <v>616</v>
+        <v>98</v>
       </c>
       <c r="I8" t="s">
-        <v>301</v>
-      </c>
-      <c r="J8" s="13" t="s">
-        <v>98</v>
-      </c>
-      <c r="K8" t="s">
-        <v>98</v>
-      </c>
-      <c r="L8" s="1" t="s">
+        <v>500</v>
+      </c>
+      <c r="K8" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="L8" s="22" t="s">
         <v>98</v>
       </c>
       <c r="M8" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="N8" t="s">
-        <v>98</v>
-      </c>
-      <c r="O8" t="s">
-        <v>534</v>
+      <c r="N8" s="22" t="s">
+        <v>98</v>
+      </c>
+      <c r="O8" s="22" t="s">
+        <v>98</v>
       </c>
     </row>
-    <row r="9" spans="1:15" ht="45" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:15" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>1139</v>
-      </c>
-      <c r="C9" s="11" t="s">
-        <v>1</v>
+        <v>261</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>74</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>6</v>
+        <v>86</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>204</v>
-      </c>
-      <c r="F9" s="11" t="s">
-        <v>2</v>
-      </c>
-      <c r="G9" s="11" t="s">
+        <v>262</v>
+      </c>
+      <c r="F9" s="3" t="s">
         <v>8</v>
       </c>
+      <c r="G9" s="3" t="s">
+        <v>9</v>
+      </c>
       <c r="H9" s="11" t="s">
-        <v>1140</v>
+        <v>98</v>
       </c>
       <c r="I9" t="s">
-        <v>203</v>
-      </c>
-      <c r="J9" s="13" t="s">
-        <v>98</v>
-      </c>
-      <c r="K9" t="s">
-        <v>98</v>
-      </c>
-      <c r="L9" s="1" t="s">
+        <v>263</v>
+      </c>
+      <c r="K9" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="L9" s="22" t="s">
         <v>98</v>
       </c>
       <c r="M9" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="N9" t="s">
-        <v>98</v>
-      </c>
-      <c r="O9" t="s">
-        <v>534</v>
+      <c r="N9" s="22" t="s">
+        <v>98</v>
+      </c>
+      <c r="O9" s="22" t="s">
+        <v>98</v>
       </c>
     </row>
-    <row r="10" spans="1:15" ht="45" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:15" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>1141</v>
-      </c>
-      <c r="C10" s="11" t="s">
-        <v>1</v>
+        <v>495</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>74</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>6</v>
+        <v>86</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>206</v>
-      </c>
-      <c r="F10" s="11" t="s">
-        <v>2</v>
-      </c>
-      <c r="G10" s="11" t="s">
+        <v>496</v>
+      </c>
+      <c r="F10" s="3" t="s">
         <v>8</v>
       </c>
+      <c r="G10" s="3" t="s">
+        <v>9</v>
+      </c>
       <c r="H10" s="11" t="s">
-        <v>1142</v>
+        <v>98</v>
       </c>
       <c r="I10" t="s">
-        <v>205</v>
-      </c>
-      <c r="J10" s="13" t="s">
-        <v>98</v>
-      </c>
-      <c r="K10" t="s">
-        <v>98</v>
-      </c>
-      <c r="L10" s="1" t="s">
+        <v>497</v>
+      </c>
+      <c r="K10" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="L10" s="22" t="s">
         <v>98</v>
       </c>
       <c r="M10" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="N10" t="s">
-        <v>98</v>
-      </c>
-      <c r="O10" t="s">
-        <v>534</v>
+      <c r="N10" s="22" t="s">
+        <v>98</v>
+      </c>
+      <c r="O10" s="22" t="s">
+        <v>98</v>
       </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:15" ht="45" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
         <v>254</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>379</v>
-      </c>
-      <c r="C11" s="11" t="s">
+        <v>1182</v>
+      </c>
+      <c r="C11" s="3" t="s">
         <v>1</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>65</v>
+        <v>131</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="F11" s="11" t="s">
+        <v>132</v>
+      </c>
+      <c r="F11" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="G11" s="11" t="s">
+      <c r="G11" s="3" t="s">
         <v>8</v>
       </c>
       <c r="H11" s="11" t="s">
-        <v>1143</v>
+        <v>1183</v>
       </c>
       <c r="I11" t="s">
-        <v>380</v>
-      </c>
-      <c r="J11" s="13" t="s">
-        <v>98</v>
-      </c>
-      <c r="K11" t="s">
-        <v>98</v>
-      </c>
-      <c r="L11" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="K11" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="L11" s="22" t="s">
         <v>98</v>
       </c>
       <c r="M11" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="N11" t="s">
-        <v>98</v>
-      </c>
-      <c r="O11" t="s">
-        <v>1144</v>
+      <c r="N11" s="22" t="s">
+        <v>98</v>
+      </c>
+      <c r="O11" s="22" t="s">
+        <v>534</v>
       </c>
     </row>
     <row r="12" spans="1:15" ht="30" x14ac:dyDescent="0.25">
@@ -53086,186 +52729,180 @@
         <v>254</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>1145</v>
-      </c>
-      <c r="C12" s="11" t="s">
-        <v>1</v>
+        <v>1198</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>74</v>
       </c>
       <c r="D12" s="3" t="s">
+        <v>318</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>319</v>
+      </c>
+      <c r="F12" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="G12" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="H12" s="11" t="s">
+        <v>1199</v>
+      </c>
+      <c r="I12" t="s">
+        <v>320</v>
+      </c>
+      <c r="K12" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="L12" s="22" t="s">
+        <v>98</v>
+      </c>
+      <c r="M12" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="N12" s="22" t="s">
+        <v>98</v>
+      </c>
+      <c r="O12" s="22" t="s">
+        <v>534</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+      <c r="A13" s="7" t="s">
+        <v>255</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>1206</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="D13" s="3" t="s">
         <v>291</v>
       </c>
-      <c r="E12" s="3" t="s">
+      <c r="E13" s="3" t="s">
         <v>296</v>
       </c>
-      <c r="F12" s="11" t="s">
-        <v>2</v>
-      </c>
-      <c r="G12" s="11" t="s">
+      <c r="F13" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="H12" s="11" t="s">
-        <v>1080</v>
-      </c>
-      <c r="I12" t="s">
-        <v>448</v>
-      </c>
-      <c r="J12" s="13" t="s">
-        <v>98</v>
-      </c>
-      <c r="K12" t="s">
-        <v>98</v>
-      </c>
-      <c r="L12" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="M12" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="N12" t="s">
-        <v>98</v>
-      </c>
-      <c r="O12" t="s">
-        <v>534</v>
-      </c>
-    </row>
-    <row r="13" spans="1:15" ht="45" x14ac:dyDescent="0.25">
-      <c r="A13" s="7" t="s">
-        <v>254</v>
-      </c>
-      <c r="B13" s="3" t="s">
-        <v>1036</v>
-      </c>
-      <c r="C13" s="11" t="s">
-        <v>1</v>
-      </c>
-      <c r="D13" s="3" t="s">
-        <v>450</v>
-      </c>
-      <c r="E13" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="F13" s="11" t="s">
-        <v>2</v>
-      </c>
-      <c r="G13" s="11" t="s">
-        <v>8</v>
+      <c r="G13" s="3" t="s">
+        <v>9</v>
       </c>
       <c r="H13" s="11" t="s">
-        <v>1037</v>
+        <v>98</v>
       </c>
       <c r="I13" t="s">
-        <v>451</v>
-      </c>
-      <c r="J13" s="13" t="s">
-        <v>98</v>
-      </c>
-      <c r="K13" t="s">
-        <v>98</v>
-      </c>
-      <c r="L13" s="1" t="s">
+        <v>297</v>
+      </c>
+      <c r="K13" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="L13" s="22" t="s">
         <v>98</v>
       </c>
       <c r="M13" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="N13" t="s">
-        <v>98</v>
-      </c>
-      <c r="O13" t="s">
-        <v>534</v>
+      <c r="N13" s="22" t="s">
+        <v>98</v>
+      </c>
+      <c r="O13" s="22" t="s">
+        <v>98</v>
       </c>
     </row>
     <row r="14" spans="1:15" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" s="7" t="s">
         <v>254</v>
       </c>
-      <c r="B14" s="15" t="s">
-        <v>1200</v>
-      </c>
-      <c r="C14" s="11" t="s">
+      <c r="B14" s="3" t="s">
+        <v>298</v>
+      </c>
+      <c r="C14" s="3" t="s">
         <v>1</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>456</v>
+        <v>6</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>1146</v>
-      </c>
-      <c r="F14" s="11" t="s">
+        <v>469</v>
+      </c>
+      <c r="F14" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="G14" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="G14" s="11" t="s">
-        <v>2</v>
-      </c>
       <c r="H14" s="11" t="s">
-        <v>98</v>
+        <v>470</v>
       </c>
       <c r="I14" t="s">
-        <v>458</v>
-      </c>
-      <c r="J14" s="14" t="s">
-        <v>1184</v>
-      </c>
-      <c r="K14" t="s">
-        <v>98</v>
-      </c>
-      <c r="L14" s="1" t="s">
+        <v>299</v>
+      </c>
+      <c r="J14" s="22" t="s">
+        <v>98</v>
+      </c>
+      <c r="K14" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="L14" s="22" t="s">
         <v>98</v>
       </c>
       <c r="M14" s="1" t="s">
-        <v>1147</v>
-      </c>
-      <c r="N14" t="s">
-        <v>98</v>
-      </c>
-      <c r="O14" t="s">
-        <v>98</v>
+        <v>98</v>
+      </c>
+      <c r="N14" s="22" t="s">
+        <v>98</v>
+      </c>
+      <c r="O14" s="22" t="s">
+        <v>534</v>
       </c>
     </row>
-    <row r="15" spans="1:15" ht="45" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:15" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" s="7" t="s">
         <v>254</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>505</v>
-      </c>
-      <c r="C15" s="11" t="s">
-        <v>74</v>
+        <v>1136</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>1</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>77</v>
+        <v>6</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="F15" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="F15" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="G15" s="11" t="s">
+      <c r="G15" s="3" t="s">
         <v>8</v>
       </c>
       <c r="H15" s="11" t="s">
-        <v>1148</v>
+        <v>616</v>
       </c>
       <c r="I15" t="s">
-        <v>506</v>
-      </c>
-      <c r="J15" s="13" t="s">
-        <v>98</v>
-      </c>
-      <c r="K15" t="s">
-        <v>98</v>
-      </c>
-      <c r="L15" s="1" t="s">
+        <v>301</v>
+      </c>
+      <c r="J15" s="22" t="s">
+        <v>98</v>
+      </c>
+      <c r="K15" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="L15" s="22" t="s">
         <v>98</v>
       </c>
       <c r="M15" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="N15" t="s">
-        <v>98</v>
-      </c>
-      <c r="O15" t="s">
+      <c r="N15" s="22" t="s">
+        <v>98</v>
+      </c>
+      <c r="O15" s="22" t="s">
         <v>534</v>
       </c>
     </row>
@@ -53274,515 +52911,515 @@
         <v>254</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>573</v>
-      </c>
-      <c r="C16" s="11" t="s">
+        <v>1137</v>
+      </c>
+      <c r="C16" s="3" t="s">
         <v>1</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>487</v>
+        <v>6</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>1149</v>
-      </c>
-      <c r="F16" s="11" t="s">
+        <v>204</v>
+      </c>
+      <c r="F16" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="G16" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="G16" s="11" t="s">
-        <v>2</v>
-      </c>
       <c r="H16" s="11" t="s">
-        <v>98</v>
+        <v>1138</v>
       </c>
       <c r="I16" t="s">
-        <v>572</v>
-      </c>
-      <c r="J16" s="13" t="s">
-        <v>98</v>
-      </c>
-      <c r="K16" t="s">
-        <v>98</v>
-      </c>
-      <c r="L16" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="J16" s="22" t="s">
+        <v>98</v>
+      </c>
+      <c r="K16" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="L16" s="22" t="s">
         <v>98</v>
       </c>
       <c r="M16" s="1" t="s">
-        <v>1150</v>
-      </c>
-      <c r="N16" t="s">
-        <v>98</v>
-      </c>
-      <c r="O16" t="s">
-        <v>98</v>
+        <v>98</v>
+      </c>
+      <c r="N16" s="22" t="s">
+        <v>98</v>
+      </c>
+      <c r="O16" s="22" t="s">
+        <v>534</v>
       </c>
     </row>
     <row r="17" spans="1:15" ht="45" x14ac:dyDescent="0.25">
       <c r="A17" s="7" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>1036</v>
-      </c>
-      <c r="C17" s="11" t="s">
+        <v>1139</v>
+      </c>
+      <c r="C17" s="3" t="s">
         <v>1</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>31</v>
+        <v>6</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="F17" s="11" t="s">
+        <v>206</v>
+      </c>
+      <c r="F17" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="G17" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="G17" s="11" t="s">
+      <c r="H17" s="11" t="s">
+        <v>1140</v>
+      </c>
+      <c r="I17" t="s">
+        <v>205</v>
+      </c>
+      <c r="J17" s="22" t="s">
+        <v>98</v>
+      </c>
+      <c r="K17" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="L17" s="22" t="s">
+        <v>98</v>
+      </c>
+      <c r="M17" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="N17" s="22" t="s">
+        <v>98</v>
+      </c>
+      <c r="O17" s="22" t="s">
+        <v>534</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A18" s="7" t="s">
+        <v>254</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>379</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D18" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="E18" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="F18" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="H17" s="11" t="s">
-        <v>98</v>
-      </c>
-      <c r="I17" t="s">
-        <v>1151</v>
-      </c>
-      <c r="J17" s="13" t="s">
-        <v>98</v>
-      </c>
-      <c r="K17" t="s">
-        <v>98</v>
-      </c>
-      <c r="L17" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="M17" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="N17" t="s">
-        <v>98</v>
-      </c>
-      <c r="O17" t="s">
-        <v>98</v>
+      <c r="G18" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="H18" s="11" t="s">
+        <v>1141</v>
+      </c>
+      <c r="I18" t="s">
+        <v>380</v>
+      </c>
+      <c r="J18" s="22" t="s">
+        <v>98</v>
+      </c>
+      <c r="K18" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="L18" s="22" t="s">
+        <v>98</v>
+      </c>
+      <c r="M18" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="N18" s="22" t="s">
+        <v>98</v>
+      </c>
+      <c r="O18" s="22" t="s">
+        <v>1142</v>
       </c>
     </row>
-    <row r="18" spans="1:15" ht="60" x14ac:dyDescent="0.25">
-      <c r="A18" s="7" t="s">
-        <v>253</v>
-      </c>
-      <c r="B18" s="3" t="s">
-        <v>1153</v>
-      </c>
-      <c r="C18" s="11" t="s">
+    <row r="19" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+      <c r="A19" s="7" t="s">
+        <v>254</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>1143</v>
+      </c>
+      <c r="C19" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D18" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="E18" s="3" t="s">
-        <v>1154</v>
-      </c>
-      <c r="F18" s="11" t="s">
+      <c r="D19" s="3" t="s">
+        <v>291</v>
+      </c>
+      <c r="E19" s="3" t="s">
+        <v>296</v>
+      </c>
+      <c r="F19" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="G19" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="G18" s="11" t="s">
-        <v>2</v>
-      </c>
-      <c r="H18" s="11" t="s">
-        <v>98</v>
-      </c>
-      <c r="I18" t="s">
-        <v>1152</v>
-      </c>
-      <c r="J18" s="13" t="s">
-        <v>98</v>
-      </c>
-      <c r="K18" t="s">
-        <v>98</v>
-      </c>
-      <c r="L18" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="M18" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="N18" t="s">
-        <v>98</v>
-      </c>
-      <c r="O18" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="19" spans="1:15" ht="60" x14ac:dyDescent="0.25">
-      <c r="A19" s="7" t="s">
-        <v>253</v>
-      </c>
-      <c r="B19" s="3" t="s">
-        <v>1139</v>
-      </c>
-      <c r="C19" s="11" t="s">
-        <v>1</v>
-      </c>
-      <c r="D19" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="E19" s="3" t="s">
-        <v>1156</v>
-      </c>
-      <c r="F19" s="11" t="s">
-        <v>8</v>
-      </c>
-      <c r="G19" s="11" t="s">
-        <v>2</v>
-      </c>
       <c r="H19" s="11" t="s">
-        <v>98</v>
+        <v>1080</v>
       </c>
       <c r="I19" t="s">
-        <v>1155</v>
-      </c>
-      <c r="J19" s="13" t="s">
-        <v>98</v>
-      </c>
-      <c r="K19" t="s">
-        <v>98</v>
-      </c>
-      <c r="L19" s="1" t="s">
+        <v>448</v>
+      </c>
+      <c r="J19" s="22" t="s">
+        <v>98</v>
+      </c>
+      <c r="K19" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="L19" s="22" t="s">
         <v>98</v>
       </c>
       <c r="M19" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="N19" t="s">
-        <v>98</v>
-      </c>
-      <c r="O19" t="s">
-        <v>98</v>
+      <c r="N19" s="22" t="s">
+        <v>98</v>
+      </c>
+      <c r="O19" s="22" t="s">
+        <v>534</v>
       </c>
     </row>
     <row r="20" spans="1:15" ht="60" x14ac:dyDescent="0.25">
       <c r="A20" s="7" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>1141</v>
-      </c>
-      <c r="C20" s="11" t="s">
+        <v>1036</v>
+      </c>
+      <c r="C20" s="3" t="s">
         <v>1</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>6</v>
+        <v>450</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>1158</v>
-      </c>
-      <c r="F20" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="F20" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="G20" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="G20" s="11" t="s">
-        <v>2</v>
-      </c>
       <c r="H20" s="11" t="s">
-        <v>98</v>
+        <v>1037</v>
       </c>
       <c r="I20" t="s">
-        <v>1157</v>
-      </c>
-      <c r="J20" s="13" t="s">
-        <v>98</v>
-      </c>
-      <c r="K20" t="s">
-        <v>98</v>
-      </c>
-      <c r="L20" s="1" t="s">
+        <v>451</v>
+      </c>
+      <c r="J20" s="22" t="s">
+        <v>98</v>
+      </c>
+      <c r="K20" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="L20" s="22" t="s">
         <v>98</v>
       </c>
       <c r="M20" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="N20" t="s">
-        <v>98</v>
-      </c>
-      <c r="O20" t="s">
-        <v>98</v>
+      <c r="N20" s="22" t="s">
+        <v>98</v>
+      </c>
+      <c r="O20" s="22" t="s">
+        <v>534</v>
       </c>
     </row>
     <row r="21" spans="1:15" ht="30" x14ac:dyDescent="0.25">
       <c r="A21" s="7" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>1138</v>
-      </c>
-      <c r="C21" s="11" t="s">
+        <v>1207</v>
+      </c>
+      <c r="C21" s="3" t="s">
         <v>1</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>6</v>
+        <v>456</v>
       </c>
       <c r="E21" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="F21" s="11" t="s">
+        <v>1144</v>
+      </c>
+      <c r="F21" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="G21" s="11" t="s">
+      <c r="G21" s="3" t="s">
         <v>2</v>
       </c>
       <c r="H21" s="11" t="s">
         <v>98</v>
       </c>
       <c r="I21" t="s">
-        <v>1159</v>
-      </c>
-      <c r="J21" s="13" t="s">
-        <v>98</v>
-      </c>
-      <c r="K21" t="s">
-        <v>98</v>
-      </c>
-      <c r="L21" s="1" t="s">
+        <v>458</v>
+      </c>
+      <c r="J21" s="22" t="s">
+        <v>455</v>
+      </c>
+      <c r="K21" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="L21" s="22" t="s">
         <v>98</v>
       </c>
       <c r="M21" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="N21" t="s">
-        <v>98</v>
-      </c>
-      <c r="O21" t="s">
+        <v>1145</v>
+      </c>
+      <c r="N21" s="22" t="s">
+        <v>98</v>
+      </c>
+      <c r="O21" s="22" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:15" ht="30" x14ac:dyDescent="0.25">
       <c r="A22" s="7" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>1161</v>
-      </c>
-      <c r="C22" s="11" t="s">
+        <v>505</v>
+      </c>
+      <c r="C22" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="D22" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="E22" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="F22" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="G22" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="H22" s="11" t="s">
+        <v>1146</v>
+      </c>
+      <c r="I22" t="s">
+        <v>506</v>
+      </c>
+      <c r="J22" s="22" t="s">
+        <v>98</v>
+      </c>
+      <c r="K22" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="L22" s="22" t="s">
+        <v>98</v>
+      </c>
+      <c r="M22" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="N22" s="22" t="s">
+        <v>98</v>
+      </c>
+      <c r="O22" s="22" t="s">
+        <v>534</v>
+      </c>
+    </row>
+    <row r="23" spans="1:15" ht="45" x14ac:dyDescent="0.25">
+      <c r="A23" s="7" t="s">
+        <v>254</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>573</v>
+      </c>
+      <c r="C23" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D22" s="3" t="s">
-        <v>456</v>
-      </c>
-      <c r="E22" s="3" t="s">
-        <v>1162</v>
-      </c>
-      <c r="F22" s="11" t="s">
+      <c r="D23" s="3" t="s">
+        <v>487</v>
+      </c>
+      <c r="E23" s="3" t="s">
+        <v>1147</v>
+      </c>
+      <c r="F23" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="G22" s="11" t="s">
+      <c r="G23" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="H22" s="11" t="s">
-        <v>98</v>
-      </c>
-      <c r="I22" t="s">
-        <v>1160</v>
-      </c>
-      <c r="J22" s="13" t="s">
-        <v>98</v>
-      </c>
-      <c r="K22" t="s">
-        <v>98</v>
-      </c>
-      <c r="L22" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="M22" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="N22" t="s">
-        <v>98</v>
-      </c>
-      <c r="O22" t="s">
+      <c r="H23" s="11" t="s">
+        <v>98</v>
+      </c>
+      <c r="I23" t="s">
+        <v>572</v>
+      </c>
+      <c r="J23" s="22" t="s">
+        <v>98</v>
+      </c>
+      <c r="K23" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="L23" s="22" t="s">
+        <v>98</v>
+      </c>
+      <c r="M23" s="1" t="s">
+        <v>1148</v>
+      </c>
+      <c r="N23" s="22" t="s">
+        <v>98</v>
+      </c>
+      <c r="O23" s="22" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="23" spans="1:15" ht="30" x14ac:dyDescent="0.25">
-      <c r="A23" s="7" t="s">
-        <v>253</v>
-      </c>
-      <c r="B23" s="3" t="s">
-        <v>1164</v>
-      </c>
-      <c r="C23" s="11" t="s">
-        <v>1</v>
-      </c>
-      <c r="D23" s="3" t="s">
-        <v>456</v>
-      </c>
-      <c r="E23" s="3" t="s">
-        <v>1165</v>
-      </c>
-      <c r="F23" s="11" t="s">
-        <v>8</v>
-      </c>
-      <c r="G23" s="11" t="s">
-        <v>2</v>
-      </c>
-      <c r="H23" s="11" t="s">
-        <v>98</v>
-      </c>
-      <c r="I23" t="s">
-        <v>1163</v>
-      </c>
-      <c r="J23" s="13" t="s">
-        <v>98</v>
-      </c>
-      <c r="K23" t="s">
-        <v>98</v>
-      </c>
-      <c r="L23" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="M23" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="N23" t="s">
-        <v>98</v>
-      </c>
-      <c r="O23" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="24" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:15" ht="60" x14ac:dyDescent="0.25">
       <c r="A24" s="7" t="s">
         <v>253</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>1167</v>
-      </c>
-      <c r="C24" s="11" t="s">
+        <v>1036</v>
+      </c>
+      <c r="C24" s="3" t="s">
         <v>1</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>456</v>
+        <v>31</v>
       </c>
       <c r="E24" s="3" t="s">
-        <v>1168</v>
-      </c>
-      <c r="F24" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="F24" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="G24" s="11" t="s">
+      <c r="G24" s="3" t="s">
         <v>2</v>
       </c>
       <c r="H24" s="11" t="s">
         <v>98</v>
       </c>
       <c r="I24" t="s">
-        <v>1166</v>
-      </c>
-      <c r="J24" s="13" t="s">
-        <v>98</v>
-      </c>
-      <c r="K24" t="s">
-        <v>98</v>
-      </c>
-      <c r="L24" s="1" t="s">
+        <v>1149</v>
+      </c>
+      <c r="J24" s="22" t="s">
+        <v>98</v>
+      </c>
+      <c r="K24" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="L24" s="22" t="s">
         <v>98</v>
       </c>
       <c r="M24" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="N24" t="s">
-        <v>98</v>
-      </c>
-      <c r="O24" t="s">
+      <c r="N24" s="22" t="s">
+        <v>98</v>
+      </c>
+      <c r="O24" s="22" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="25" spans="1:15" ht="45" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:15" ht="60" x14ac:dyDescent="0.25">
       <c r="A25" s="7" t="s">
         <v>253</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>1170</v>
-      </c>
-      <c r="C25" s="11" t="s">
+        <v>1151</v>
+      </c>
+      <c r="C25" s="3" t="s">
         <v>1</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>291</v>
+        <v>6</v>
       </c>
       <c r="E25" s="3" t="s">
-        <v>296</v>
-      </c>
-      <c r="F25" s="11" t="s">
+        <v>1152</v>
+      </c>
+      <c r="F25" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="G25" s="11" t="s">
+      <c r="G25" s="3" t="s">
         <v>2</v>
       </c>
       <c r="H25" s="11" t="s">
         <v>98</v>
       </c>
       <c r="I25" t="s">
-        <v>1169</v>
-      </c>
-      <c r="J25" s="13" t="s">
-        <v>98</v>
-      </c>
-      <c r="K25" t="s">
-        <v>98</v>
-      </c>
-      <c r="L25" s="1" t="s">
+        <v>1150</v>
+      </c>
+      <c r="J25" s="22" t="s">
+        <v>98</v>
+      </c>
+      <c r="K25" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="L25" s="22" t="s">
         <v>98</v>
       </c>
       <c r="M25" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="N25" t="s">
-        <v>98</v>
-      </c>
-      <c r="O25" t="s">
+      <c r="N25" s="22" t="s">
+        <v>98</v>
+      </c>
+      <c r="O25" s="22" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="26" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:15" ht="60" x14ac:dyDescent="0.25">
       <c r="A26" s="7" t="s">
         <v>253</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>1172</v>
-      </c>
-      <c r="C26" s="11" t="s">
+        <v>1137</v>
+      </c>
+      <c r="C26" s="3" t="s">
         <v>1</v>
       </c>
       <c r="D26" s="3" t="s">
-        <v>291</v>
+        <v>6</v>
       </c>
       <c r="E26" s="3" t="s">
-        <v>296</v>
-      </c>
-      <c r="F26" s="11" t="s">
+        <v>1154</v>
+      </c>
+      <c r="F26" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="G26" s="11" t="s">
+      <c r="G26" s="3" t="s">
         <v>2</v>
       </c>
       <c r="H26" s="11" t="s">
         <v>98</v>
       </c>
       <c r="I26" t="s">
-        <v>1171</v>
-      </c>
-      <c r="J26" s="13" t="s">
-        <v>98</v>
-      </c>
-      <c r="K26" t="s">
-        <v>98</v>
-      </c>
-      <c r="L26" s="1" t="s">
+        <v>1153</v>
+      </c>
+      <c r="J26" s="22" t="s">
+        <v>98</v>
+      </c>
+      <c r="K26" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="L26" s="22" t="s">
         <v>98</v>
       </c>
       <c r="M26" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="N26" t="s">
-        <v>98</v>
-      </c>
-      <c r="O26" t="s">
+      <c r="N26" s="22" t="s">
+        <v>98</v>
+      </c>
+      <c r="O26" s="22" t="s">
         <v>98</v>
       </c>
     </row>
@@ -53791,9 +53428,9 @@
         <v>253</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>1174</v>
-      </c>
-      <c r="C27" s="11" t="s">
+        <v>1139</v>
+      </c>
+      <c r="C27" s="3" t="s">
         <v>1</v>
       </c>
       <c r="D27" s="3" t="s">
@@ -53802,269 +53439,269 @@
       <c r="E27" s="3" t="s">
         <v>1156</v>
       </c>
-      <c r="F27" s="11" t="s">
+      <c r="F27" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="G27" s="11" t="s">
+      <c r="G27" s="3" t="s">
         <v>2</v>
       </c>
       <c r="H27" s="11" t="s">
         <v>98</v>
       </c>
       <c r="I27" t="s">
-        <v>1173</v>
-      </c>
-      <c r="J27" s="13" t="s">
-        <v>98</v>
-      </c>
-      <c r="K27" t="s">
-        <v>98</v>
-      </c>
-      <c r="L27" s="1" t="s">
+        <v>1155</v>
+      </c>
+      <c r="J27" s="22" t="s">
+        <v>98</v>
+      </c>
+      <c r="K27" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="L27" s="22" t="s">
         <v>98</v>
       </c>
       <c r="M27" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="N27" t="s">
-        <v>98</v>
-      </c>
-      <c r="O27" t="s">
+      <c r="N27" s="22" t="s">
+        <v>98</v>
+      </c>
+      <c r="O27" s="22" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="28" spans="1:15" ht="60" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:15" ht="30" x14ac:dyDescent="0.25">
       <c r="A28" s="7" t="s">
         <v>253</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>1176</v>
-      </c>
-      <c r="C28" s="11" t="s">
+        <v>1136</v>
+      </c>
+      <c r="C28" s="3" t="s">
         <v>1</v>
       </c>
       <c r="D28" s="3" t="s">
         <v>6</v>
       </c>
       <c r="E28" s="3" t="s">
-        <v>1154</v>
-      </c>
-      <c r="F28" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="F28" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="G28" s="11" t="s">
+      <c r="G28" s="3" t="s">
         <v>2</v>
       </c>
       <c r="H28" s="11" t="s">
         <v>98</v>
       </c>
       <c r="I28" t="s">
-        <v>1175</v>
-      </c>
-      <c r="J28" s="13" t="s">
-        <v>98</v>
-      </c>
-      <c r="K28" t="s">
-        <v>98</v>
-      </c>
-      <c r="L28" s="1" t="s">
+        <v>1157</v>
+      </c>
+      <c r="J28" s="22" t="s">
+        <v>98</v>
+      </c>
+      <c r="K28" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="L28" s="22" t="s">
         <v>98</v>
       </c>
       <c r="M28" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="N28" t="s">
-        <v>98</v>
-      </c>
-      <c r="O28" t="s">
+      <c r="N28" s="22" t="s">
+        <v>98</v>
+      </c>
+      <c r="O28" s="22" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="29" spans="1:15" ht="60" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:15" ht="30" x14ac:dyDescent="0.25">
       <c r="A29" s="7" t="s">
         <v>253</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>1178</v>
-      </c>
-      <c r="C29" s="11" t="s">
+        <v>1159</v>
+      </c>
+      <c r="C29" s="3" t="s">
         <v>1</v>
       </c>
       <c r="D29" s="3" t="s">
-        <v>6</v>
+        <v>456</v>
       </c>
       <c r="E29" s="3" t="s">
-        <v>1156</v>
-      </c>
-      <c r="F29" s="11" t="s">
+        <v>1160</v>
+      </c>
+      <c r="F29" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="G29" s="11" t="s">
+      <c r="G29" s="3" t="s">
         <v>2</v>
       </c>
       <c r="H29" s="11" t="s">
         <v>98</v>
       </c>
       <c r="I29" t="s">
-        <v>1177</v>
-      </c>
-      <c r="J29" s="13" t="s">
-        <v>98</v>
-      </c>
-      <c r="K29" t="s">
-        <v>98</v>
-      </c>
-      <c r="L29" s="1" t="s">
+        <v>1158</v>
+      </c>
+      <c r="J29" s="22" t="s">
+        <v>98</v>
+      </c>
+      <c r="K29" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="L29" s="22" t="s">
         <v>98</v>
       </c>
       <c r="M29" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="N29" t="s">
-        <v>98</v>
-      </c>
-      <c r="O29" t="s">
+      <c r="N29" s="22" t="s">
+        <v>98</v>
+      </c>
+      <c r="O29" s="22" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="30" spans="1:15" ht="45" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:15" ht="30" x14ac:dyDescent="0.25">
       <c r="A30" s="7" t="s">
         <v>253</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>1136</v>
-      </c>
-      <c r="C30" s="11" t="s">
+        <v>1162</v>
+      </c>
+      <c r="C30" s="3" t="s">
         <v>1</v>
       </c>
       <c r="D30" s="3" t="s">
-        <v>1134</v>
+        <v>456</v>
       </c>
       <c r="E30" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="F30" s="11" t="s">
+        <v>1163</v>
+      </c>
+      <c r="F30" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="G30" s="11" t="s">
+      <c r="G30" s="3" t="s">
         <v>2</v>
       </c>
       <c r="H30" s="11" t="s">
         <v>98</v>
       </c>
       <c r="I30" t="s">
-        <v>1179</v>
-      </c>
-      <c r="J30" s="13" t="s">
-        <v>98</v>
-      </c>
-      <c r="K30" t="s">
-        <v>98</v>
-      </c>
-      <c r="L30" s="1" t="s">
+        <v>1161</v>
+      </c>
+      <c r="J30" s="22" t="s">
+        <v>98</v>
+      </c>
+      <c r="K30" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="L30" s="22" t="s">
         <v>98</v>
       </c>
       <c r="M30" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="N30" t="s">
-        <v>98</v>
-      </c>
-      <c r="O30" t="s">
+      <c r="N30" s="22" t="s">
+        <v>98</v>
+      </c>
+      <c r="O30" s="22" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="31" spans="1:15" ht="45" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:15" ht="30" x14ac:dyDescent="0.25">
       <c r="A31" s="7" t="s">
         <v>253</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>505</v>
-      </c>
-      <c r="C31" s="11" t="s">
-        <v>74</v>
+        <v>1165</v>
+      </c>
+      <c r="C31" s="3" t="s">
+        <v>1</v>
       </c>
       <c r="D31" s="3" t="s">
-        <v>1134</v>
+        <v>456</v>
       </c>
       <c r="E31" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="F31" s="11" t="s">
+        <v>1166</v>
+      </c>
+      <c r="F31" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="G31" s="11" t="s">
+      <c r="G31" s="3" t="s">
         <v>2</v>
       </c>
       <c r="H31" s="11" t="s">
         <v>98</v>
       </c>
       <c r="I31" t="s">
-        <v>1180</v>
-      </c>
-      <c r="J31" s="13" t="s">
-        <v>98</v>
-      </c>
-      <c r="K31" t="s">
-        <v>98</v>
-      </c>
-      <c r="L31" s="1" t="s">
+        <v>1164</v>
+      </c>
+      <c r="J31" s="22" t="s">
+        <v>98</v>
+      </c>
+      <c r="K31" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="L31" s="22" t="s">
         <v>98</v>
       </c>
       <c r="M31" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="N31" t="s">
-        <v>98</v>
-      </c>
-      <c r="O31" t="s">
+      <c r="N31" s="22" t="s">
+        <v>98</v>
+      </c>
+      <c r="O31" s="22" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="32" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:15" ht="45" x14ac:dyDescent="0.25">
       <c r="A32" s="7" t="s">
         <v>253</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>1182</v>
-      </c>
-      <c r="C32" s="11" t="s">
+        <v>1168</v>
+      </c>
+      <c r="C32" s="3" t="s">
         <v>1</v>
       </c>
       <c r="D32" s="3" t="s">
-        <v>112</v>
+        <v>291</v>
       </c>
       <c r="E32" s="3" t="s">
-        <v>1183</v>
-      </c>
-      <c r="F32" s="11" t="s">
+        <v>296</v>
+      </c>
+      <c r="F32" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="G32" s="11" t="s">
+      <c r="G32" s="3" t="s">
         <v>2</v>
       </c>
       <c r="H32" s="11" t="s">
         <v>98</v>
       </c>
       <c r="I32" t="s">
-        <v>1181</v>
-      </c>
-      <c r="J32" s="13" t="s">
-        <v>98</v>
-      </c>
-      <c r="K32" t="s">
-        <v>98</v>
-      </c>
-      <c r="L32" s="1" t="s">
+        <v>1167</v>
+      </c>
+      <c r="J32" s="22" t="s">
+        <v>98</v>
+      </c>
+      <c r="K32" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="L32" s="22" t="s">
         <v>98</v>
       </c>
       <c r="M32" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="N32" t="s">
-        <v>98</v>
-      </c>
-      <c r="O32" t="s">
+      <c r="N32" s="22" t="s">
+        <v>98</v>
+      </c>
+      <c r="O32" s="22" t="s">
         <v>98</v>
       </c>
     </row>
@@ -54073,280 +53710,280 @@
         <v>253</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>1188</v>
-      </c>
-      <c r="C33" s="11" t="s">
-        <v>74</v>
+        <v>1170</v>
+      </c>
+      <c r="C33" s="3" t="s">
+        <v>1</v>
       </c>
       <c r="D33" s="3" t="s">
-        <v>112</v>
+        <v>291</v>
       </c>
       <c r="E33" s="3" t="s">
-        <v>1183</v>
-      </c>
-      <c r="F33" s="11" t="s">
+        <v>296</v>
+      </c>
+      <c r="F33" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="G33" s="11" t="s">
+      <c r="G33" s="3" t="s">
         <v>2</v>
       </c>
       <c r="H33" s="11" t="s">
         <v>98</v>
       </c>
       <c r="I33" t="s">
-        <v>1187</v>
-      </c>
-      <c r="J33" s="13" t="s">
-        <v>98</v>
-      </c>
-      <c r="K33" t="s">
-        <v>98</v>
-      </c>
-      <c r="L33" s="1" t="s">
+        <v>1169</v>
+      </c>
+      <c r="J33" s="22" t="s">
+        <v>98</v>
+      </c>
+      <c r="K33" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="L33" s="22" t="s">
         <v>98</v>
       </c>
       <c r="M33" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="N33" t="s">
-        <v>98</v>
-      </c>
-      <c r="O33" t="s">
+      <c r="N33" s="22" t="s">
+        <v>98</v>
+      </c>
+      <c r="O33" s="22" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="34" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:15" ht="60" x14ac:dyDescent="0.25">
       <c r="A34" s="7" t="s">
         <v>253</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>1190</v>
-      </c>
-      <c r="C34" s="11" t="s">
+        <v>1172</v>
+      </c>
+      <c r="C34" s="3" t="s">
         <v>1</v>
       </c>
       <c r="D34" s="3" t="s">
         <v>6</v>
       </c>
       <c r="E34" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="F34" s="11" t="s">
+        <v>1154</v>
+      </c>
+      <c r="F34" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="G34" s="11" t="s">
+      <c r="G34" s="3" t="s">
         <v>2</v>
       </c>
       <c r="H34" s="11" t="s">
         <v>98</v>
       </c>
       <c r="I34" t="s">
-        <v>1189</v>
-      </c>
-      <c r="J34" s="13" t="s">
-        <v>98</v>
-      </c>
-      <c r="K34" t="s">
-        <v>98</v>
-      </c>
-      <c r="L34" s="1" t="s">
+        <v>1171</v>
+      </c>
+      <c r="J34" s="22" t="s">
+        <v>98</v>
+      </c>
+      <c r="K34" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="L34" s="22" t="s">
         <v>98</v>
       </c>
       <c r="M34" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="N34" t="s">
-        <v>98</v>
-      </c>
-      <c r="O34" t="s">
+      <c r="N34" s="22" t="s">
+        <v>98</v>
+      </c>
+      <c r="O34" s="22" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="35" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:15" ht="60" x14ac:dyDescent="0.25">
       <c r="A35" s="7" t="s">
         <v>253</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>1192</v>
-      </c>
-      <c r="C35" s="11" t="s">
+        <v>1174</v>
+      </c>
+      <c r="C35" s="3" t="s">
         <v>1</v>
       </c>
       <c r="D35" s="3" t="s">
-        <v>1193</v>
+        <v>6</v>
       </c>
       <c r="E35" s="3" t="s">
-        <v>1194</v>
-      </c>
-      <c r="F35" s="11" t="s">
+        <v>1152</v>
+      </c>
+      <c r="F35" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="G35" s="11" t="s">
+      <c r="G35" s="3" t="s">
         <v>2</v>
       </c>
       <c r="H35" s="11" t="s">
         <v>98</v>
       </c>
       <c r="I35" t="s">
-        <v>1191</v>
-      </c>
-      <c r="J35" s="13" t="s">
-        <v>98</v>
-      </c>
-      <c r="K35" t="s">
-        <v>98</v>
-      </c>
-      <c r="L35" s="1" t="s">
+        <v>1173</v>
+      </c>
+      <c r="J35" s="22" t="s">
+        <v>98</v>
+      </c>
+      <c r="K35" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="L35" s="22" t="s">
         <v>98</v>
       </c>
       <c r="M35" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="N35" t="s">
-        <v>98</v>
-      </c>
-      <c r="O35" t="s">
+      <c r="N35" s="22" t="s">
+        <v>98</v>
+      </c>
+      <c r="O35" s="22" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="36" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:15" ht="60" x14ac:dyDescent="0.25">
       <c r="A36" s="7" t="s">
         <v>253</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>1196</v>
-      </c>
-      <c r="C36" s="11" t="s">
+        <v>1176</v>
+      </c>
+      <c r="C36" s="3" t="s">
         <v>1</v>
       </c>
       <c r="D36" s="3" t="s">
-        <v>131</v>
+        <v>6</v>
       </c>
       <c r="E36" s="3" t="s">
-        <v>132</v>
-      </c>
-      <c r="F36" s="11" t="s">
+        <v>1154</v>
+      </c>
+      <c r="F36" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="G36" s="11" t="s">
+      <c r="G36" s="3" t="s">
         <v>2</v>
       </c>
       <c r="H36" s="11" t="s">
         <v>98</v>
       </c>
       <c r="I36" t="s">
-        <v>1195</v>
-      </c>
-      <c r="J36" s="13" t="s">
-        <v>98</v>
-      </c>
-      <c r="K36" t="s">
-        <v>98</v>
-      </c>
-      <c r="L36" s="1" t="s">
+        <v>1175</v>
+      </c>
+      <c r="J36" s="22" t="s">
+        <v>98</v>
+      </c>
+      <c r="K36" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="L36" s="22" t="s">
         <v>98</v>
       </c>
       <c r="M36" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="N36" t="s">
-        <v>98</v>
-      </c>
-      <c r="O36" t="s">
+      <c r="N36" s="22" t="s">
+        <v>98</v>
+      </c>
+      <c r="O36" s="22" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="37" spans="1:15" ht="45" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:15" ht="60" x14ac:dyDescent="0.25">
       <c r="A37" s="7" t="s">
         <v>253</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>1061</v>
-      </c>
-      <c r="C37" s="11" t="s">
-        <v>74</v>
+        <v>1134</v>
+      </c>
+      <c r="C37" s="3" t="s">
+        <v>1</v>
       </c>
       <c r="D37" s="3" t="s">
-        <v>153</v>
+        <v>1208</v>
       </c>
       <c r="E37" s="3" t="s">
-        <v>132</v>
-      </c>
-      <c r="F37" s="11" t="s">
+        <v>78</v>
+      </c>
+      <c r="F37" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="G37" s="11" t="s">
+      <c r="G37" s="3" t="s">
         <v>2</v>
       </c>
       <c r="H37" s="11" t="s">
         <v>98</v>
       </c>
       <c r="I37" t="s">
-        <v>1197</v>
-      </c>
-      <c r="J37" s="13" t="s">
-        <v>98</v>
-      </c>
-      <c r="K37" t="s">
-        <v>98</v>
-      </c>
-      <c r="L37" s="1" t="s">
+        <v>1177</v>
+      </c>
+      <c r="J37" s="22" t="s">
+        <v>98</v>
+      </c>
+      <c r="K37" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="L37" s="22" t="s">
         <v>98</v>
       </c>
       <c r="M37" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="N37" t="s">
-        <v>98</v>
-      </c>
-      <c r="O37" t="s">
+      <c r="N37" s="22" t="s">
+        <v>98</v>
+      </c>
+      <c r="O37" s="22" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="38" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:15" ht="60" x14ac:dyDescent="0.25">
       <c r="A38" s="7" t="s">
         <v>253</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>1199</v>
-      </c>
-      <c r="C38" s="11" t="s">
-        <v>1</v>
+        <v>505</v>
+      </c>
+      <c r="C38" s="3" t="s">
+        <v>74</v>
       </c>
       <c r="D38" s="3" t="s">
-        <v>86</v>
+        <v>1208</v>
       </c>
       <c r="E38" s="3" t="s">
-        <v>85</v>
-      </c>
-      <c r="F38" s="11" t="s">
+        <v>78</v>
+      </c>
+      <c r="F38" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="G38" s="11" t="s">
+      <c r="G38" s="3" t="s">
         <v>2</v>
       </c>
       <c r="H38" s="11" t="s">
         <v>98</v>
       </c>
       <c r="I38" t="s">
-        <v>1198</v>
-      </c>
-      <c r="J38" s="13" t="s">
-        <v>98</v>
-      </c>
-      <c r="K38" t="s">
-        <v>98</v>
-      </c>
-      <c r="L38" s="1" t="s">
+        <v>1178</v>
+      </c>
+      <c r="J38" s="22" t="s">
+        <v>98</v>
+      </c>
+      <c r="K38" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="L38" s="22" t="s">
         <v>98</v>
       </c>
       <c r="M38" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="N38" t="s">
-        <v>98</v>
-      </c>
-      <c r="O38" t="s">
+      <c r="N38" s="22" t="s">
+        <v>98</v>
+      </c>
+      <c r="O38" s="22" t="s">
         <v>98</v>
       </c>
     </row>
@@ -54355,45 +53992,45 @@
         <v>253</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>1205</v>
-      </c>
-      <c r="C39" s="11" t="s">
-        <v>74</v>
+        <v>1180</v>
+      </c>
+      <c r="C39" s="3" t="s">
+        <v>1</v>
       </c>
       <c r="D39" s="3" t="s">
-        <v>45</v>
+        <v>112</v>
       </c>
       <c r="E39" s="3" t="s">
-        <v>460</v>
-      </c>
-      <c r="F39" s="11" t="s">
+        <v>1181</v>
+      </c>
+      <c r="F39" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="G39" s="11" t="s">
+      <c r="G39" s="3" t="s">
         <v>2</v>
       </c>
       <c r="H39" s="11" t="s">
         <v>98</v>
       </c>
       <c r="I39" t="s">
-        <v>1204</v>
-      </c>
-      <c r="J39" s="13" t="s">
-        <v>98</v>
-      </c>
-      <c r="K39" t="s">
-        <v>98</v>
-      </c>
-      <c r="L39" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="M39" t="s">
-        <v>98</v>
-      </c>
-      <c r="N39" t="s">
-        <v>98</v>
-      </c>
-      <c r="O39" t="s">
+        <v>1179</v>
+      </c>
+      <c r="J39" s="22" t="s">
+        <v>98</v>
+      </c>
+      <c r="K39" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="L39" s="22" t="s">
+        <v>98</v>
+      </c>
+      <c r="M39" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="N39" s="22" t="s">
+        <v>98</v>
+      </c>
+      <c r="O39" s="22" t="s">
         <v>98</v>
       </c>
     </row>
@@ -54402,45 +54039,374 @@
         <v>253</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>1207</v>
-      </c>
-      <c r="C40" s="11" t="s">
+        <v>1185</v>
+      </c>
+      <c r="C40" s="3" t="s">
         <v>74</v>
       </c>
       <c r="D40" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="E40" s="3" t="s">
+        <v>1181</v>
+      </c>
+      <c r="F40" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="G40" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="H40" s="11" t="s">
+        <v>98</v>
+      </c>
+      <c r="I40" t="s">
+        <v>1184</v>
+      </c>
+      <c r="J40" s="22" t="s">
+        <v>98</v>
+      </c>
+      <c r="K40" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="L40" s="22" t="s">
+        <v>98</v>
+      </c>
+      <c r="M40" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="N40" s="22" t="s">
+        <v>98</v>
+      </c>
+      <c r="O40" s="22" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="41" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+      <c r="A41" s="7" t="s">
+        <v>253</v>
+      </c>
+      <c r="B41" s="3" t="s">
+        <v>1187</v>
+      </c>
+      <c r="C41" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D41" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E41" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="F41" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="G41" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="H41" s="11" t="s">
+        <v>98</v>
+      </c>
+      <c r="I41" t="s">
+        <v>1186</v>
+      </c>
+      <c r="J41" s="22" t="s">
+        <v>98</v>
+      </c>
+      <c r="K41" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="L41" s="22" t="s">
+        <v>98</v>
+      </c>
+      <c r="M41" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="N41" s="22" t="s">
+        <v>98</v>
+      </c>
+      <c r="O41" s="22" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="42" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+      <c r="A42" s="7" t="s">
+        <v>253</v>
+      </c>
+      <c r="B42" s="3" t="s">
+        <v>1189</v>
+      </c>
+      <c r="C42" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D42" s="3" t="s">
+        <v>1190</v>
+      </c>
+      <c r="E42" s="3" t="s">
+        <v>1191</v>
+      </c>
+      <c r="F42" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="G42" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="H42" s="11" t="s">
+        <v>98</v>
+      </c>
+      <c r="I42" t="s">
+        <v>1188</v>
+      </c>
+      <c r="J42" s="22" t="s">
+        <v>98</v>
+      </c>
+      <c r="K42" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="L42" s="22" t="s">
+        <v>98</v>
+      </c>
+      <c r="M42" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="N42" s="22" t="s">
+        <v>98</v>
+      </c>
+      <c r="O42" s="22" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="43" spans="1:15" ht="45" x14ac:dyDescent="0.25">
+      <c r="A43" s="7" t="s">
+        <v>253</v>
+      </c>
+      <c r="B43" s="3" t="s">
+        <v>1193</v>
+      </c>
+      <c r="C43" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D43" s="3" t="s">
+        <v>131</v>
+      </c>
+      <c r="E43" s="3" t="s">
+        <v>132</v>
+      </c>
+      <c r="F43" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="G43" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="H43" s="11" t="s">
+        <v>98</v>
+      </c>
+      <c r="I43" t="s">
+        <v>1192</v>
+      </c>
+      <c r="J43" s="22" t="s">
+        <v>98</v>
+      </c>
+      <c r="K43" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="L43" s="22" t="s">
+        <v>98</v>
+      </c>
+      <c r="M43" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="N43" s="22" t="s">
+        <v>98</v>
+      </c>
+      <c r="O43" s="22" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="44" spans="1:15" ht="45" x14ac:dyDescent="0.25">
+      <c r="A44" s="7" t="s">
+        <v>253</v>
+      </c>
+      <c r="B44" s="3" t="s">
+        <v>1061</v>
+      </c>
+      <c r="C44" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="D44" s="3" t="s">
+        <v>153</v>
+      </c>
+      <c r="E44" s="3" t="s">
+        <v>132</v>
+      </c>
+      <c r="F44" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="G44" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="H44" s="11" t="s">
+        <v>98</v>
+      </c>
+      <c r="I44" t="s">
+        <v>1194</v>
+      </c>
+      <c r="J44" s="22" t="s">
+        <v>98</v>
+      </c>
+      <c r="K44" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="L44" s="22" t="s">
+        <v>98</v>
+      </c>
+      <c r="M44" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="N44" s="22" t="s">
+        <v>98</v>
+      </c>
+      <c r="O44" s="22" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="45" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+      <c r="A45" s="7" t="s">
+        <v>253</v>
+      </c>
+      <c r="B45" s="3" t="s">
+        <v>1196</v>
+      </c>
+      <c r="C45" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D45" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="E45" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="F45" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="G45" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="H45" s="11" t="s">
+        <v>98</v>
+      </c>
+      <c r="I45" t="s">
+        <v>1195</v>
+      </c>
+      <c r="J45" s="22" t="s">
+        <v>98</v>
+      </c>
+      <c r="K45" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="L45" s="22" t="s">
+        <v>98</v>
+      </c>
+      <c r="M45" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="N45" s="22" t="s">
+        <v>98</v>
+      </c>
+      <c r="O45" s="22" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="46" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+      <c r="A46" s="7" t="s">
+        <v>253</v>
+      </c>
+      <c r="B46" s="3" t="s">
+        <v>1201</v>
+      </c>
+      <c r="C46" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="D46" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="E40" s="3" t="s">
+      <c r="E46" s="3" t="s">
         <v>460</v>
       </c>
-      <c r="F40" s="11" t="s">
+      <c r="F46" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="G40" s="11" t="s">
+      <c r="G46" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="H40" s="11" t="s">
-        <v>98</v>
-      </c>
-      <c r="I40" t="s">
-        <v>1206</v>
-      </c>
-      <c r="J40" s="13" t="s">
-        <v>98</v>
-      </c>
-      <c r="K40" t="s">
-        <v>98</v>
-      </c>
-      <c r="L40" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="M40" t="s">
-        <v>98</v>
-      </c>
-      <c r="N40" t="s">
-        <v>98</v>
-      </c>
-      <c r="O40" t="s">
+      <c r="H46" s="11" t="s">
+        <v>98</v>
+      </c>
+      <c r="I46" t="s">
+        <v>1200</v>
+      </c>
+      <c r="J46" s="22" t="s">
+        <v>98</v>
+      </c>
+      <c r="K46" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="L46" s="22" t="s">
+        <v>98</v>
+      </c>
+      <c r="M46" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="N46" s="22" t="s">
+        <v>98</v>
+      </c>
+      <c r="O46" s="22" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="47" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+      <c r="A47" s="7" t="s">
+        <v>253</v>
+      </c>
+      <c r="B47" s="3" t="s">
+        <v>1203</v>
+      </c>
+      <c r="C47" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="D47" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="E47" s="3" t="s">
+        <v>460</v>
+      </c>
+      <c r="F47" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="G47" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="H47" s="11" t="s">
+        <v>98</v>
+      </c>
+      <c r="I47" t="s">
+        <v>1202</v>
+      </c>
+      <c r="J47" s="22" t="s">
+        <v>98</v>
+      </c>
+      <c r="K47" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="L47" s="22" t="s">
+        <v>98</v>
+      </c>
+      <c r="M47" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="N47" s="22" t="s">
+        <v>98</v>
+      </c>
+      <c r="O47" s="22" t="s">
         <v>98</v>
       </c>
     </row>

</xml_diff>